<commit_message>
Main analyses complete, writing up re-analysis
</commit_message>
<xml_diff>
--- a/MSc_Thesis/MSc_Thesis_Split/Data/Citations_Datasets/mokry_obesity_2016.xlsx
+++ b/MSc_Thesis/MSc_Thesis_Split/Data/Citations_Datasets/mokry_obesity_2016.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4f99f7067dc2a9a5/Documents/R/Working Directory/Data_Science_MSc/Dissertation_Bayes_MR/MSc_Thesis/MSc_Thesis_Split/Data/Citations_Datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{22C4E43D-6371-4515-9FCB-E71DF9F4DBB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4F584BA-4AD1-4B06-BBDC-BB0F4958DBBE}"/>
+  <xr:revisionPtr revIDLastSave="39" documentId="8_{22C4E43D-6371-4515-9FCB-E71DF9F4DBB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A93F10F-09D3-4F31-BA50-4CB9BFD7CF3F}"/>
   <bookViews>
-    <workbookView xWindow="12710" yWindow="0" windowWidth="12980" windowHeight="15370" xr2:uid="{8A3BB852-7168-48D5-AFAC-CE153936FD9B}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="12980" windowHeight="15370" activeTab="1" xr2:uid="{8A3BB852-7168-48D5-AFAC-CE153936FD9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Table004 (Page 7-8)" sheetId="2" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1309" uniqueCount="353">
   <si>
     <t>BMI-Associated</t>
   </si>
@@ -1056,13 +1056,67 @@
   </si>
   <si>
     <t>Upp_CI</t>
+  </si>
+  <si>
+    <t>SE_Lower_Only</t>
+  </si>
+  <si>
+    <t>SE_Both</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>Study_Ref</t>
+  </si>
+  <si>
+    <t>Study_DOI</t>
+  </si>
+  <si>
+    <t>Exposure</t>
+  </si>
+  <si>
+    <t>Outcome</t>
+  </si>
+  <si>
+    <t>Instrument</t>
+  </si>
+  <si>
+    <t>Reported_Measure</t>
+  </si>
+  <si>
+    <t>Coeff_G_X</t>
+  </si>
+  <si>
+    <t>Coeff_G_X_SE</t>
+  </si>
+  <si>
+    <t>Coeff_G_Y</t>
+  </si>
+  <si>
+    <t>Coeff_G_Y_SE</t>
+  </si>
+  <si>
+    <t>Mokry et al</t>
+  </si>
+  <si>
+    <t>[@mokry_obesity_2016]</t>
+  </si>
+  <si>
+    <t>10.1371/journal.pmed.1002053</t>
+  </si>
+  <si>
+    <t>Multiple Sclerosis</t>
+  </si>
+  <si>
+    <t>OR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1074,6 +1128,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1154,6 +1214,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1521,10 +1585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17ADCFF7-C1EB-4801-B550-02DC019036B8}">
-  <dimension ref="A1:AB72"/>
+  <dimension ref="A1:AD72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB3" sqref="AB3:AB72"/>
+    <sheetView topLeftCell="T2" workbookViewId="0">
+      <selection activeCell="AC72" sqref="AC3:AC72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1545,7 +1609,7 @@
     <col min="15" max="15" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1604,7 +1668,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -1657,10 +1721,13 @@
         <v>334</v>
       </c>
       <c r="AB2" s="1" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.35">
+        <v>335</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -1743,8 +1810,16 @@
         <f>(Y3-Z3)/1.96</f>
         <v>1.5540411981994171E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC3">
+        <f>(AA3-Z3)/2/1.96</f>
+        <v>1.7775489958670895E-2</v>
+      </c>
+      <c r="AD3">
+        <f>(AA3-Y3)/1.96</f>
+        <v>2.0010567935347619E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -1827,8 +1902,16 @@
         <f t="shared" ref="AB4:AB67" si="3">(Y4-Z4)/1.96</f>
         <v>2.0827548224619984E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC4">
+        <f t="shared" ref="AC4:AC67" si="4">(AA4-Z4)/2/1.96</f>
+        <v>2.0419058079983801E-2</v>
+      </c>
+      <c r="AD4">
+        <f t="shared" ref="AD4:AD67" si="5">(AA4-Y4)/1.96</f>
+        <v>2.0010567935347619E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -1911,8 +1994,16 @@
         <f t="shared" si="3"/>
         <v>1.9816241487889776E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC5">
+        <f t="shared" si="4"/>
+        <v>2.1775471671213478E-2</v>
+      </c>
+      <c r="AD5">
+        <f t="shared" si="5"/>
+        <v>2.3734701854537188E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>48</v>
       </c>
@@ -1995,8 +2086,16 @@
         <f t="shared" si="3"/>
         <v>1.5231103647796521E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC6">
+        <f t="shared" si="4"/>
+        <v>1.5010331638503445E-2</v>
+      </c>
+      <c r="AD6">
+        <f t="shared" si="5"/>
+        <v>1.4789559629210367E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>55</v>
       </c>
@@ -2079,8 +2178,16 @@
         <f t="shared" si="3"/>
         <v>2.0827548224619984E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC7">
+        <f t="shared" si="4"/>
+        <v>2.286024456369572E-2</v>
+      </c>
+      <c r="AD7">
+        <f t="shared" si="5"/>
+        <v>2.4892940902771454E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>62</v>
       </c>
@@ -2163,8 +2270,16 @@
         <f t="shared" si="3"/>
         <v>2.5138290309583051E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC8">
+        <f t="shared" si="4"/>
+        <v>2.219677984429333E-2</v>
+      </c>
+      <c r="AD8">
+        <f t="shared" si="5"/>
+        <v>1.9255269379003605E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>69</v>
       </c>
@@ -2247,8 +2362,16 @@
         <f t="shared" si="3"/>
         <v>2.0208743926043816E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC9">
+        <f t="shared" si="4"/>
+        <v>2.219677984429333E-2</v>
+      </c>
+      <c r="AD9">
+        <f t="shared" si="5"/>
+        <v>2.418481576254284E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>74</v>
       </c>
@@ -2331,8 +2454,16 @@
         <f t="shared" si="3"/>
         <v>1.5699825850384548E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC10">
+        <f t="shared" si="4"/>
+        <v>1.795428488821418E-2</v>
+      </c>
+      <c r="AD10">
+        <f t="shared" si="5"/>
+        <v>2.0208743926043816E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>81</v>
       </c>
@@ -2415,8 +2546,16 @@
         <f t="shared" si="3"/>
         <v>2.0410885006989385E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC11">
+        <f t="shared" si="4"/>
+        <v>2.0018269245279413E-2</v>
+      </c>
+      <c r="AD11">
+        <f t="shared" si="5"/>
+        <v>1.9625653483569438E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>88</v>
       </c>
@@ -2499,8 +2638,16 @@
         <f t="shared" si="3"/>
         <v>1.9625653483569438E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC12">
+        <f t="shared" si="4"/>
+        <v>1.6932415547161402E-2</v>
+      </c>
+      <c r="AD12">
+        <f t="shared" si="5"/>
+        <v>1.4239177610753362E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>95</v>
       </c>
@@ -2583,8 +2730,16 @@
         <f t="shared" si="3"/>
         <v>2.0617111396875849E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC13">
+        <f t="shared" si="4"/>
+        <v>1.7775489958670895E-2</v>
+      </c>
+      <c r="AD13">
+        <f t="shared" si="5"/>
+        <v>1.4933868520465937E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>99</v>
       </c>
@@ -2667,8 +2822,16 @@
         <f t="shared" si="3"/>
         <v>2.5643793255555259E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC14">
+        <f t="shared" si="4"/>
+        <v>2.7403124648172694E-2</v>
+      </c>
+      <c r="AD14">
+        <f t="shared" si="5"/>
+        <v>2.9162456040790135E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>103</v>
       </c>
@@ -2751,8 +2914,16 @@
         <f t="shared" si="3"/>
         <v>2.9729034757130523E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC15">
+        <f t="shared" si="4"/>
+        <v>2.8910378904847774E-2</v>
+      </c>
+      <c r="AD15">
+        <f t="shared" si="5"/>
+        <v>2.8091723052565024E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>108</v>
       </c>
@@ -2835,8 +3006,16 @@
         <f t="shared" si="3"/>
         <v>2.4892940902771454E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC16">
+        <f t="shared" si="4"/>
+        <v>2.1984106183941941E-2</v>
+      </c>
+      <c r="AD16">
+        <f t="shared" si="5"/>
+        <v>1.9075271465112429E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>113</v>
       </c>
@@ -2919,8 +3098,16 @@
         <f t="shared" si="3"/>
         <v>2.1042325782678128E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC17">
+        <f t="shared" si="4"/>
+        <v>2.0625534854360972E-2</v>
+      </c>
+      <c r="AD17">
+        <f t="shared" si="5"/>
+        <v>2.0208743926043816E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>120</v>
       </c>
@@ -3003,8 +3190,16 @@
         <f t="shared" si="3"/>
         <v>1.6028671547642325E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC18">
+        <f t="shared" si="4"/>
+        <v>1.832289147225909E-2</v>
+      </c>
+      <c r="AD18">
+        <f t="shared" si="5"/>
+        <v>2.0617111396875849E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>126</v>
       </c>
@@ -3087,8 +3282,16 @@
         <f t="shared" si="3"/>
         <v>2.0410885006989385E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC19">
+        <f t="shared" si="4"/>
+        <v>1.7600222318099878E-2</v>
+      </c>
+      <c r="AD19">
+        <f t="shared" si="5"/>
+        <v>1.4789559629210367E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>130</v>
       </c>
@@ -3171,8 +3374,16 @@
         <f t="shared" si="3"/>
         <v>1.5699825850384548E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC20">
+        <f t="shared" si="4"/>
+        <v>1.795428488821418E-2</v>
+      </c>
+      <c r="AD20">
+        <f t="shared" si="5"/>
+        <v>2.0208743926043816E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>136</v>
       </c>
@@ -3255,8 +3466,16 @@
         <f t="shared" si="3"/>
         <v>1.6028671547642325E-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC21">
+        <f t="shared" si="4"/>
+        <v>1.832289147225909E-2</v>
+      </c>
+      <c r="AD21">
+        <f t="shared" si="5"/>
+        <v>2.0617111396875849E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>141</v>
       </c>
@@ -3339,8 +3558,16 @@
         <f t="shared" si="3"/>
         <v>1.5231103647796521E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC22">
+        <f t="shared" si="4"/>
+        <v>1.7428378565682977E-2</v>
+      </c>
+      <c r="AD22">
+        <f t="shared" si="5"/>
+        <v>1.9625653483569438E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>144</v>
       </c>
@@ -3423,8 +3650,16 @@
         <f t="shared" si="3"/>
         <v>2.1042325782678128E-2</v>
       </c>
-    </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC23">
+        <f t="shared" si="4"/>
+        <v>2.3090308046130589E-2</v>
+      </c>
+      <c r="AD23">
+        <f t="shared" si="5"/>
+        <v>2.5138290309583051E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>149</v>
       </c>
@@ -3507,8 +3742,16 @@
         <f t="shared" si="3"/>
         <v>2.0617111396875849E-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC24">
+        <f t="shared" si="4"/>
+        <v>2.021667644238281E-2</v>
+      </c>
+      <c r="AD24">
+        <f t="shared" si="5"/>
+        <v>1.9816241487889776E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>154</v>
       </c>
@@ -3591,8 +3834,16 @@
         <f t="shared" si="3"/>
         <v>2.5904247639501662E-2</v>
       </c>
-    </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC25">
+        <f t="shared" si="4"/>
+        <v>2.5278291490875252E-2</v>
+      </c>
+      <c r="AD25">
+        <f t="shared" si="5"/>
+        <v>2.4652335342248845E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>157</v>
       </c>
@@ -3675,8 +3926,16 @@
         <f t="shared" si="3"/>
         <v>2.1042325782678128E-2</v>
       </c>
-    </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC26">
+        <f t="shared" si="4"/>
+        <v>2.0625534854360972E-2</v>
+      </c>
+      <c r="AD26">
+        <f t="shared" si="5"/>
+        <v>2.0208743926043816E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>163</v>
       </c>
@@ -3759,8 +4018,16 @@
         <f t="shared" si="3"/>
         <v>2.0617111396875849E-2</v>
       </c>
-    </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC27">
+        <f t="shared" si="4"/>
+        <v>2.021667644238281E-2</v>
+      </c>
+      <c r="AD27">
+        <f t="shared" si="5"/>
+        <v>1.9816241487889776E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>166</v>
       </c>
@@ -3843,8 +4110,16 @@
         <f t="shared" si="3"/>
         <v>1.586254442348526E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC28">
+        <f t="shared" si="4"/>
+        <v>1.8136714715237322E-2</v>
+      </c>
+      <c r="AD28">
+        <f t="shared" si="5"/>
+        <v>2.0410885006989385E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>171</v>
       </c>
@@ -3927,8 +4202,16 @@
         <f t="shared" si="3"/>
         <v>2.0827548224619984E-2</v>
       </c>
-    </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC29">
+        <f t="shared" si="4"/>
+        <v>1.795428488821418E-2</v>
+      </c>
+      <c r="AD29">
+        <f t="shared" si="5"/>
+        <v>1.5081021551808382E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>176</v>
       </c>
@@ -4011,8 +4294,16 @@
         <f t="shared" si="3"/>
         <v>2.1042325782678128E-2</v>
       </c>
-    </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC30">
+        <f t="shared" si="4"/>
+        <v>2.0625534854360972E-2</v>
+      </c>
+      <c r="AD30">
+        <f t="shared" si="5"/>
+        <v>2.0208743926043816E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>180</v>
       </c>
@@ -4095,8 +4386,16 @@
         <f t="shared" si="3"/>
         <v>2.0208743926043816E-2</v>
       </c>
-    </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC31">
+        <f t="shared" si="4"/>
+        <v>1.9823720491662328E-2</v>
+      </c>
+      <c r="AD31">
+        <f t="shared" si="5"/>
+        <v>1.9438697057280834E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>185</v>
       </c>
@@ -4179,8 +4478,16 @@
         <f t="shared" si="3"/>
         <v>2.1042325782678128E-2</v>
       </c>
-    </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC32">
+        <f t="shared" si="4"/>
+        <v>2.0625534854360972E-2</v>
+      </c>
+      <c r="AD32">
+        <f t="shared" si="5"/>
+        <v>2.0208743926043816E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>190</v>
       </c>
@@ -4263,8 +4570,16 @@
         <f t="shared" si="3"/>
         <v>2.0617111396875849E-2</v>
       </c>
-    </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC33">
+        <f t="shared" si="4"/>
+        <v>2.2634723369562348E-2</v>
+      </c>
+      <c r="AD33">
+        <f t="shared" si="5"/>
+        <v>2.4652335342248845E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>193</v>
       </c>
@@ -4347,8 +4662,16 @@
         <f t="shared" si="3"/>
         <v>2.0617111396875849E-2</v>
       </c>
-    </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC34">
+        <f t="shared" si="4"/>
+        <v>1.7775489958670895E-2</v>
+      </c>
+      <c r="AD34">
+        <f t="shared" si="5"/>
+        <v>1.4933868520465937E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>196</v>
       </c>
@@ -4431,8 +4754,16 @@
         <f t="shared" si="3"/>
         <v>2.0410885006989385E-2</v>
       </c>
-    </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC35">
+        <f t="shared" si="4"/>
+        <v>2.2413611171258761E-2</v>
+      </c>
+      <c r="AD35">
+        <f t="shared" si="5"/>
+        <v>2.4416337335528129E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>199</v>
       </c>
@@ -4515,8 +4846,16 @@
         <f t="shared" si="3"/>
         <v>2.1261579796208196E-2</v>
       </c>
-    </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC36">
+        <f t="shared" si="4"/>
+        <v>2.0836232401598792E-2</v>
+      </c>
+      <c r="AD36">
+        <f t="shared" si="5"/>
+        <v>2.0410885006989385E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>203</v>
       </c>
@@ -4599,8 +4938,16 @@
         <f t="shared" si="3"/>
         <v>2.0617111396875849E-2</v>
       </c>
-    </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC37">
+        <f t="shared" si="4"/>
+        <v>2.021667644238281E-2</v>
+      </c>
+      <c r="AD37">
+        <f t="shared" si="5"/>
+        <v>1.9816241487889776E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>207</v>
       </c>
@@ -4683,8 +5030,16 @@
         <f t="shared" si="3"/>
         <v>2.0208743926043816E-2</v>
       </c>
-    </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC38">
+        <f t="shared" si="4"/>
+        <v>1.9823720491662328E-2</v>
+      </c>
+      <c r="AD38">
+        <f t="shared" si="5"/>
+        <v>1.9438697057280834E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>211</v>
       </c>
@@ -4767,8 +5122,16 @@
         <f t="shared" si="3"/>
         <v>1.5384203148309978E-2</v>
       </c>
-    </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC39">
+        <f t="shared" si="4"/>
+        <v>1.7600222318099878E-2</v>
+      </c>
+      <c r="AD39">
+        <f t="shared" si="5"/>
+        <v>1.9816241487889776E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>215</v>
       </c>
@@ -4851,8 +5214,16 @@
         <f t="shared" si="3"/>
         <v>2.0617111396875849E-2</v>
       </c>
-    </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC40">
+        <f t="shared" si="4"/>
+        <v>2.2634723369562348E-2</v>
+      </c>
+      <c r="AD40">
+        <f t="shared" si="5"/>
+        <v>2.4652335342248845E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>218</v>
       </c>
@@ -4935,8 +5306,16 @@
         <f t="shared" si="3"/>
         <v>3.6273429430474645E-2</v>
       </c>
-    </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC41">
+        <f t="shared" si="4"/>
+        <v>3.5069130262398725E-2</v>
+      </c>
+      <c r="AD41">
+        <f t="shared" si="5"/>
+        <v>3.3864831094322805E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>222</v>
       </c>
@@ -5019,8 +5398,16 @@
         <f t="shared" si="3"/>
         <v>1.5540411981994171E-2</v>
       </c>
-    </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC42">
+        <f t="shared" si="4"/>
+        <v>1.7775489958670895E-2</v>
+      </c>
+      <c r="AD42">
+        <f t="shared" si="5"/>
+        <v>2.0010567935347619E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>226</v>
       </c>
@@ -5103,8 +5490,16 @@
         <f t="shared" si="3"/>
         <v>2.0208743926043816E-2</v>
       </c>
-    </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC43">
+        <f t="shared" si="4"/>
+        <v>1.9823720491662328E-2</v>
+      </c>
+      <c r="AD43">
+        <f t="shared" si="5"/>
+        <v>1.9438697057280834E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>228</v>
       </c>
@@ -5187,8 +5582,16 @@
         <f t="shared" si="3"/>
         <v>1.5231103647796521E-2</v>
       </c>
-    </row>
-    <row r="45" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC44">
+        <f t="shared" si="4"/>
+        <v>1.7428378565682977E-2</v>
+      </c>
+      <c r="AD44">
+        <f t="shared" si="5"/>
+        <v>1.9625653483569438E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>232</v>
       </c>
@@ -5271,8 +5674,16 @@
         <f t="shared" si="3"/>
         <v>2.0410885006989385E-2</v>
       </c>
-    </row>
-    <row r="46" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC45">
+        <f t="shared" si="4"/>
+        <v>1.7600222318099878E-2</v>
+      </c>
+      <c r="AD45">
+        <f t="shared" si="5"/>
+        <v>1.4789559629210367E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>235</v>
       </c>
@@ -5355,8 +5766,16 @@
         <f t="shared" si="3"/>
         <v>1.5231103647796521E-2</v>
       </c>
-    </row>
-    <row r="47" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC46">
+        <f t="shared" si="4"/>
+        <v>1.7428378565682977E-2</v>
+      </c>
+      <c r="AD46">
+        <f t="shared" si="5"/>
+        <v>1.9625653483569438E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>237</v>
       </c>
@@ -5439,8 +5858,16 @@
         <f t="shared" si="3"/>
         <v>1.5384203148309978E-2</v>
       </c>
-    </row>
-    <row r="48" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC47">
+        <f t="shared" si="4"/>
+        <v>1.7600222318099878E-2</v>
+      </c>
+      <c r="AD47">
+        <f t="shared" si="5"/>
+        <v>1.9816241487889776E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>240</v>
       </c>
@@ -5523,8 +5950,16 @@
         <f t="shared" si="3"/>
         <v>2.0208743926043816E-2</v>
       </c>
-    </row>
-    <row r="49" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC48">
+        <f t="shared" si="4"/>
+        <v>1.9823720491662328E-2</v>
+      </c>
+      <c r="AD48">
+        <f t="shared" si="5"/>
+        <v>1.9438697057280834E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>243</v>
       </c>
@@ -5607,8 +6042,16 @@
         <f t="shared" si="3"/>
         <v>2.0617111396875849E-2</v>
       </c>
-    </row>
-    <row r="50" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC49">
+        <f t="shared" si="4"/>
+        <v>2.021667644238281E-2</v>
+      </c>
+      <c r="AD49">
+        <f t="shared" si="5"/>
+        <v>1.9816241487889776E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>246</v>
       </c>
@@ -5691,8 +6134,16 @@
         <f t="shared" si="3"/>
         <v>2.0827548224619984E-2</v>
       </c>
-    </row>
-    <row r="51" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC50">
+        <f t="shared" si="4"/>
+        <v>2.0419058079983801E-2</v>
+      </c>
+      <c r="AD50">
+        <f t="shared" si="5"/>
+        <v>2.0010567935347619E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>248</v>
       </c>
@@ -5775,8 +6226,16 @@
         <f t="shared" si="3"/>
         <v>3.1246747571795241E-2</v>
       </c>
-    </row>
-    <row r="52" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC51">
+        <f t="shared" si="4"/>
+        <v>3.0344883383001391E-2</v>
+      </c>
+      <c r="AD51">
+        <f t="shared" si="5"/>
+        <v>2.9443019194207536E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>252</v>
       </c>
@@ -5859,8 +6318,16 @@
         <f t="shared" si="3"/>
         <v>1.6028671547642325E-2</v>
       </c>
-    </row>
-    <row r="53" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC52">
+        <f t="shared" si="4"/>
+        <v>1.5784541764818246E-2</v>
+      </c>
+      <c r="AD52">
+        <f t="shared" si="5"/>
+        <v>1.5540411981994171E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>255</v>
       </c>
@@ -5943,8 +6410,16 @@
         <f t="shared" si="3"/>
         <v>2.0010567935347619E-2</v>
       </c>
-    </row>
-    <row r="54" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC53">
+        <f t="shared" si="4"/>
+        <v>2.1984106183941941E-2</v>
+      </c>
+      <c r="AD53">
+        <f t="shared" si="5"/>
+        <v>2.3957644432536267E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>259</v>
       </c>
@@ -6027,8 +6502,16 @@
         <f t="shared" si="3"/>
         <v>2.6718359957814238E-2</v>
       </c>
-    </row>
-    <row r="55" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC54">
+        <f t="shared" si="4"/>
+        <v>2.851821581329508E-2</v>
+      </c>
+      <c r="AD54">
+        <f t="shared" si="5"/>
+        <v>3.0318071668775915E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>262</v>
       </c>
@@ -6111,8 +6594,16 @@
         <f t="shared" si="3"/>
         <v>1.5540411981994171E-2</v>
       </c>
-    </row>
-    <row r="56" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC55">
+        <f t="shared" si="4"/>
+        <v>1.7775489958670895E-2</v>
+      </c>
+      <c r="AD55">
+        <f t="shared" si="5"/>
+        <v>2.0010567935347619E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>265</v>
       </c>
@@ -6195,8 +6686,16 @@
         <f t="shared" si="3"/>
         <v>2.538852528523668E-2</v>
       </c>
-    </row>
-    <row r="57" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC56">
+        <f t="shared" si="4"/>
+        <v>2.4786670523889762E-2</v>
+      </c>
+      <c r="AD56">
+        <f t="shared" si="5"/>
+        <v>2.418481576254284E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>268</v>
       </c>
@@ -6279,8 +6778,16 @@
         <f t="shared" si="3"/>
         <v>2.0617111396875849E-2</v>
       </c>
-    </row>
-    <row r="58" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC57">
+        <f t="shared" si="4"/>
+        <v>2.021667644238281E-2</v>
+      </c>
+      <c r="AD57">
+        <f t="shared" si="5"/>
+        <v>1.9816241487889776E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>270</v>
       </c>
@@ -6363,8 +6870,16 @@
         <f t="shared" si="3"/>
         <v>1.5384203148309978E-2</v>
       </c>
-    </row>
-    <row r="59" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC58">
+        <f t="shared" si="4"/>
+        <v>1.7600222318099878E-2</v>
+      </c>
+      <c r="AD58">
+        <f t="shared" si="5"/>
+        <v>1.9816241487889776E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>273</v>
       </c>
@@ -6447,8 +6962,16 @@
         <f t="shared" si="3"/>
         <v>2.1485451709248368E-2</v>
       </c>
-    </row>
-    <row r="60" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC59">
+        <f t="shared" si="4"/>
+        <v>2.1051281553062108E-2</v>
+      </c>
+      <c r="AD59">
+        <f t="shared" si="5"/>
+        <v>2.0617111396875849E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>276</v>
       </c>
@@ -6531,8 +7054,16 @@
         <f t="shared" si="3"/>
         <v>1.5540411981994171E-2</v>
       </c>
-    </row>
-    <row r="61" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC60">
+        <f t="shared" si="4"/>
+        <v>1.7775489958670895E-2</v>
+      </c>
+      <c r="AD60">
+        <f t="shared" si="5"/>
+        <v>2.0010567935347619E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>279</v>
       </c>
@@ -6615,8 +7146,16 @@
         <f t="shared" si="3"/>
         <v>1.5231103647796521E-2</v>
       </c>
-    </row>
-    <row r="62" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC61">
+        <f t="shared" si="4"/>
+        <v>1.7428378565682977E-2</v>
+      </c>
+      <c r="AD61">
+        <f t="shared" si="5"/>
+        <v>1.9625653483569438E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>282</v>
       </c>
@@ -6699,8 +7238,16 @@
         <f t="shared" si="3"/>
         <v>3.0020663277006889E-2</v>
       </c>
-    </row>
-    <row r="63" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC62">
+        <f t="shared" si="4"/>
+        <v>2.9186314075955181E-2</v>
+      </c>
+      <c r="AD62">
+        <f t="shared" si="5"/>
+        <v>2.8351964874903473E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>287</v>
       </c>
@@ -6783,8 +7330,16 @@
         <f t="shared" si="3"/>
         <v>3.0930929498181069E-2</v>
       </c>
-    </row>
-    <row r="64" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC63">
+        <f t="shared" si="4"/>
+        <v>3.0046692769485604E-2</v>
+      </c>
+      <c r="AD63">
+        <f t="shared" si="5"/>
+        <v>2.9162456040790135E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>291</v>
       </c>
@@ -6867,8 +7422,16 @@
         <f t="shared" si="3"/>
         <v>1.5540411981994171E-2</v>
       </c>
-    </row>
-    <row r="65" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC64">
+        <f t="shared" si="4"/>
+        <v>1.7775489958670895E-2</v>
+      </c>
+      <c r="AD64">
+        <f t="shared" si="5"/>
+        <v>2.0010567935347619E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>293</v>
       </c>
@@ -6951,8 +7514,16 @@
         <f t="shared" si="3"/>
         <v>2.0827548224619984E-2</v>
       </c>
-    </row>
-    <row r="66" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC65">
+        <f t="shared" si="4"/>
+        <v>1.795428488821418E-2</v>
+      </c>
+      <c r="AD65">
+        <f t="shared" si="5"/>
+        <v>1.5081021551808382E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>296</v>
       </c>
@@ -7035,8 +7606,16 @@
         <f t="shared" si="3"/>
         <v>2.0410885006989385E-2</v>
       </c>
-    </row>
-    <row r="67" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC66">
+        <f t="shared" si="4"/>
+        <v>1.7600222318099878E-2</v>
+      </c>
+      <c r="AD66">
+        <f t="shared" si="5"/>
+        <v>1.4789559629210367E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>300</v>
       </c>
@@ -7119,8 +7698,16 @@
         <f t="shared" si="3"/>
         <v>2.0208743926043816E-2</v>
       </c>
-    </row>
-    <row r="68" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC67">
+        <f t="shared" si="4"/>
+        <v>1.9823720491662328E-2</v>
+      </c>
+      <c r="AD67">
+        <f t="shared" si="5"/>
+        <v>1.9438697057280834E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>303</v>
       </c>
@@ -7172,11 +7759,11 @@
         <v>322035</v>
       </c>
       <c r="S68">
-        <f t="shared" ref="S68:S72" si="4">_xlfn.T.INV.2T(Q68,R68)</f>
+        <f t="shared" ref="S68:S72" si="6">_xlfn.T.INV.2T(Q68,R68)</f>
         <v>5.5415731179516623</v>
       </c>
       <c r="T68">
-        <f t="shared" ref="T68:T72" si="5">ABS(S68)</f>
+        <f t="shared" ref="T68:T72" si="7">ABS(S68)</f>
         <v>5.5415731179516623</v>
       </c>
       <c r="U68" t="str">
@@ -7184,7 +7771,7 @@
         <v>0.040</v>
       </c>
       <c r="V68">
-        <f t="shared" ref="V68:V72" si="6">U68/T68</f>
+        <f t="shared" ref="V68:V72" si="8">U68/T68</f>
         <v>7.21816696245005E-3</v>
       </c>
       <c r="Y68">
@@ -7200,11 +7787,19 @@
         <v>0.13976194237515863</v>
       </c>
       <c r="AB68">
-        <f t="shared" ref="AB68:AB72" si="7">(Y68-Z68)/1.96</f>
+        <f t="shared" ref="AB68:AB72" si="9">(Y68-Z68)/1.96</f>
         <v>4.0036538490558826E-2</v>
       </c>
-    </row>
-    <row r="69" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC68">
+        <f t="shared" ref="AC68:AC72" si="10">(AA68-Z68)/2/1.96</f>
+        <v>4.0807308595070944E-2</v>
+      </c>
+      <c r="AD68">
+        <f t="shared" ref="AD68:AD72" si="11">(AA68-Y68)/1.96</f>
+        <v>4.1578078699583063E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>308</v>
       </c>
@@ -7256,11 +7851,11 @@
         <v>322035</v>
       </c>
       <c r="S69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>5.5196170398503144</v>
       </c>
       <c r="T69">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5.5196170398503144</v>
       </c>
       <c r="U69" t="str">
@@ -7268,7 +7863,7 @@
         <v>0.019</v>
       </c>
       <c r="V69">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>3.4422677991651496E-3</v>
       </c>
       <c r="Y69">
@@ -7284,11 +7879,19 @@
         <v>5.8268908123975824E-2</v>
       </c>
       <c r="AB69">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2.0410885006989385E-2</v>
       </c>
-    </row>
-    <row r="70" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC69">
+        <f t="shared" si="10"/>
+        <v>2.0018269245279413E-2</v>
+      </c>
+      <c r="AD69">
+        <f t="shared" si="11"/>
+        <v>1.9625653483569438E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>312</v>
       </c>
@@ -7340,11 +7943,11 @@
         <v>322035</v>
       </c>
       <c r="S70">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>5.49545425854319</v>
       </c>
       <c r="T70">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5.49545425854319</v>
       </c>
       <c r="U70" t="str">
@@ -7352,7 +7955,7 @@
         <v>0.022</v>
       </c>
       <c r="V70">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>4.0033087284456915E-3</v>
       </c>
       <c r="Y70">
@@ -7368,11 +7971,19 @@
         <v>3.9220713153281329E-2</v>
       </c>
       <c r="AB70">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2.1042325782678128E-2</v>
       </c>
-    </row>
-    <row r="71" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC70">
+        <f t="shared" si="10"/>
+        <v>2.3090308046130589E-2</v>
+      </c>
+      <c r="AD70">
+        <f t="shared" si="11"/>
+        <v>2.5138290309583051E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>316</v>
       </c>
@@ -7424,11 +8035,11 @@
         <v>322035</v>
       </c>
       <c r="S71">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>5.4823612021473993</v>
       </c>
       <c r="T71">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5.4823612021473993</v>
       </c>
       <c r="U71" t="str">
@@ -7436,7 +8047,7 @@
         <v>0.017</v>
       </c>
       <c r="V71">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>3.1008536966410077E-3</v>
       </c>
       <c r="Y71">
@@ -7452,11 +8063,19 @@
         <v>3.9220713153281329E-2</v>
       </c>
       <c r="AB71">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2.0827548224619984E-2</v>
       </c>
-    </row>
-    <row r="72" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC71">
+        <f t="shared" si="10"/>
+        <v>2.0419058079983801E-2</v>
+      </c>
+      <c r="AD71">
+        <f t="shared" si="11"/>
+        <v>2.0010567935347619E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>319</v>
       </c>
@@ -7508,11 +8127,11 @@
         <v>322035</v>
       </c>
       <c r="S72">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>5.4550317441294514</v>
       </c>
       <c r="T72">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5.4550317441294514</v>
       </c>
       <c r="U72" t="str">
@@ -7520,7 +8139,7 @@
         <v>0.019</v>
       </c>
       <c r="V72">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>3.4830228110857933E-3</v>
       </c>
       <c r="Y72">
@@ -7536,8 +8155,16 @@
         <v>3.9220713153281329E-2</v>
       </c>
       <c r="AB72">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2.0827548224619984E-2</v>
+      </c>
+      <c r="AC72">
+        <f t="shared" si="10"/>
+        <v>2.0419058079983801E-2</v>
+      </c>
+      <c r="AD72">
+        <f t="shared" si="11"/>
+        <v>2.0010567935347619E-2</v>
       </c>
     </row>
   </sheetData>
@@ -7550,12 +8177,2501 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE890338-A9EB-449D-8D4F-895A2109274B}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K71"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G71"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>337</v>
+      </c>
+      <c r="B1" t="s">
+        <v>338</v>
+      </c>
+      <c r="C1" t="s">
+        <v>339</v>
+      </c>
+      <c r="D1" t="s">
+        <v>340</v>
+      </c>
+      <c r="E1" t="s">
+        <v>341</v>
+      </c>
+      <c r="F1" t="s">
+        <v>342</v>
+      </c>
+      <c r="G1" t="s">
+        <v>343</v>
+      </c>
+      <c r="H1" t="s">
+        <v>344</v>
+      </c>
+      <c r="I1" t="s">
+        <v>345</v>
+      </c>
+      <c r="J1" t="s">
+        <v>346</v>
+      </c>
+      <c r="K1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>348</v>
+      </c>
+      <c r="B2" t="s">
+        <v>349</v>
+      </c>
+      <c r="C2" t="s">
+        <v>350</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>351</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" t="s">
+        <v>352</v>
+      </c>
+      <c r="H2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2">
+        <v>1.7106513699587575E-3</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>1.7775489958670895E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>348</v>
+      </c>
+      <c r="B3" t="s">
+        <v>349</v>
+      </c>
+      <c r="C3" t="s">
+        <v>350</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>351</v>
+      </c>
+      <c r="F3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" t="s">
+        <v>352</v>
+      </c>
+      <c r="H3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I3">
+        <v>3.649024665057384E-3</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>2.0419058079983801E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>348</v>
+      </c>
+      <c r="B4" t="s">
+        <v>349</v>
+      </c>
+      <c r="C4" t="s">
+        <v>350</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>351</v>
+      </c>
+      <c r="F4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" t="s">
+        <v>352</v>
+      </c>
+      <c r="H4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I4">
+        <v>4.0064745893953089E-3</v>
+      </c>
+      <c r="J4">
+        <v>4.8790164169432049E-2</v>
+      </c>
+      <c r="K4">
+        <v>2.1775471671213478E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>348</v>
+      </c>
+      <c r="B5" t="s">
+        <v>349</v>
+      </c>
+      <c r="C5" t="s">
+        <v>350</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>351</v>
+      </c>
+      <c r="F5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" t="s">
+        <v>352</v>
+      </c>
+      <c r="H5" t="s">
+        <v>51</v>
+      </c>
+      <c r="I5">
+        <v>3.0940714867255959E-3</v>
+      </c>
+      <c r="J5">
+        <v>1.980262729617973E-2</v>
+      </c>
+      <c r="K5">
+        <v>1.5010331638503445E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>348</v>
+      </c>
+      <c r="B6" t="s">
+        <v>349</v>
+      </c>
+      <c r="C6" t="s">
+        <v>350</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>351</v>
+      </c>
+      <c r="F6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G6" t="s">
+        <v>352</v>
+      </c>
+      <c r="H6" t="s">
+        <v>58</v>
+      </c>
+      <c r="I6">
+        <v>3.8703756544317736E-3</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>2.286024456369572E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>348</v>
+      </c>
+      <c r="B7" t="s">
+        <v>349</v>
+      </c>
+      <c r="C7" t="s">
+        <v>350</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" t="s">
+        <v>351</v>
+      </c>
+      <c r="F7" t="s">
+        <v>62</v>
+      </c>
+      <c r="G7" t="s">
+        <v>352</v>
+      </c>
+      <c r="H7" t="s">
+        <v>65</v>
+      </c>
+      <c r="I7">
+        <v>4.017638968914862E-3</v>
+      </c>
+      <c r="J7">
+        <v>3.9220713153281329E-2</v>
+      </c>
+      <c r="K7">
+        <v>2.219677984429333E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>348</v>
+      </c>
+      <c r="B8" t="s">
+        <v>349</v>
+      </c>
+      <c r="C8" t="s">
+        <v>350</v>
+      </c>
+      <c r="D8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" t="s">
+        <v>351</v>
+      </c>
+      <c r="F8" t="s">
+        <v>69</v>
+      </c>
+      <c r="G8" t="s">
+        <v>352</v>
+      </c>
+      <c r="H8" t="s">
+        <v>72</v>
+      </c>
+      <c r="I8">
+        <v>3.7386530646937952E-3</v>
+      </c>
+      <c r="J8">
+        <v>2.9558802241544429E-2</v>
+      </c>
+      <c r="K8">
+        <v>2.219677984429333E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>348</v>
+      </c>
+      <c r="B9" t="s">
+        <v>349</v>
+      </c>
+      <c r="C9" t="s">
+        <v>350</v>
+      </c>
+      <c r="D9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" t="s">
+        <v>351</v>
+      </c>
+      <c r="F9" t="s">
+        <v>74</v>
+      </c>
+      <c r="G9" t="s">
+        <v>352</v>
+      </c>
+      <c r="H9" t="s">
+        <v>77</v>
+      </c>
+      <c r="I9">
+        <v>3.1102284521522887E-3</v>
+      </c>
+      <c r="J9">
+        <v>-1.0050335853501451E-2</v>
+      </c>
+      <c r="K9">
+        <v>1.795428488821418E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>348</v>
+      </c>
+      <c r="B10" t="s">
+        <v>349</v>
+      </c>
+      <c r="C10" t="s">
+        <v>350</v>
+      </c>
+      <c r="D10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" t="s">
+        <v>351</v>
+      </c>
+      <c r="F10" t="s">
+        <v>81</v>
+      </c>
+      <c r="G10" t="s">
+        <v>352</v>
+      </c>
+      <c r="H10" t="s">
+        <v>84</v>
+      </c>
+      <c r="I10">
+        <v>3.1802854664185814E-3</v>
+      </c>
+      <c r="J10">
+        <v>1.980262729617973E-2</v>
+      </c>
+      <c r="K10">
+        <v>2.0018269245279413E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>348</v>
+      </c>
+      <c r="B11" t="s">
+        <v>349</v>
+      </c>
+      <c r="C11" t="s">
+        <v>350</v>
+      </c>
+      <c r="D11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" t="s">
+        <v>351</v>
+      </c>
+      <c r="F11" t="s">
+        <v>88</v>
+      </c>
+      <c r="G11" t="s">
+        <v>352</v>
+      </c>
+      <c r="H11" t="s">
+        <v>91</v>
+      </c>
+      <c r="I11">
+        <v>3.0830327170072495E-3</v>
+      </c>
+      <c r="J11">
+        <v>5.8268908123975824E-2</v>
+      </c>
+      <c r="K11">
+        <v>1.6932415547161402E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>348</v>
+      </c>
+      <c r="B12" t="s">
+        <v>349</v>
+      </c>
+      <c r="C12" t="s">
+        <v>350</v>
+      </c>
+      <c r="D12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" t="s">
+        <v>351</v>
+      </c>
+      <c r="F12" t="s">
+        <v>95</v>
+      </c>
+      <c r="G12" t="s">
+        <v>352</v>
+      </c>
+      <c r="H12" t="s">
+        <v>91</v>
+      </c>
+      <c r="I12">
+        <v>3.1217885107430307E-3</v>
+      </c>
+      <c r="J12">
+        <v>9.950330853168092E-3</v>
+      </c>
+      <c r="K12">
+        <v>1.7775489958670895E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>348</v>
+      </c>
+      <c r="B13" t="s">
+        <v>349</v>
+      </c>
+      <c r="C13" t="s">
+        <v>350</v>
+      </c>
+      <c r="D13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" t="s">
+        <v>351</v>
+      </c>
+      <c r="F13" t="s">
+        <v>99</v>
+      </c>
+      <c r="G13" t="s">
+        <v>352</v>
+      </c>
+      <c r="H13" t="s">
+        <v>65</v>
+      </c>
+      <c r="I13">
+        <v>4.6164610650375592E-3</v>
+      </c>
+      <c r="J13">
+        <v>1.980262729617973E-2</v>
+      </c>
+      <c r="K13">
+        <v>2.7403124648172694E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>348</v>
+      </c>
+      <c r="B14" t="s">
+        <v>349</v>
+      </c>
+      <c r="C14" t="s">
+        <v>350</v>
+      </c>
+      <c r="D14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" t="s">
+        <v>351</v>
+      </c>
+      <c r="F14" t="s">
+        <v>103</v>
+      </c>
+      <c r="G14" t="s">
+        <v>352</v>
+      </c>
+      <c r="H14" t="s">
+        <v>51</v>
+      </c>
+      <c r="I14">
+        <v>4.5505201226154141E-3</v>
+      </c>
+      <c r="J14">
+        <v>5.8268908123975824E-2</v>
+      </c>
+      <c r="K14">
+        <v>2.8910378904847774E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>348</v>
+      </c>
+      <c r="B15" t="s">
+        <v>349</v>
+      </c>
+      <c r="C15" t="s">
+        <v>350</v>
+      </c>
+      <c r="D15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" t="s">
+        <v>351</v>
+      </c>
+      <c r="F15" t="s">
+        <v>108</v>
+      </c>
+      <c r="G15" t="s">
+        <v>352</v>
+      </c>
+      <c r="H15" t="s">
+        <v>111</v>
+      </c>
+      <c r="I15">
+        <v>4.1554174164966174E-3</v>
+      </c>
+      <c r="J15">
+        <v>4.8790164169432049E-2</v>
+      </c>
+      <c r="K15">
+        <v>2.1984106183941941E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>348</v>
+      </c>
+      <c r="B16" t="s">
+        <v>349</v>
+      </c>
+      <c r="C16" t="s">
+        <v>350</v>
+      </c>
+      <c r="D16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" t="s">
+        <v>351</v>
+      </c>
+      <c r="F16" t="s">
+        <v>113</v>
+      </c>
+      <c r="G16" t="s">
+        <v>352</v>
+      </c>
+      <c r="H16" t="s">
+        <v>91</v>
+      </c>
+      <c r="I16">
+        <v>3.6469588572924081E-3</v>
+      </c>
+      <c r="J16">
+        <v>-1.0050335853501451E-2</v>
+      </c>
+      <c r="K16">
+        <v>2.0625534854360972E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>348</v>
+      </c>
+      <c r="B17" t="s">
+        <v>349</v>
+      </c>
+      <c r="C17" t="s">
+        <v>350</v>
+      </c>
+      <c r="D17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" t="s">
+        <v>351</v>
+      </c>
+      <c r="F17" t="s">
+        <v>120</v>
+      </c>
+      <c r="G17" t="s">
+        <v>352</v>
+      </c>
+      <c r="H17" t="s">
+        <v>122</v>
+      </c>
+      <c r="I17">
+        <v>3.1016834013285568E-3</v>
+      </c>
+      <c r="J17">
+        <v>-3.0459207484708574E-2</v>
+      </c>
+      <c r="K17">
+        <v>1.832289147225909E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>348</v>
+      </c>
+      <c r="B18" t="s">
+        <v>349</v>
+      </c>
+      <c r="C18" t="s">
+        <v>350</v>
+      </c>
+      <c r="D18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" t="s">
+        <v>351</v>
+      </c>
+      <c r="F18" t="s">
+        <v>126</v>
+      </c>
+      <c r="G18" t="s">
+        <v>352</v>
+      </c>
+      <c r="H18" t="s">
+        <v>122</v>
+      </c>
+      <c r="I18">
+        <v>3.1093712759504904E-3</v>
+      </c>
+      <c r="J18">
+        <v>1.980262729617973E-2</v>
+      </c>
+      <c r="K18">
+        <v>1.7600222318099878E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>348</v>
+      </c>
+      <c r="B19" t="s">
+        <v>349</v>
+      </c>
+      <c r="C19" t="s">
+        <v>350</v>
+      </c>
+      <c r="D19" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" t="s">
+        <v>351</v>
+      </c>
+      <c r="F19" t="s">
+        <v>130</v>
+      </c>
+      <c r="G19" t="s">
+        <v>352</v>
+      </c>
+      <c r="H19" t="s">
+        <v>133</v>
+      </c>
+      <c r="I19">
+        <v>3.0459209921138621E-3</v>
+      </c>
+      <c r="J19">
+        <v>-1.0050335853501451E-2</v>
+      </c>
+      <c r="K19">
+        <v>1.795428488821418E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>348</v>
+      </c>
+      <c r="B20" t="s">
+        <v>349</v>
+      </c>
+      <c r="C20" t="s">
+        <v>350</v>
+      </c>
+      <c r="D20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" t="s">
+        <v>351</v>
+      </c>
+      <c r="F20" t="s">
+        <v>136</v>
+      </c>
+      <c r="G20" t="s">
+        <v>352</v>
+      </c>
+      <c r="H20" t="s">
+        <v>139</v>
+      </c>
+      <c r="I20">
+        <v>3.5748833303499571E-3</v>
+      </c>
+      <c r="J20">
+        <v>-3.0459207484708574E-2</v>
+      </c>
+      <c r="K20">
+        <v>1.832289147225909E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>348</v>
+      </c>
+      <c r="B21" t="s">
+        <v>349</v>
+      </c>
+      <c r="C21" t="s">
+        <v>350</v>
+      </c>
+      <c r="D21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" t="s">
+        <v>351</v>
+      </c>
+      <c r="F21" t="s">
+        <v>141</v>
+      </c>
+      <c r="G21" t="s">
+        <v>352</v>
+      </c>
+      <c r="H21" t="s">
+        <v>133</v>
+      </c>
+      <c r="I21">
+        <v>3.1102577503204702E-3</v>
+      </c>
+      <c r="J21">
+        <v>1.980262729617973E-2</v>
+      </c>
+      <c r="K21">
+        <v>1.7428378565682977E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>348</v>
+      </c>
+      <c r="B22" t="s">
+        <v>349</v>
+      </c>
+      <c r="C22" t="s">
+        <v>350</v>
+      </c>
+      <c r="D22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" t="s">
+        <v>351</v>
+      </c>
+      <c r="F22" t="s">
+        <v>144</v>
+      </c>
+      <c r="G22" t="s">
+        <v>352</v>
+      </c>
+      <c r="H22" t="s">
+        <v>147</v>
+      </c>
+      <c r="I22">
+        <v>3.9103977687082164E-3</v>
+      </c>
+      <c r="J22">
+        <v>-1.0050335853501451E-2</v>
+      </c>
+      <c r="K22">
+        <v>2.3090308046130589E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>348</v>
+      </c>
+      <c r="B23" t="s">
+        <v>349</v>
+      </c>
+      <c r="C23" t="s">
+        <v>350</v>
+      </c>
+      <c r="D23" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" t="s">
+        <v>351</v>
+      </c>
+      <c r="F23" t="s">
+        <v>149</v>
+      </c>
+      <c r="G23" t="s">
+        <v>352</v>
+      </c>
+      <c r="H23" t="s">
+        <v>152</v>
+      </c>
+      <c r="I23">
+        <v>3.3351457186432043E-3</v>
+      </c>
+      <c r="J23">
+        <v>9.950330853168092E-3</v>
+      </c>
+      <c r="K23">
+        <v>2.021667644238281E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>348</v>
+      </c>
+      <c r="B24" t="s">
+        <v>349</v>
+      </c>
+      <c r="C24" t="s">
+        <v>350</v>
+      </c>
+      <c r="D24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" t="s">
+        <v>351</v>
+      </c>
+      <c r="F24" t="s">
+        <v>154</v>
+      </c>
+      <c r="G24" t="s">
+        <v>352</v>
+      </c>
+      <c r="H24" t="s">
+        <v>77</v>
+      </c>
+      <c r="I24">
+        <v>4.6363533717789568E-3</v>
+      </c>
+      <c r="J24">
+        <v>9.950330853168092E-3</v>
+      </c>
+      <c r="K24">
+        <v>2.5278291490875252E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>348</v>
+      </c>
+      <c r="B25" t="s">
+        <v>349</v>
+      </c>
+      <c r="C25" t="s">
+        <v>350</v>
+      </c>
+      <c r="D25" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" t="s">
+        <v>351</v>
+      </c>
+      <c r="F25" t="s">
+        <v>157</v>
+      </c>
+      <c r="G25" t="s">
+        <v>352</v>
+      </c>
+      <c r="H25" t="s">
+        <v>160</v>
+      </c>
+      <c r="I25">
+        <v>3.1009539353891694E-3</v>
+      </c>
+      <c r="J25">
+        <v>-1.0050335853501451E-2</v>
+      </c>
+      <c r="K25">
+        <v>2.0625534854360972E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>348</v>
+      </c>
+      <c r="B26" t="s">
+        <v>349</v>
+      </c>
+      <c r="C26" t="s">
+        <v>350</v>
+      </c>
+      <c r="D26" t="s">
+        <v>3</v>
+      </c>
+      <c r="E26" t="s">
+        <v>351</v>
+      </c>
+      <c r="F26" t="s">
+        <v>163</v>
+      </c>
+      <c r="G26" t="s">
+        <v>352</v>
+      </c>
+      <c r="H26" t="s">
+        <v>160</v>
+      </c>
+      <c r="I26">
+        <v>3.1303571212109218E-3</v>
+      </c>
+      <c r="J26">
+        <v>9.950330853168092E-3</v>
+      </c>
+      <c r="K26">
+        <v>2.021667644238281E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>348</v>
+      </c>
+      <c r="B27" t="s">
+        <v>349</v>
+      </c>
+      <c r="C27" t="s">
+        <v>350</v>
+      </c>
+      <c r="D27" t="s">
+        <v>3</v>
+      </c>
+      <c r="E27" t="s">
+        <v>351</v>
+      </c>
+      <c r="F27" t="s">
+        <v>166</v>
+      </c>
+      <c r="G27" t="s">
+        <v>352</v>
+      </c>
+      <c r="H27" t="s">
+        <v>169</v>
+      </c>
+      <c r="I27">
+        <v>3.3858286475286349E-3</v>
+      </c>
+      <c r="J27">
+        <v>-2.0202707317519466E-2</v>
+      </c>
+      <c r="K27">
+        <v>1.8136714715237322E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>348</v>
+      </c>
+      <c r="B28" t="s">
+        <v>349</v>
+      </c>
+      <c r="C28" t="s">
+        <v>350</v>
+      </c>
+      <c r="D28" t="s">
+        <v>3</v>
+      </c>
+      <c r="E28" t="s">
+        <v>351</v>
+      </c>
+      <c r="F28" t="s">
+        <v>171</v>
+      </c>
+      <c r="G28" t="s">
+        <v>352</v>
+      </c>
+      <c r="H28" t="s">
+        <v>169</v>
+      </c>
+      <c r="I28">
+        <v>3.3858286475286349E-3</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <v>1.795428488821418E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>348</v>
+      </c>
+      <c r="B29" t="s">
+        <v>349</v>
+      </c>
+      <c r="C29" t="s">
+        <v>350</v>
+      </c>
+      <c r="D29" t="s">
+        <v>3</v>
+      </c>
+      <c r="E29" t="s">
+        <v>351</v>
+      </c>
+      <c r="F29" t="s">
+        <v>176</v>
+      </c>
+      <c r="G29" t="s">
+        <v>352</v>
+      </c>
+      <c r="H29" t="s">
+        <v>160</v>
+      </c>
+      <c r="I29">
+        <v>3.2840062847118239E-3</v>
+      </c>
+      <c r="J29">
+        <v>-1.0050335853501451E-2</v>
+      </c>
+      <c r="K29">
+        <v>2.0625534854360972E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>348</v>
+      </c>
+      <c r="B30" t="s">
+        <v>349</v>
+      </c>
+      <c r="C30" t="s">
+        <v>350</v>
+      </c>
+      <c r="D30" t="s">
+        <v>3</v>
+      </c>
+      <c r="E30" t="s">
+        <v>351</v>
+      </c>
+      <c r="F30" t="s">
+        <v>180</v>
+      </c>
+      <c r="G30" t="s">
+        <v>352</v>
+      </c>
+      <c r="H30" t="s">
+        <v>169</v>
+      </c>
+      <c r="I30">
+        <v>3.4401141223554918E-3</v>
+      </c>
+      <c r="J30">
+        <v>2.9558802241544429E-2</v>
+      </c>
+      <c r="K30">
+        <v>1.9823720491662328E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>348</v>
+      </c>
+      <c r="B31" t="s">
+        <v>349</v>
+      </c>
+      <c r="C31" t="s">
+        <v>350</v>
+      </c>
+      <c r="D31" t="s">
+        <v>3</v>
+      </c>
+      <c r="E31" t="s">
+        <v>351</v>
+      </c>
+      <c r="F31" t="s">
+        <v>185</v>
+      </c>
+      <c r="G31" t="s">
+        <v>352</v>
+      </c>
+      <c r="H31" t="s">
+        <v>188</v>
+      </c>
+      <c r="I31">
+        <v>3.1570426012529937E-3</v>
+      </c>
+      <c r="J31">
+        <v>-1.0050335853501451E-2</v>
+      </c>
+      <c r="K31">
+        <v>2.0625534854360972E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>348</v>
+      </c>
+      <c r="B32" t="s">
+        <v>349</v>
+      </c>
+      <c r="C32" t="s">
+        <v>350</v>
+      </c>
+      <c r="D32" t="s">
+        <v>3</v>
+      </c>
+      <c r="E32" t="s">
+        <v>351</v>
+      </c>
+      <c r="F32" t="s">
+        <v>190</v>
+      </c>
+      <c r="G32" t="s">
+        <v>352</v>
+      </c>
+      <c r="H32" t="s">
+        <v>152</v>
+      </c>
+      <c r="I32">
+        <v>3.8188506389133458E-3</v>
+      </c>
+      <c r="J32">
+        <v>9.950330853168092E-3</v>
+      </c>
+      <c r="K32">
+        <v>2.2634723369562348E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>348</v>
+      </c>
+      <c r="B33" t="s">
+        <v>349</v>
+      </c>
+      <c r="C33" t="s">
+        <v>350</v>
+      </c>
+      <c r="D33" t="s">
+        <v>3</v>
+      </c>
+      <c r="E33" t="s">
+        <v>351</v>
+      </c>
+      <c r="F33" t="s">
+        <v>193</v>
+      </c>
+      <c r="G33" t="s">
+        <v>352</v>
+      </c>
+      <c r="H33" t="s">
+        <v>188</v>
+      </c>
+      <c r="I33">
+        <v>3.2611000381207386E-3</v>
+      </c>
+      <c r="J33">
+        <v>9.950330853168092E-3</v>
+      </c>
+      <c r="K33">
+        <v>1.7775489958670895E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>348</v>
+      </c>
+      <c r="B34" t="s">
+        <v>349</v>
+      </c>
+      <c r="C34" t="s">
+        <v>350</v>
+      </c>
+      <c r="D34" t="s">
+        <v>3</v>
+      </c>
+      <c r="E34" t="s">
+        <v>351</v>
+      </c>
+      <c r="F34" t="s">
+        <v>196</v>
+      </c>
+      <c r="G34" t="s">
+        <v>352</v>
+      </c>
+      <c r="H34" t="s">
+        <v>160</v>
+      </c>
+      <c r="I34">
+        <v>3.4163905161264875E-3</v>
+      </c>
+      <c r="J34">
+        <v>1.980262729617973E-2</v>
+      </c>
+      <c r="K34">
+        <v>2.2413611171258761E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>348</v>
+      </c>
+      <c r="B35" t="s">
+        <v>349</v>
+      </c>
+      <c r="C35" t="s">
+        <v>350</v>
+      </c>
+      <c r="D35" t="s">
+        <v>3</v>
+      </c>
+      <c r="E35" t="s">
+        <v>351</v>
+      </c>
+      <c r="F35" t="s">
+        <v>199</v>
+      </c>
+      <c r="G35" t="s">
+        <v>352</v>
+      </c>
+      <c r="H35" t="s">
+        <v>201</v>
+      </c>
+      <c r="I35">
+        <v>3.1270864211269097E-3</v>
+      </c>
+      <c r="J35">
+        <v>-2.0202707317519466E-2</v>
+      </c>
+      <c r="K35">
+        <v>2.0836232401598792E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>348</v>
+      </c>
+      <c r="B36" t="s">
+        <v>349</v>
+      </c>
+      <c r="C36" t="s">
+        <v>350</v>
+      </c>
+      <c r="D36" t="s">
+        <v>3</v>
+      </c>
+      <c r="E36" t="s">
+        <v>351</v>
+      </c>
+      <c r="F36" t="s">
+        <v>203</v>
+      </c>
+      <c r="G36" t="s">
+        <v>352</v>
+      </c>
+      <c r="H36" t="s">
+        <v>160</v>
+      </c>
+      <c r="I36">
+        <v>3.4495150546990511E-3</v>
+      </c>
+      <c r="J36">
+        <v>9.950330853168092E-3</v>
+      </c>
+      <c r="K36">
+        <v>2.021667644238281E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>348</v>
+      </c>
+      <c r="B37" t="s">
+        <v>349</v>
+      </c>
+      <c r="C37" t="s">
+        <v>350</v>
+      </c>
+      <c r="D37" t="s">
+        <v>3</v>
+      </c>
+      <c r="E37" t="s">
+        <v>351</v>
+      </c>
+      <c r="F37" t="s">
+        <v>207</v>
+      </c>
+      <c r="G37" t="s">
+        <v>352</v>
+      </c>
+      <c r="H37" t="s">
+        <v>201</v>
+      </c>
+      <c r="I37">
+        <v>3.1359227769991375E-3</v>
+      </c>
+      <c r="J37">
+        <v>2.9558802241544429E-2</v>
+      </c>
+      <c r="K37">
+        <v>1.9823720491662328E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>348</v>
+      </c>
+      <c r="B38" t="s">
+        <v>349</v>
+      </c>
+      <c r="C38" t="s">
+        <v>350</v>
+      </c>
+      <c r="D38" t="s">
+        <v>3</v>
+      </c>
+      <c r="E38" t="s">
+        <v>351</v>
+      </c>
+      <c r="F38" t="s">
+        <v>211</v>
+      </c>
+      <c r="G38" t="s">
+        <v>352</v>
+      </c>
+      <c r="H38" t="s">
+        <v>188</v>
+      </c>
+      <c r="I38">
+        <v>3.2970040060210383E-3</v>
+      </c>
+      <c r="J38">
+        <v>9.950330853168092E-3</v>
+      </c>
+      <c r="K38">
+        <v>1.7600222318099878E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>348</v>
+      </c>
+      <c r="B39" t="s">
+        <v>349</v>
+      </c>
+      <c r="C39" t="s">
+        <v>350</v>
+      </c>
+      <c r="D39" t="s">
+        <v>3</v>
+      </c>
+      <c r="E39" t="s">
+        <v>351</v>
+      </c>
+      <c r="F39" t="s">
+        <v>215</v>
+      </c>
+      <c r="G39" t="s">
+        <v>352</v>
+      </c>
+      <c r="H39" t="s">
+        <v>147</v>
+      </c>
+      <c r="I39">
+        <v>4.731827345175914E-3</v>
+      </c>
+      <c r="J39">
+        <v>9.950330853168092E-3</v>
+      </c>
+      <c r="K39">
+        <v>2.2634723369562348E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>348</v>
+      </c>
+      <c r="B40" t="s">
+        <v>349</v>
+      </c>
+      <c r="C40" t="s">
+        <v>350</v>
+      </c>
+      <c r="D40" t="s">
+        <v>3</v>
+      </c>
+      <c r="E40" t="s">
+        <v>351</v>
+      </c>
+      <c r="F40" t="s">
+        <v>218</v>
+      </c>
+      <c r="G40" t="s">
+        <v>352</v>
+      </c>
+      <c r="H40" t="s">
+        <v>58</v>
+      </c>
+      <c r="I40">
+        <v>7.6547101529929129E-3</v>
+      </c>
+      <c r="J40">
+        <v>1.980262729617973E-2</v>
+      </c>
+      <c r="K40">
+        <v>3.5069130262398725E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>348</v>
+      </c>
+      <c r="B41" t="s">
+        <v>349</v>
+      </c>
+      <c r="C41" t="s">
+        <v>350</v>
+      </c>
+      <c r="D41" t="s">
+        <v>3</v>
+      </c>
+      <c r="E41" t="s">
+        <v>351</v>
+      </c>
+      <c r="F41" t="s">
+        <v>222</v>
+      </c>
+      <c r="G41" t="s">
+        <v>352</v>
+      </c>
+      <c r="H41" t="s">
+        <v>201</v>
+      </c>
+      <c r="I41">
+        <v>3.2347153051164972E-3</v>
+      </c>
+      <c r="J41">
+        <v>0</v>
+      </c>
+      <c r="K41">
+        <v>1.7775489958670895E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>348</v>
+      </c>
+      <c r="B42" t="s">
+        <v>349</v>
+      </c>
+      <c r="C42" t="s">
+        <v>350</v>
+      </c>
+      <c r="D42" t="s">
+        <v>3</v>
+      </c>
+      <c r="E42" t="s">
+        <v>351</v>
+      </c>
+      <c r="F42" t="s">
+        <v>226</v>
+      </c>
+      <c r="G42" t="s">
+        <v>352</v>
+      </c>
+      <c r="H42" t="s">
+        <v>169</v>
+      </c>
+      <c r="I42">
+        <v>3.7365871844980301E-3</v>
+      </c>
+      <c r="J42">
+        <v>2.9558802241544429E-2</v>
+      </c>
+      <c r="K42">
+        <v>1.9823720491662328E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>348</v>
+      </c>
+      <c r="B43" t="s">
+        <v>349</v>
+      </c>
+      <c r="C43" t="s">
+        <v>350</v>
+      </c>
+      <c r="D43" t="s">
+        <v>3</v>
+      </c>
+      <c r="E43" t="s">
+        <v>351</v>
+      </c>
+      <c r="F43" t="s">
+        <v>228</v>
+      </c>
+      <c r="G43" t="s">
+        <v>352</v>
+      </c>
+      <c r="H43" t="s">
+        <v>230</v>
+      </c>
+      <c r="I43">
+        <v>3.0908838625917667E-3</v>
+      </c>
+      <c r="J43">
+        <v>1.980262729617973E-2</v>
+      </c>
+      <c r="K43">
+        <v>1.7428378565682977E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>348</v>
+      </c>
+      <c r="B44" t="s">
+        <v>349</v>
+      </c>
+      <c r="C44" t="s">
+        <v>350</v>
+      </c>
+      <c r="D44" t="s">
+        <v>3</v>
+      </c>
+      <c r="E44" t="s">
+        <v>351</v>
+      </c>
+      <c r="F44" t="s">
+        <v>232</v>
+      </c>
+      <c r="G44" t="s">
+        <v>352</v>
+      </c>
+      <c r="H44" t="s">
+        <v>230</v>
+      </c>
+      <c r="I44">
+        <v>3.0928807413129855E-3</v>
+      </c>
+      <c r="J44">
+        <v>1.980262729617973E-2</v>
+      </c>
+      <c r="K44">
+        <v>1.7600222318099878E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>348</v>
+      </c>
+      <c r="B45" t="s">
+        <v>349</v>
+      </c>
+      <c r="C45" t="s">
+        <v>350</v>
+      </c>
+      <c r="D45" t="s">
+        <v>3</v>
+      </c>
+      <c r="E45" t="s">
+        <v>351</v>
+      </c>
+      <c r="F45" t="s">
+        <v>235</v>
+      </c>
+      <c r="G45" t="s">
+        <v>352</v>
+      </c>
+      <c r="H45" t="s">
+        <v>188</v>
+      </c>
+      <c r="I45">
+        <v>3.4610202407590472E-3</v>
+      </c>
+      <c r="J45">
+        <v>1.980262729617973E-2</v>
+      </c>
+      <c r="K45">
+        <v>1.7428378565682977E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>348</v>
+      </c>
+      <c r="B46" t="s">
+        <v>349</v>
+      </c>
+      <c r="C46" t="s">
+        <v>350</v>
+      </c>
+      <c r="D46" t="s">
+        <v>3</v>
+      </c>
+      <c r="E46" t="s">
+        <v>351</v>
+      </c>
+      <c r="F46" t="s">
+        <v>237</v>
+      </c>
+      <c r="G46" t="s">
+        <v>352</v>
+      </c>
+      <c r="H46" t="s">
+        <v>188</v>
+      </c>
+      <c r="I46">
+        <v>3.4963252656081026E-3</v>
+      </c>
+      <c r="J46">
+        <v>9.950330853168092E-3</v>
+      </c>
+      <c r="K46">
+        <v>1.7600222318099878E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>348</v>
+      </c>
+      <c r="B47" t="s">
+        <v>349</v>
+      </c>
+      <c r="C47" t="s">
+        <v>350</v>
+      </c>
+      <c r="D47" t="s">
+        <v>3</v>
+      </c>
+      <c r="E47" t="s">
+        <v>351</v>
+      </c>
+      <c r="F47" t="s">
+        <v>240</v>
+      </c>
+      <c r="G47" t="s">
+        <v>352</v>
+      </c>
+      <c r="H47" t="s">
+        <v>230</v>
+      </c>
+      <c r="I47">
+        <v>3.187050371155891E-3</v>
+      </c>
+      <c r="J47">
+        <v>2.9558802241544429E-2</v>
+      </c>
+      <c r="K47">
+        <v>1.9823720491662328E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>348</v>
+      </c>
+      <c r="B48" t="s">
+        <v>349</v>
+      </c>
+      <c r="C48" t="s">
+        <v>350</v>
+      </c>
+      <c r="D48" t="s">
+        <v>3</v>
+      </c>
+      <c r="E48" t="s">
+        <v>351</v>
+      </c>
+      <c r="F48" t="s">
+        <v>243</v>
+      </c>
+      <c r="G48" t="s">
+        <v>352</v>
+      </c>
+      <c r="H48" t="s">
+        <v>245</v>
+      </c>
+      <c r="I48">
+        <v>3.0193108779371599E-3</v>
+      </c>
+      <c r="J48">
+        <v>9.950330853168092E-3</v>
+      </c>
+      <c r="K48">
+        <v>2.021667644238281E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>348</v>
+      </c>
+      <c r="B49" t="s">
+        <v>349</v>
+      </c>
+      <c r="C49" t="s">
+        <v>350</v>
+      </c>
+      <c r="D49" t="s">
+        <v>3</v>
+      </c>
+      <c r="E49" t="s">
+        <v>351</v>
+      </c>
+      <c r="F49" t="s">
+        <v>246</v>
+      </c>
+      <c r="G49" t="s">
+        <v>352</v>
+      </c>
+      <c r="H49" t="s">
+        <v>245</v>
+      </c>
+      <c r="I49">
+        <v>3.071047346779402E-3</v>
+      </c>
+      <c r="J49">
+        <v>0</v>
+      </c>
+      <c r="K49">
+        <v>2.0419058079983801E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>348</v>
+      </c>
+      <c r="B50" t="s">
+        <v>349</v>
+      </c>
+      <c r="C50" t="s">
+        <v>350</v>
+      </c>
+      <c r="D50" t="s">
+        <v>3</v>
+      </c>
+      <c r="E50" t="s">
+        <v>351</v>
+      </c>
+      <c r="F50" t="s">
+        <v>248</v>
+      </c>
+      <c r="G50" t="s">
+        <v>352</v>
+      </c>
+      <c r="H50" t="s">
+        <v>139</v>
+      </c>
+      <c r="I50">
+        <v>4.8409172195352148E-3</v>
+      </c>
+      <c r="J50">
+        <v>9.950330853168092E-3</v>
+      </c>
+      <c r="K50">
+        <v>3.0344883383001391E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>348</v>
+      </c>
+      <c r="B51" t="s">
+        <v>349</v>
+      </c>
+      <c r="C51" t="s">
+        <v>350</v>
+      </c>
+      <c r="D51" t="s">
+        <v>3</v>
+      </c>
+      <c r="E51" t="s">
+        <v>351</v>
+      </c>
+      <c r="F51" t="s">
+        <v>252</v>
+      </c>
+      <c r="G51" t="s">
+        <v>352</v>
+      </c>
+      <c r="H51" t="s">
+        <v>245</v>
+      </c>
+      <c r="I51">
+        <v>3.1132498103861412E-3</v>
+      </c>
+      <c r="J51">
+        <v>-3.0459207484708574E-2</v>
+      </c>
+      <c r="K51">
+        <v>1.5784541764818246E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>348</v>
+      </c>
+      <c r="B52" t="s">
+        <v>349</v>
+      </c>
+      <c r="C52" t="s">
+        <v>350</v>
+      </c>
+      <c r="D52" t="s">
+        <v>3</v>
+      </c>
+      <c r="E52" t="s">
+        <v>351</v>
+      </c>
+      <c r="F52" t="s">
+        <v>255</v>
+      </c>
+      <c r="G52" t="s">
+        <v>352</v>
+      </c>
+      <c r="H52" t="s">
+        <v>91</v>
+      </c>
+      <c r="I52">
+        <v>5.3679176144036979E-3</v>
+      </c>
+      <c r="J52">
+        <v>3.9220713153281329E-2</v>
+      </c>
+      <c r="K52">
+        <v>2.1984106183941941E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>348</v>
+      </c>
+      <c r="B53" t="s">
+        <v>349</v>
+      </c>
+      <c r="C53" t="s">
+        <v>350</v>
+      </c>
+      <c r="D53" t="s">
+        <v>3</v>
+      </c>
+      <c r="E53" t="s">
+        <v>351</v>
+      </c>
+      <c r="F53" t="s">
+        <v>259</v>
+      </c>
+      <c r="G53" t="s">
+        <v>352</v>
+      </c>
+      <c r="H53" t="s">
+        <v>91</v>
+      </c>
+      <c r="I53">
+        <v>5.3834551170713757E-3</v>
+      </c>
+      <c r="J53">
+        <v>-2.0202707317519466E-2</v>
+      </c>
+      <c r="K53">
+        <v>2.851821581329508E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>348</v>
+      </c>
+      <c r="B54" t="s">
+        <v>349</v>
+      </c>
+      <c r="C54" t="s">
+        <v>350</v>
+      </c>
+      <c r="D54" t="s">
+        <v>3</v>
+      </c>
+      <c r="E54" t="s">
+        <v>351</v>
+      </c>
+      <c r="F54" t="s">
+        <v>262</v>
+      </c>
+      <c r="G54" t="s">
+        <v>352</v>
+      </c>
+      <c r="H54" t="s">
+        <v>245</v>
+      </c>
+      <c r="I54">
+        <v>3.157964334726288E-3</v>
+      </c>
+      <c r="J54">
+        <v>0</v>
+      </c>
+      <c r="K54">
+        <v>1.7775489958670895E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>348</v>
+      </c>
+      <c r="B55" t="s">
+        <v>349</v>
+      </c>
+      <c r="C55" t="s">
+        <v>350</v>
+      </c>
+      <c r="D55" t="s">
+        <v>3</v>
+      </c>
+      <c r="E55" t="s">
+        <v>351</v>
+      </c>
+      <c r="F55" t="s">
+        <v>265</v>
+      </c>
+      <c r="G55" t="s">
+        <v>352</v>
+      </c>
+      <c r="H55" t="s">
+        <v>122</v>
+      </c>
+      <c r="I55">
+        <v>4.5724640231131859E-3</v>
+      </c>
+      <c r="J55">
+        <v>2.9558802241544429E-2</v>
+      </c>
+      <c r="K55">
+        <v>2.4786670523889762E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>348</v>
+      </c>
+      <c r="B56" t="s">
+        <v>349</v>
+      </c>
+      <c r="C56" t="s">
+        <v>350</v>
+      </c>
+      <c r="D56" t="s">
+        <v>3</v>
+      </c>
+      <c r="E56" t="s">
+        <v>351</v>
+      </c>
+      <c r="F56" t="s">
+        <v>268</v>
+      </c>
+      <c r="G56" t="s">
+        <v>352</v>
+      </c>
+      <c r="H56" t="s">
+        <v>230</v>
+      </c>
+      <c r="I56">
+        <v>3.3414160168904051E-3</v>
+      </c>
+      <c r="J56">
+        <v>9.950330853168092E-3</v>
+      </c>
+      <c r="K56">
+        <v>2.021667644238281E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>348</v>
+      </c>
+      <c r="B57" t="s">
+        <v>349</v>
+      </c>
+      <c r="C57" t="s">
+        <v>350</v>
+      </c>
+      <c r="D57" t="s">
+        <v>3</v>
+      </c>
+      <c r="E57" t="s">
+        <v>351</v>
+      </c>
+      <c r="F57" t="s">
+        <v>270</v>
+      </c>
+      <c r="G57" t="s">
+        <v>352</v>
+      </c>
+      <c r="H57" t="s">
+        <v>245</v>
+      </c>
+      <c r="I57">
+        <v>3.1792521978924546E-3</v>
+      </c>
+      <c r="J57">
+        <v>9.950330853168092E-3</v>
+      </c>
+      <c r="K57">
+        <v>1.7600222318099878E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>348</v>
+      </c>
+      <c r="B58" t="s">
+        <v>349</v>
+      </c>
+      <c r="C58" t="s">
+        <v>350</v>
+      </c>
+      <c r="D58" t="s">
+        <v>3</v>
+      </c>
+      <c r="E58" t="s">
+        <v>351</v>
+      </c>
+      <c r="F58" t="s">
+        <v>273</v>
+      </c>
+      <c r="G58" t="s">
+        <v>352</v>
+      </c>
+      <c r="H58" t="s">
+        <v>230</v>
+      </c>
+      <c r="I58">
+        <v>3.3624599660399333E-3</v>
+      </c>
+      <c r="J58">
+        <v>-3.0459207484708574E-2</v>
+      </c>
+      <c r="K58">
+        <v>2.1051281553062108E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>348</v>
+      </c>
+      <c r="B59" t="s">
+        <v>349</v>
+      </c>
+      <c r="C59" t="s">
+        <v>350</v>
+      </c>
+      <c r="D59" t="s">
+        <v>3</v>
+      </c>
+      <c r="E59" t="s">
+        <v>351</v>
+      </c>
+      <c r="F59" t="s">
+        <v>276</v>
+      </c>
+      <c r="G59" t="s">
+        <v>352</v>
+      </c>
+      <c r="H59" t="s">
+        <v>278</v>
+      </c>
+      <c r="I59">
+        <v>3.0193538814245456E-3</v>
+      </c>
+      <c r="J59">
+        <v>0</v>
+      </c>
+      <c r="K59">
+        <v>1.7775489958670895E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>348</v>
+      </c>
+      <c r="B60" t="s">
+        <v>349</v>
+      </c>
+      <c r="C60" t="s">
+        <v>350</v>
+      </c>
+      <c r="D60" t="s">
+        <v>3</v>
+      </c>
+      <c r="E60" t="s">
+        <v>351</v>
+      </c>
+      <c r="F60" t="s">
+        <v>279</v>
+      </c>
+      <c r="G60" t="s">
+        <v>352</v>
+      </c>
+      <c r="H60" t="s">
+        <v>278</v>
+      </c>
+      <c r="I60">
+        <v>3.0243671843956333E-3</v>
+      </c>
+      <c r="J60">
+        <v>1.980262729617973E-2</v>
+      </c>
+      <c r="K60">
+        <v>1.7428378565682977E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>348</v>
+      </c>
+      <c r="B61" t="s">
+        <v>349</v>
+      </c>
+      <c r="C61" t="s">
+        <v>350</v>
+      </c>
+      <c r="D61" t="s">
+        <v>3</v>
+      </c>
+      <c r="E61" t="s">
+        <v>351</v>
+      </c>
+      <c r="F61" t="s">
+        <v>282</v>
+      </c>
+      <c r="G61" t="s">
+        <v>352</v>
+      </c>
+      <c r="H61" t="s">
+        <v>91</v>
+      </c>
+      <c r="I61">
+        <v>5.5237368363655111E-3</v>
+      </c>
+      <c r="J61">
+        <v>4.8790164169432049E-2</v>
+      </c>
+      <c r="K61">
+        <v>2.9186314075955181E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>348</v>
+      </c>
+      <c r="B62" t="s">
+        <v>349</v>
+      </c>
+      <c r="C62" t="s">
+        <v>350</v>
+      </c>
+      <c r="D62" t="s">
+        <v>3</v>
+      </c>
+      <c r="E62" t="s">
+        <v>351</v>
+      </c>
+      <c r="F62" t="s">
+        <v>287</v>
+      </c>
+      <c r="G62" t="s">
+        <v>352</v>
+      </c>
+      <c r="H62" t="s">
+        <v>152</v>
+      </c>
+      <c r="I62">
+        <v>4.4739424041467394E-3</v>
+      </c>
+      <c r="J62">
+        <v>1.980262729617973E-2</v>
+      </c>
+      <c r="K62">
+        <v>3.0046692769485604E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>348</v>
+      </c>
+      <c r="B63" t="s">
+        <v>349</v>
+      </c>
+      <c r="C63" t="s">
+        <v>350</v>
+      </c>
+      <c r="D63" t="s">
+        <v>3</v>
+      </c>
+      <c r="E63" t="s">
+        <v>351</v>
+      </c>
+      <c r="F63" t="s">
+        <v>291</v>
+      </c>
+      <c r="G63" t="s">
+        <v>352</v>
+      </c>
+      <c r="H63" t="s">
+        <v>245</v>
+      </c>
+      <c r="I63">
+        <v>3.2255089532494787E-3</v>
+      </c>
+      <c r="J63">
+        <v>0</v>
+      </c>
+      <c r="K63">
+        <v>1.7775489958670895E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>348</v>
+      </c>
+      <c r="B64" t="s">
+        <v>349</v>
+      </c>
+      <c r="C64" t="s">
+        <v>350</v>
+      </c>
+      <c r="D64" t="s">
+        <v>3</v>
+      </c>
+      <c r="E64" t="s">
+        <v>351</v>
+      </c>
+      <c r="F64" t="s">
+        <v>293</v>
+      </c>
+      <c r="G64" t="s">
+        <v>352</v>
+      </c>
+      <c r="H64" t="s">
+        <v>230</v>
+      </c>
+      <c r="I64">
+        <v>3.413229426799249E-3</v>
+      </c>
+      <c r="J64">
+        <v>0</v>
+      </c>
+      <c r="K64">
+        <v>1.795428488821418E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>348</v>
+      </c>
+      <c r="B65" t="s">
+        <v>349</v>
+      </c>
+      <c r="C65" t="s">
+        <v>350</v>
+      </c>
+      <c r="D65" t="s">
+        <v>3</v>
+      </c>
+      <c r="E65" t="s">
+        <v>351</v>
+      </c>
+      <c r="F65" t="s">
+        <v>296</v>
+      </c>
+      <c r="G65" t="s">
+        <v>352</v>
+      </c>
+      <c r="H65" t="s">
+        <v>278</v>
+      </c>
+      <c r="I65">
+        <v>3.0575583491919659E-3</v>
+      </c>
+      <c r="J65">
+        <v>1.980262729617973E-2</v>
+      </c>
+      <c r="K65">
+        <v>1.7600222318099878E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>348</v>
+      </c>
+      <c r="B66" t="s">
+        <v>349</v>
+      </c>
+      <c r="C66" t="s">
+        <v>350</v>
+      </c>
+      <c r="D66" t="s">
+        <v>3</v>
+      </c>
+      <c r="E66" t="s">
+        <v>351</v>
+      </c>
+      <c r="F66" t="s">
+        <v>300</v>
+      </c>
+      <c r="G66" t="s">
+        <v>352</v>
+      </c>
+      <c r="H66" t="s">
+        <v>201</v>
+      </c>
+      <c r="I66">
+        <v>3.609083481225025E-3</v>
+      </c>
+      <c r="J66">
+        <v>2.9558802241544429E-2</v>
+      </c>
+      <c r="K66">
+        <v>1.9823720491662328E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>348</v>
+      </c>
+      <c r="B67" t="s">
+        <v>349</v>
+      </c>
+      <c r="C67" t="s">
+        <v>350</v>
+      </c>
+      <c r="D67" t="s">
+        <v>3</v>
+      </c>
+      <c r="E67" t="s">
+        <v>351</v>
+      </c>
+      <c r="F67" t="s">
+        <v>303</v>
+      </c>
+      <c r="G67" t="s">
+        <v>352</v>
+      </c>
+      <c r="H67" t="s">
+        <v>51</v>
+      </c>
+      <c r="I67">
+        <v>7.21816696245005E-3</v>
+      </c>
+      <c r="J67">
+        <v>5.8268908123975824E-2</v>
+      </c>
+      <c r="K67">
+        <v>4.0807308595070944E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>348</v>
+      </c>
+      <c r="B68" t="s">
+        <v>349</v>
+      </c>
+      <c r="C68" t="s">
+        <v>350</v>
+      </c>
+      <c r="D68" t="s">
+        <v>3</v>
+      </c>
+      <c r="E68" t="s">
+        <v>351</v>
+      </c>
+      <c r="F68" t="s">
+        <v>308</v>
+      </c>
+      <c r="G68" t="s">
+        <v>352</v>
+      </c>
+      <c r="H68" t="s">
+        <v>230</v>
+      </c>
+      <c r="I68">
+        <v>3.4422677991651496E-3</v>
+      </c>
+      <c r="J68">
+        <v>1.980262729617973E-2</v>
+      </c>
+      <c r="K68">
+        <v>2.0018269245279413E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>348</v>
+      </c>
+      <c r="B69" t="s">
+        <v>349</v>
+      </c>
+      <c r="C69" t="s">
+        <v>350</v>
+      </c>
+      <c r="D69" t="s">
+        <v>3</v>
+      </c>
+      <c r="E69" t="s">
+        <v>351</v>
+      </c>
+      <c r="F69" t="s">
+        <v>312</v>
+      </c>
+      <c r="G69" t="s">
+        <v>352</v>
+      </c>
+      <c r="H69" t="s">
+        <v>160</v>
+      </c>
+      <c r="I69">
+        <v>4.0033087284456915E-3</v>
+      </c>
+      <c r="J69">
+        <v>-1.0050335853501451E-2</v>
+      </c>
+      <c r="K69">
+        <v>2.3090308046130589E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>348</v>
+      </c>
+      <c r="B70" t="s">
+        <v>349</v>
+      </c>
+      <c r="C70" t="s">
+        <v>350</v>
+      </c>
+      <c r="D70" t="s">
+        <v>3</v>
+      </c>
+      <c r="E70" t="s">
+        <v>351</v>
+      </c>
+      <c r="F70" t="s">
+        <v>316</v>
+      </c>
+      <c r="G70" t="s">
+        <v>352</v>
+      </c>
+      <c r="H70" t="s">
+        <v>278</v>
+      </c>
+      <c r="I70">
+        <v>3.1008536966410077E-3</v>
+      </c>
+      <c r="J70">
+        <v>0</v>
+      </c>
+      <c r="K70">
+        <v>2.0419058079983801E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>348</v>
+      </c>
+      <c r="B71" t="s">
+        <v>349</v>
+      </c>
+      <c r="C71" t="s">
+        <v>350</v>
+      </c>
+      <c r="D71" t="s">
+        <v>3</v>
+      </c>
+      <c r="E71" t="s">
+        <v>351</v>
+      </c>
+      <c r="F71" t="s">
+        <v>319</v>
+      </c>
+      <c r="G71" t="s">
+        <v>352</v>
+      </c>
+      <c r="H71" t="s">
+        <v>230</v>
+      </c>
+      <c r="I71">
+        <v>3.4830228110857933E-3</v>
+      </c>
+      <c r="J71">
+        <v>0</v>
+      </c>
+      <c r="K71">
+        <v>2.0419058079983801E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Re-analysis tibble fixed, results written up to last paragraph
</commit_message>
<xml_diff>
--- a/MSc_Thesis/MSc_Thesis_Split/Data/Citations_Datasets/mokry_obesity_2016.xlsx
+++ b/MSc_Thesis/MSc_Thesis_Split/Data/Citations_Datasets/mokry_obesity_2016.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4f99f7067dc2a9a5/Documents/R/Working Directory/Data_Science_MSc/Dissertation_Bayes_MR/MSc_Thesis/MSc_Thesis_Split/Data/Citations_Datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="8_{22C4E43D-6371-4515-9FCB-E71DF9F4DBB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A93F10F-09D3-4F31-BA50-4CB9BFD7CF3F}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{22C4E43D-6371-4515-9FCB-E71DF9F4DBB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4F584BA-4AD1-4B06-BBDC-BB0F4958DBBE}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="12980" windowHeight="15370" activeTab="1" xr2:uid="{8A3BB852-7168-48D5-AFAC-CE153936FD9B}"/>
+    <workbookView xWindow="12710" yWindow="0" windowWidth="12980" windowHeight="15370" xr2:uid="{8A3BB852-7168-48D5-AFAC-CE153936FD9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Table004 (Page 7-8)" sheetId="2" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1309" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="335">
   <si>
     <t>BMI-Associated</t>
   </si>
@@ -1056,67 +1056,13 @@
   </si>
   <si>
     <t>Upp_CI</t>
-  </si>
-  <si>
-    <t>SE_Lower_Only</t>
-  </si>
-  <si>
-    <t>SE_Both</t>
-  </si>
-  <si>
-    <t>Author</t>
-  </si>
-  <si>
-    <t>Study_Ref</t>
-  </si>
-  <si>
-    <t>Study_DOI</t>
-  </si>
-  <si>
-    <t>Exposure</t>
-  </si>
-  <si>
-    <t>Outcome</t>
-  </si>
-  <si>
-    <t>Instrument</t>
-  </si>
-  <si>
-    <t>Reported_Measure</t>
-  </si>
-  <si>
-    <t>Coeff_G_X</t>
-  </si>
-  <si>
-    <t>Coeff_G_X_SE</t>
-  </si>
-  <si>
-    <t>Coeff_G_Y</t>
-  </si>
-  <si>
-    <t>Coeff_G_Y_SE</t>
-  </si>
-  <si>
-    <t>Mokry et al</t>
-  </si>
-  <si>
-    <t>[@mokry_obesity_2016]</t>
-  </si>
-  <si>
-    <t>10.1371/journal.pmed.1002053</t>
-  </si>
-  <si>
-    <t>Multiple Sclerosis</t>
-  </si>
-  <si>
-    <t>OR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1128,12 +1074,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1214,10 +1154,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1585,10 +1521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17ADCFF7-C1EB-4801-B550-02DC019036B8}">
-  <dimension ref="A1:AD72"/>
+  <dimension ref="A1:AB72"/>
   <sheetViews>
-    <sheetView topLeftCell="T2" workbookViewId="0">
-      <selection activeCell="AC72" sqref="AC3:AC72"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AB3" sqref="AB3:AB72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1609,7 +1545,7 @@
     <col min="15" max="15" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1668,7 +1604,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -1721,13 +1657,10 @@
         <v>334</v>
       </c>
       <c r="AB2" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="AC2" s="1" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -1810,16 +1743,8 @@
         <f>(Y3-Z3)/1.96</f>
         <v>1.5540411981994171E-2</v>
       </c>
-      <c r="AC3">
-        <f>(AA3-Z3)/2/1.96</f>
-        <v>1.7775489958670895E-2</v>
-      </c>
-      <c r="AD3">
-        <f>(AA3-Y3)/1.96</f>
-        <v>2.0010567935347619E-2</v>
-      </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -1902,16 +1827,8 @@
         <f t="shared" ref="AB4:AB67" si="3">(Y4-Z4)/1.96</f>
         <v>2.0827548224619984E-2</v>
       </c>
-      <c r="AC4">
-        <f t="shared" ref="AC4:AC67" si="4">(AA4-Z4)/2/1.96</f>
-        <v>2.0419058079983801E-2</v>
-      </c>
-      <c r="AD4">
-        <f t="shared" ref="AD4:AD67" si="5">(AA4-Y4)/1.96</f>
-        <v>2.0010567935347619E-2</v>
-      </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -1994,16 +1911,8 @@
         <f t="shared" si="3"/>
         <v>1.9816241487889776E-2</v>
       </c>
-      <c r="AC5">
-        <f t="shared" si="4"/>
-        <v>2.1775471671213478E-2</v>
-      </c>
-      <c r="AD5">
-        <f t="shared" si="5"/>
-        <v>2.3734701854537188E-2</v>
-      </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>48</v>
       </c>
@@ -2086,16 +1995,8 @@
         <f t="shared" si="3"/>
         <v>1.5231103647796521E-2</v>
       </c>
-      <c r="AC6">
-        <f t="shared" si="4"/>
-        <v>1.5010331638503445E-2</v>
-      </c>
-      <c r="AD6">
-        <f t="shared" si="5"/>
-        <v>1.4789559629210367E-2</v>
-      </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>55</v>
       </c>
@@ -2178,16 +2079,8 @@
         <f t="shared" si="3"/>
         <v>2.0827548224619984E-2</v>
       </c>
-      <c r="AC7">
-        <f t="shared" si="4"/>
-        <v>2.286024456369572E-2</v>
-      </c>
-      <c r="AD7">
-        <f t="shared" si="5"/>
-        <v>2.4892940902771454E-2</v>
-      </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>62</v>
       </c>
@@ -2270,16 +2163,8 @@
         <f t="shared" si="3"/>
         <v>2.5138290309583051E-2</v>
       </c>
-      <c r="AC8">
-        <f t="shared" si="4"/>
-        <v>2.219677984429333E-2</v>
-      </c>
-      <c r="AD8">
-        <f t="shared" si="5"/>
-        <v>1.9255269379003605E-2</v>
-      </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>69</v>
       </c>
@@ -2362,16 +2247,8 @@
         <f t="shared" si="3"/>
         <v>2.0208743926043816E-2</v>
       </c>
-      <c r="AC9">
-        <f t="shared" si="4"/>
-        <v>2.219677984429333E-2</v>
-      </c>
-      <c r="AD9">
-        <f t="shared" si="5"/>
-        <v>2.418481576254284E-2</v>
-      </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>74</v>
       </c>
@@ -2454,16 +2331,8 @@
         <f t="shared" si="3"/>
         <v>1.5699825850384548E-2</v>
       </c>
-      <c r="AC10">
-        <f t="shared" si="4"/>
-        <v>1.795428488821418E-2</v>
-      </c>
-      <c r="AD10">
-        <f t="shared" si="5"/>
-        <v>2.0208743926043816E-2</v>
-      </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>81</v>
       </c>
@@ -2546,16 +2415,8 @@
         <f t="shared" si="3"/>
         <v>2.0410885006989385E-2</v>
       </c>
-      <c r="AC11">
-        <f t="shared" si="4"/>
-        <v>2.0018269245279413E-2</v>
-      </c>
-      <c r="AD11">
-        <f t="shared" si="5"/>
-        <v>1.9625653483569438E-2</v>
-      </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>88</v>
       </c>
@@ -2638,16 +2499,8 @@
         <f t="shared" si="3"/>
         <v>1.9625653483569438E-2</v>
       </c>
-      <c r="AC12">
-        <f t="shared" si="4"/>
-        <v>1.6932415547161402E-2</v>
-      </c>
-      <c r="AD12">
-        <f t="shared" si="5"/>
-        <v>1.4239177610753362E-2</v>
-      </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>95</v>
       </c>
@@ -2730,16 +2583,8 @@
         <f t="shared" si="3"/>
         <v>2.0617111396875849E-2</v>
       </c>
-      <c r="AC13">
-        <f t="shared" si="4"/>
-        <v>1.7775489958670895E-2</v>
-      </c>
-      <c r="AD13">
-        <f t="shared" si="5"/>
-        <v>1.4933868520465937E-2</v>
-      </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>99</v>
       </c>
@@ -2822,16 +2667,8 @@
         <f t="shared" si="3"/>
         <v>2.5643793255555259E-2</v>
       </c>
-      <c r="AC14">
-        <f t="shared" si="4"/>
-        <v>2.7403124648172694E-2</v>
-      </c>
-      <c r="AD14">
-        <f t="shared" si="5"/>
-        <v>2.9162456040790135E-2</v>
-      </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>103</v>
       </c>
@@ -2914,16 +2751,8 @@
         <f t="shared" si="3"/>
         <v>2.9729034757130523E-2</v>
       </c>
-      <c r="AC15">
-        <f t="shared" si="4"/>
-        <v>2.8910378904847774E-2</v>
-      </c>
-      <c r="AD15">
-        <f t="shared" si="5"/>
-        <v>2.8091723052565024E-2</v>
-      </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>108</v>
       </c>
@@ -3006,16 +2835,8 @@
         <f t="shared" si="3"/>
         <v>2.4892940902771454E-2</v>
       </c>
-      <c r="AC16">
-        <f t="shared" si="4"/>
-        <v>2.1984106183941941E-2</v>
-      </c>
-      <c r="AD16">
-        <f t="shared" si="5"/>
-        <v>1.9075271465112429E-2</v>
-      </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>113</v>
       </c>
@@ -3098,16 +2919,8 @@
         <f t="shared" si="3"/>
         <v>2.1042325782678128E-2</v>
       </c>
-      <c r="AC17">
-        <f t="shared" si="4"/>
-        <v>2.0625534854360972E-2</v>
-      </c>
-      <c r="AD17">
-        <f t="shared" si="5"/>
-        <v>2.0208743926043816E-2</v>
-      </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>120</v>
       </c>
@@ -3190,16 +3003,8 @@
         <f t="shared" si="3"/>
         <v>1.6028671547642325E-2</v>
       </c>
-      <c r="AC18">
-        <f t="shared" si="4"/>
-        <v>1.832289147225909E-2</v>
-      </c>
-      <c r="AD18">
-        <f t="shared" si="5"/>
-        <v>2.0617111396875849E-2</v>
-      </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>126</v>
       </c>
@@ -3282,16 +3087,8 @@
         <f t="shared" si="3"/>
         <v>2.0410885006989385E-2</v>
       </c>
-      <c r="AC19">
-        <f t="shared" si="4"/>
-        <v>1.7600222318099878E-2</v>
-      </c>
-      <c r="AD19">
-        <f t="shared" si="5"/>
-        <v>1.4789559629210367E-2</v>
-      </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>130</v>
       </c>
@@ -3374,16 +3171,8 @@
         <f t="shared" si="3"/>
         <v>1.5699825850384548E-2</v>
       </c>
-      <c r="AC20">
-        <f t="shared" si="4"/>
-        <v>1.795428488821418E-2</v>
-      </c>
-      <c r="AD20">
-        <f t="shared" si="5"/>
-        <v>2.0208743926043816E-2</v>
-      </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>136</v>
       </c>
@@ -3466,16 +3255,8 @@
         <f t="shared" si="3"/>
         <v>1.6028671547642325E-2</v>
       </c>
-      <c r="AC21">
-        <f t="shared" si="4"/>
-        <v>1.832289147225909E-2</v>
-      </c>
-      <c r="AD21">
-        <f t="shared" si="5"/>
-        <v>2.0617111396875849E-2</v>
-      </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>141</v>
       </c>
@@ -3558,16 +3339,8 @@
         <f t="shared" si="3"/>
         <v>1.5231103647796521E-2</v>
       </c>
-      <c r="AC22">
-        <f t="shared" si="4"/>
-        <v>1.7428378565682977E-2</v>
-      </c>
-      <c r="AD22">
-        <f t="shared" si="5"/>
-        <v>1.9625653483569438E-2</v>
-      </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>144</v>
       </c>
@@ -3650,16 +3423,8 @@
         <f t="shared" si="3"/>
         <v>2.1042325782678128E-2</v>
       </c>
-      <c r="AC23">
-        <f t="shared" si="4"/>
-        <v>2.3090308046130589E-2</v>
-      </c>
-      <c r="AD23">
-        <f t="shared" si="5"/>
-        <v>2.5138290309583051E-2</v>
-      </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>149</v>
       </c>
@@ -3742,16 +3507,8 @@
         <f t="shared" si="3"/>
         <v>2.0617111396875849E-2</v>
       </c>
-      <c r="AC24">
-        <f t="shared" si="4"/>
-        <v>2.021667644238281E-2</v>
-      </c>
-      <c r="AD24">
-        <f t="shared" si="5"/>
-        <v>1.9816241487889776E-2</v>
-      </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>154</v>
       </c>
@@ -3834,16 +3591,8 @@
         <f t="shared" si="3"/>
         <v>2.5904247639501662E-2</v>
       </c>
-      <c r="AC25">
-        <f t="shared" si="4"/>
-        <v>2.5278291490875252E-2</v>
-      </c>
-      <c r="AD25">
-        <f t="shared" si="5"/>
-        <v>2.4652335342248845E-2</v>
-      </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>157</v>
       </c>
@@ -3926,16 +3675,8 @@
         <f t="shared" si="3"/>
         <v>2.1042325782678128E-2</v>
       </c>
-      <c r="AC26">
-        <f t="shared" si="4"/>
-        <v>2.0625534854360972E-2</v>
-      </c>
-      <c r="AD26">
-        <f t="shared" si="5"/>
-        <v>2.0208743926043816E-2</v>
-      </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>163</v>
       </c>
@@ -4018,16 +3759,8 @@
         <f t="shared" si="3"/>
         <v>2.0617111396875849E-2</v>
       </c>
-      <c r="AC27">
-        <f t="shared" si="4"/>
-        <v>2.021667644238281E-2</v>
-      </c>
-      <c r="AD27">
-        <f t="shared" si="5"/>
-        <v>1.9816241487889776E-2</v>
-      </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>166</v>
       </c>
@@ -4110,16 +3843,8 @@
         <f t="shared" si="3"/>
         <v>1.586254442348526E-2</v>
       </c>
-      <c r="AC28">
-        <f t="shared" si="4"/>
-        <v>1.8136714715237322E-2</v>
-      </c>
-      <c r="AD28">
-        <f t="shared" si="5"/>
-        <v>2.0410885006989385E-2</v>
-      </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>171</v>
       </c>
@@ -4202,16 +3927,8 @@
         <f t="shared" si="3"/>
         <v>2.0827548224619984E-2</v>
       </c>
-      <c r="AC29">
-        <f t="shared" si="4"/>
-        <v>1.795428488821418E-2</v>
-      </c>
-      <c r="AD29">
-        <f t="shared" si="5"/>
-        <v>1.5081021551808382E-2</v>
-      </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>176</v>
       </c>
@@ -4294,16 +4011,8 @@
         <f t="shared" si="3"/>
         <v>2.1042325782678128E-2</v>
       </c>
-      <c r="AC30">
-        <f t="shared" si="4"/>
-        <v>2.0625534854360972E-2</v>
-      </c>
-      <c r="AD30">
-        <f t="shared" si="5"/>
-        <v>2.0208743926043816E-2</v>
-      </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>180</v>
       </c>
@@ -4386,16 +4095,8 @@
         <f t="shared" si="3"/>
         <v>2.0208743926043816E-2</v>
       </c>
-      <c r="AC31">
-        <f t="shared" si="4"/>
-        <v>1.9823720491662328E-2</v>
-      </c>
-      <c r="AD31">
-        <f t="shared" si="5"/>
-        <v>1.9438697057280834E-2</v>
-      </c>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>185</v>
       </c>
@@ -4478,16 +4179,8 @@
         <f t="shared" si="3"/>
         <v>2.1042325782678128E-2</v>
       </c>
-      <c r="AC32">
-        <f t="shared" si="4"/>
-        <v>2.0625534854360972E-2</v>
-      </c>
-      <c r="AD32">
-        <f t="shared" si="5"/>
-        <v>2.0208743926043816E-2</v>
-      </c>
     </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>190</v>
       </c>
@@ -4570,16 +4263,8 @@
         <f t="shared" si="3"/>
         <v>2.0617111396875849E-2</v>
       </c>
-      <c r="AC33">
-        <f t="shared" si="4"/>
-        <v>2.2634723369562348E-2</v>
-      </c>
-      <c r="AD33">
-        <f t="shared" si="5"/>
-        <v>2.4652335342248845E-2</v>
-      </c>
     </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>193</v>
       </c>
@@ -4662,16 +4347,8 @@
         <f t="shared" si="3"/>
         <v>2.0617111396875849E-2</v>
       </c>
-      <c r="AC34">
-        <f t="shared" si="4"/>
-        <v>1.7775489958670895E-2</v>
-      </c>
-      <c r="AD34">
-        <f t="shared" si="5"/>
-        <v>1.4933868520465937E-2</v>
-      </c>
     </row>
-    <row r="35" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>196</v>
       </c>
@@ -4754,16 +4431,8 @@
         <f t="shared" si="3"/>
         <v>2.0410885006989385E-2</v>
       </c>
-      <c r="AC35">
-        <f t="shared" si="4"/>
-        <v>2.2413611171258761E-2</v>
-      </c>
-      <c r="AD35">
-        <f t="shared" si="5"/>
-        <v>2.4416337335528129E-2</v>
-      </c>
     </row>
-    <row r="36" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>199</v>
       </c>
@@ -4846,16 +4515,8 @@
         <f t="shared" si="3"/>
         <v>2.1261579796208196E-2</v>
       </c>
-      <c r="AC36">
-        <f t="shared" si="4"/>
-        <v>2.0836232401598792E-2</v>
-      </c>
-      <c r="AD36">
-        <f t="shared" si="5"/>
-        <v>2.0410885006989385E-2</v>
-      </c>
     </row>
-    <row r="37" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>203</v>
       </c>
@@ -4938,16 +4599,8 @@
         <f t="shared" si="3"/>
         <v>2.0617111396875849E-2</v>
       </c>
-      <c r="AC37">
-        <f t="shared" si="4"/>
-        <v>2.021667644238281E-2</v>
-      </c>
-      <c r="AD37">
-        <f t="shared" si="5"/>
-        <v>1.9816241487889776E-2</v>
-      </c>
     </row>
-    <row r="38" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>207</v>
       </c>
@@ -5030,16 +4683,8 @@
         <f t="shared" si="3"/>
         <v>2.0208743926043816E-2</v>
       </c>
-      <c r="AC38">
-        <f t="shared" si="4"/>
-        <v>1.9823720491662328E-2</v>
-      </c>
-      <c r="AD38">
-        <f t="shared" si="5"/>
-        <v>1.9438697057280834E-2</v>
-      </c>
     </row>
-    <row r="39" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>211</v>
       </c>
@@ -5122,16 +4767,8 @@
         <f t="shared" si="3"/>
         <v>1.5384203148309978E-2</v>
       </c>
-      <c r="AC39">
-        <f t="shared" si="4"/>
-        <v>1.7600222318099878E-2</v>
-      </c>
-      <c r="AD39">
-        <f t="shared" si="5"/>
-        <v>1.9816241487889776E-2</v>
-      </c>
     </row>
-    <row r="40" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>215</v>
       </c>
@@ -5214,16 +4851,8 @@
         <f t="shared" si="3"/>
         <v>2.0617111396875849E-2</v>
       </c>
-      <c r="AC40">
-        <f t="shared" si="4"/>
-        <v>2.2634723369562348E-2</v>
-      </c>
-      <c r="AD40">
-        <f t="shared" si="5"/>
-        <v>2.4652335342248845E-2</v>
-      </c>
     </row>
-    <row r="41" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>218</v>
       </c>
@@ -5306,16 +4935,8 @@
         <f t="shared" si="3"/>
         <v>3.6273429430474645E-2</v>
       </c>
-      <c r="AC41">
-        <f t="shared" si="4"/>
-        <v>3.5069130262398725E-2</v>
-      </c>
-      <c r="AD41">
-        <f t="shared" si="5"/>
-        <v>3.3864831094322805E-2</v>
-      </c>
     </row>
-    <row r="42" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>222</v>
       </c>
@@ -5398,16 +5019,8 @@
         <f t="shared" si="3"/>
         <v>1.5540411981994171E-2</v>
       </c>
-      <c r="AC42">
-        <f t="shared" si="4"/>
-        <v>1.7775489958670895E-2</v>
-      </c>
-      <c r="AD42">
-        <f t="shared" si="5"/>
-        <v>2.0010567935347619E-2</v>
-      </c>
     </row>
-    <row r="43" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>226</v>
       </c>
@@ -5490,16 +5103,8 @@
         <f t="shared" si="3"/>
         <v>2.0208743926043816E-2</v>
       </c>
-      <c r="AC43">
-        <f t="shared" si="4"/>
-        <v>1.9823720491662328E-2</v>
-      </c>
-      <c r="AD43">
-        <f t="shared" si="5"/>
-        <v>1.9438697057280834E-2</v>
-      </c>
     </row>
-    <row r="44" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>228</v>
       </c>
@@ -5582,16 +5187,8 @@
         <f t="shared" si="3"/>
         <v>1.5231103647796521E-2</v>
       </c>
-      <c r="AC44">
-        <f t="shared" si="4"/>
-        <v>1.7428378565682977E-2</v>
-      </c>
-      <c r="AD44">
-        <f t="shared" si="5"/>
-        <v>1.9625653483569438E-2</v>
-      </c>
     </row>
-    <row r="45" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>232</v>
       </c>
@@ -5674,16 +5271,8 @@
         <f t="shared" si="3"/>
         <v>2.0410885006989385E-2</v>
       </c>
-      <c r="AC45">
-        <f t="shared" si="4"/>
-        <v>1.7600222318099878E-2</v>
-      </c>
-      <c r="AD45">
-        <f t="shared" si="5"/>
-        <v>1.4789559629210367E-2</v>
-      </c>
     </row>
-    <row r="46" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>235</v>
       </c>
@@ -5766,16 +5355,8 @@
         <f t="shared" si="3"/>
         <v>1.5231103647796521E-2</v>
       </c>
-      <c r="AC46">
-        <f t="shared" si="4"/>
-        <v>1.7428378565682977E-2</v>
-      </c>
-      <c r="AD46">
-        <f t="shared" si="5"/>
-        <v>1.9625653483569438E-2</v>
-      </c>
     </row>
-    <row r="47" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>237</v>
       </c>
@@ -5858,16 +5439,8 @@
         <f t="shared" si="3"/>
         <v>1.5384203148309978E-2</v>
       </c>
-      <c r="AC47">
-        <f t="shared" si="4"/>
-        <v>1.7600222318099878E-2</v>
-      </c>
-      <c r="AD47">
-        <f t="shared" si="5"/>
-        <v>1.9816241487889776E-2</v>
-      </c>
     </row>
-    <row r="48" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>240</v>
       </c>
@@ -5950,16 +5523,8 @@
         <f t="shared" si="3"/>
         <v>2.0208743926043816E-2</v>
       </c>
-      <c r="AC48">
-        <f t="shared" si="4"/>
-        <v>1.9823720491662328E-2</v>
-      </c>
-      <c r="AD48">
-        <f t="shared" si="5"/>
-        <v>1.9438697057280834E-2</v>
-      </c>
     </row>
-    <row r="49" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>243</v>
       </c>
@@ -6042,16 +5607,8 @@
         <f t="shared" si="3"/>
         <v>2.0617111396875849E-2</v>
       </c>
-      <c r="AC49">
-        <f t="shared" si="4"/>
-        <v>2.021667644238281E-2</v>
-      </c>
-      <c r="AD49">
-        <f t="shared" si="5"/>
-        <v>1.9816241487889776E-2</v>
-      </c>
     </row>
-    <row r="50" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>246</v>
       </c>
@@ -6134,16 +5691,8 @@
         <f t="shared" si="3"/>
         <v>2.0827548224619984E-2</v>
       </c>
-      <c r="AC50">
-        <f t="shared" si="4"/>
-        <v>2.0419058079983801E-2</v>
-      </c>
-      <c r="AD50">
-        <f t="shared" si="5"/>
-        <v>2.0010567935347619E-2</v>
-      </c>
     </row>
-    <row r="51" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>248</v>
       </c>
@@ -6226,16 +5775,8 @@
         <f t="shared" si="3"/>
         <v>3.1246747571795241E-2</v>
       </c>
-      <c r="AC51">
-        <f t="shared" si="4"/>
-        <v>3.0344883383001391E-2</v>
-      </c>
-      <c r="AD51">
-        <f t="shared" si="5"/>
-        <v>2.9443019194207536E-2</v>
-      </c>
     </row>
-    <row r="52" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>252</v>
       </c>
@@ -6318,16 +5859,8 @@
         <f t="shared" si="3"/>
         <v>1.6028671547642325E-2</v>
       </c>
-      <c r="AC52">
-        <f t="shared" si="4"/>
-        <v>1.5784541764818246E-2</v>
-      </c>
-      <c r="AD52">
-        <f t="shared" si="5"/>
-        <v>1.5540411981994171E-2</v>
-      </c>
     </row>
-    <row r="53" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>255</v>
       </c>
@@ -6410,16 +5943,8 @@
         <f t="shared" si="3"/>
         <v>2.0010567935347619E-2</v>
       </c>
-      <c r="AC53">
-        <f t="shared" si="4"/>
-        <v>2.1984106183941941E-2</v>
-      </c>
-      <c r="AD53">
-        <f t="shared" si="5"/>
-        <v>2.3957644432536267E-2</v>
-      </c>
     </row>
-    <row r="54" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>259</v>
       </c>
@@ -6502,16 +6027,8 @@
         <f t="shared" si="3"/>
         <v>2.6718359957814238E-2</v>
       </c>
-      <c r="AC54">
-        <f t="shared" si="4"/>
-        <v>2.851821581329508E-2</v>
-      </c>
-      <c r="AD54">
-        <f t="shared" si="5"/>
-        <v>3.0318071668775915E-2</v>
-      </c>
     </row>
-    <row r="55" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>262</v>
       </c>
@@ -6594,16 +6111,8 @@
         <f t="shared" si="3"/>
         <v>1.5540411981994171E-2</v>
       </c>
-      <c r="AC55">
-        <f t="shared" si="4"/>
-        <v>1.7775489958670895E-2</v>
-      </c>
-      <c r="AD55">
-        <f t="shared" si="5"/>
-        <v>2.0010567935347619E-2</v>
-      </c>
     </row>
-    <row r="56" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>265</v>
       </c>
@@ -6686,16 +6195,8 @@
         <f t="shared" si="3"/>
         <v>2.538852528523668E-2</v>
       </c>
-      <c r="AC56">
-        <f t="shared" si="4"/>
-        <v>2.4786670523889762E-2</v>
-      </c>
-      <c r="AD56">
-        <f t="shared" si="5"/>
-        <v>2.418481576254284E-2</v>
-      </c>
     </row>
-    <row r="57" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>268</v>
       </c>
@@ -6778,16 +6279,8 @@
         <f t="shared" si="3"/>
         <v>2.0617111396875849E-2</v>
       </c>
-      <c r="AC57">
-        <f t="shared" si="4"/>
-        <v>2.021667644238281E-2</v>
-      </c>
-      <c r="AD57">
-        <f t="shared" si="5"/>
-        <v>1.9816241487889776E-2</v>
-      </c>
     </row>
-    <row r="58" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>270</v>
       </c>
@@ -6870,16 +6363,8 @@
         <f t="shared" si="3"/>
         <v>1.5384203148309978E-2</v>
       </c>
-      <c r="AC58">
-        <f t="shared" si="4"/>
-        <v>1.7600222318099878E-2</v>
-      </c>
-      <c r="AD58">
-        <f t="shared" si="5"/>
-        <v>1.9816241487889776E-2</v>
-      </c>
     </row>
-    <row r="59" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>273</v>
       </c>
@@ -6962,16 +6447,8 @@
         <f t="shared" si="3"/>
         <v>2.1485451709248368E-2</v>
       </c>
-      <c r="AC59">
-        <f t="shared" si="4"/>
-        <v>2.1051281553062108E-2</v>
-      </c>
-      <c r="AD59">
-        <f t="shared" si="5"/>
-        <v>2.0617111396875849E-2</v>
-      </c>
     </row>
-    <row r="60" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>276</v>
       </c>
@@ -7054,16 +6531,8 @@
         <f t="shared" si="3"/>
         <v>1.5540411981994171E-2</v>
       </c>
-      <c r="AC60">
-        <f t="shared" si="4"/>
-        <v>1.7775489958670895E-2</v>
-      </c>
-      <c r="AD60">
-        <f t="shared" si="5"/>
-        <v>2.0010567935347619E-2</v>
-      </c>
     </row>
-    <row r="61" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>279</v>
       </c>
@@ -7146,16 +6615,8 @@
         <f t="shared" si="3"/>
         <v>1.5231103647796521E-2</v>
       </c>
-      <c r="AC61">
-        <f t="shared" si="4"/>
-        <v>1.7428378565682977E-2</v>
-      </c>
-      <c r="AD61">
-        <f t="shared" si="5"/>
-        <v>1.9625653483569438E-2</v>
-      </c>
     </row>
-    <row r="62" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>282</v>
       </c>
@@ -7238,16 +6699,8 @@
         <f t="shared" si="3"/>
         <v>3.0020663277006889E-2</v>
       </c>
-      <c r="AC62">
-        <f t="shared" si="4"/>
-        <v>2.9186314075955181E-2</v>
-      </c>
-      <c r="AD62">
-        <f t="shared" si="5"/>
-        <v>2.8351964874903473E-2</v>
-      </c>
     </row>
-    <row r="63" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>287</v>
       </c>
@@ -7330,16 +6783,8 @@
         <f t="shared" si="3"/>
         <v>3.0930929498181069E-2</v>
       </c>
-      <c r="AC63">
-        <f t="shared" si="4"/>
-        <v>3.0046692769485604E-2</v>
-      </c>
-      <c r="AD63">
-        <f t="shared" si="5"/>
-        <v>2.9162456040790135E-2</v>
-      </c>
     </row>
-    <row r="64" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>291</v>
       </c>
@@ -7422,16 +6867,8 @@
         <f t="shared" si="3"/>
         <v>1.5540411981994171E-2</v>
       </c>
-      <c r="AC64">
-        <f t="shared" si="4"/>
-        <v>1.7775489958670895E-2</v>
-      </c>
-      <c r="AD64">
-        <f t="shared" si="5"/>
-        <v>2.0010567935347619E-2</v>
-      </c>
     </row>
-    <row r="65" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>293</v>
       </c>
@@ -7514,16 +6951,8 @@
         <f t="shared" si="3"/>
         <v>2.0827548224619984E-2</v>
       </c>
-      <c r="AC65">
-        <f t="shared" si="4"/>
-        <v>1.795428488821418E-2</v>
-      </c>
-      <c r="AD65">
-        <f t="shared" si="5"/>
-        <v>1.5081021551808382E-2</v>
-      </c>
     </row>
-    <row r="66" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>296</v>
       </c>
@@ -7606,16 +7035,8 @@
         <f t="shared" si="3"/>
         <v>2.0410885006989385E-2</v>
       </c>
-      <c r="AC66">
-        <f t="shared" si="4"/>
-        <v>1.7600222318099878E-2</v>
-      </c>
-      <c r="AD66">
-        <f t="shared" si="5"/>
-        <v>1.4789559629210367E-2</v>
-      </c>
     </row>
-    <row r="67" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>300</v>
       </c>
@@ -7698,16 +7119,8 @@
         <f t="shared" si="3"/>
         <v>2.0208743926043816E-2</v>
       </c>
-      <c r="AC67">
-        <f t="shared" si="4"/>
-        <v>1.9823720491662328E-2</v>
-      </c>
-      <c r="AD67">
-        <f t="shared" si="5"/>
-        <v>1.9438697057280834E-2</v>
-      </c>
     </row>
-    <row r="68" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>303</v>
       </c>
@@ -7759,11 +7172,11 @@
         <v>322035</v>
       </c>
       <c r="S68">
-        <f t="shared" ref="S68:S72" si="6">_xlfn.T.INV.2T(Q68,R68)</f>
+        <f t="shared" ref="S68:S72" si="4">_xlfn.T.INV.2T(Q68,R68)</f>
         <v>5.5415731179516623</v>
       </c>
       <c r="T68">
-        <f t="shared" ref="T68:T72" si="7">ABS(S68)</f>
+        <f t="shared" ref="T68:T72" si="5">ABS(S68)</f>
         <v>5.5415731179516623</v>
       </c>
       <c r="U68" t="str">
@@ -7771,7 +7184,7 @@
         <v>0.040</v>
       </c>
       <c r="V68">
-        <f t="shared" ref="V68:V72" si="8">U68/T68</f>
+        <f t="shared" ref="V68:V72" si="6">U68/T68</f>
         <v>7.21816696245005E-3</v>
       </c>
       <c r="Y68">
@@ -7787,19 +7200,11 @@
         <v>0.13976194237515863</v>
       </c>
       <c r="AB68">
-        <f t="shared" ref="AB68:AB72" si="9">(Y68-Z68)/1.96</f>
+        <f t="shared" ref="AB68:AB72" si="7">(Y68-Z68)/1.96</f>
         <v>4.0036538490558826E-2</v>
       </c>
-      <c r="AC68">
-        <f t="shared" ref="AC68:AC72" si="10">(AA68-Z68)/2/1.96</f>
-        <v>4.0807308595070944E-2</v>
-      </c>
-      <c r="AD68">
-        <f t="shared" ref="AD68:AD72" si="11">(AA68-Y68)/1.96</f>
-        <v>4.1578078699583063E-2</v>
-      </c>
     </row>
-    <row r="69" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>308</v>
       </c>
@@ -7851,11 +7256,11 @@
         <v>322035</v>
       </c>
       <c r="S69">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>5.5196170398503144</v>
       </c>
       <c r="T69">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>5.5196170398503144</v>
       </c>
       <c r="U69" t="str">
@@ -7863,7 +7268,7 @@
         <v>0.019</v>
       </c>
       <c r="V69">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>3.4422677991651496E-3</v>
       </c>
       <c r="Y69">
@@ -7879,19 +7284,11 @@
         <v>5.8268908123975824E-2</v>
       </c>
       <c r="AB69">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>2.0410885006989385E-2</v>
       </c>
-      <c r="AC69">
-        <f t="shared" si="10"/>
-        <v>2.0018269245279413E-2</v>
-      </c>
-      <c r="AD69">
-        <f t="shared" si="11"/>
-        <v>1.9625653483569438E-2</v>
-      </c>
     </row>
-    <row r="70" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>312</v>
       </c>
@@ -7943,11 +7340,11 @@
         <v>322035</v>
       </c>
       <c r="S70">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>5.49545425854319</v>
       </c>
       <c r="T70">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>5.49545425854319</v>
       </c>
       <c r="U70" t="str">
@@ -7955,7 +7352,7 @@
         <v>0.022</v>
       </c>
       <c r="V70">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>4.0033087284456915E-3</v>
       </c>
       <c r="Y70">
@@ -7971,19 +7368,11 @@
         <v>3.9220713153281329E-2</v>
       </c>
       <c r="AB70">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>2.1042325782678128E-2</v>
       </c>
-      <c r="AC70">
-        <f t="shared" si="10"/>
-        <v>2.3090308046130589E-2</v>
-      </c>
-      <c r="AD70">
-        <f t="shared" si="11"/>
-        <v>2.5138290309583051E-2</v>
-      </c>
     </row>
-    <row r="71" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>316</v>
       </c>
@@ -8035,11 +7424,11 @@
         <v>322035</v>
       </c>
       <c r="S71">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>5.4823612021473993</v>
       </c>
       <c r="T71">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>5.4823612021473993</v>
       </c>
       <c r="U71" t="str">
@@ -8047,7 +7436,7 @@
         <v>0.017</v>
       </c>
       <c r="V71">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>3.1008536966410077E-3</v>
       </c>
       <c r="Y71">
@@ -8063,19 +7452,11 @@
         <v>3.9220713153281329E-2</v>
       </c>
       <c r="AB71">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>2.0827548224619984E-2</v>
       </c>
-      <c r="AC71">
-        <f t="shared" si="10"/>
-        <v>2.0419058079983801E-2</v>
-      </c>
-      <c r="AD71">
-        <f t="shared" si="11"/>
-        <v>2.0010567935347619E-2</v>
-      </c>
     </row>
-    <row r="72" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>319</v>
       </c>
@@ -8127,11 +7508,11 @@
         <v>322035</v>
       </c>
       <c r="S72">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>5.4550317441294514</v>
       </c>
       <c r="T72">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>5.4550317441294514</v>
       </c>
       <c r="U72" t="str">
@@ -8139,7 +7520,7 @@
         <v>0.019</v>
       </c>
       <c r="V72">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>3.4830228110857933E-3</v>
       </c>
       <c r="Y72">
@@ -8155,16 +7536,8 @@
         <v>3.9220713153281329E-2</v>
       </c>
       <c r="AB72">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>2.0827548224619984E-2</v>
-      </c>
-      <c r="AC72">
-        <f t="shared" si="10"/>
-        <v>2.0419058079983801E-2</v>
-      </c>
-      <c r="AD72">
-        <f t="shared" si="11"/>
-        <v>2.0010567935347619E-2</v>
       </c>
     </row>
   </sheetData>
@@ -8177,2501 +7550,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE890338-A9EB-449D-8D4F-895A2109274B}">
-  <dimension ref="A1:K71"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G71"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>337</v>
-      </c>
-      <c r="B1" t="s">
-        <v>338</v>
-      </c>
-      <c r="C1" t="s">
-        <v>339</v>
-      </c>
-      <c r="D1" t="s">
-        <v>340</v>
-      </c>
-      <c r="E1" t="s">
-        <v>341</v>
-      </c>
-      <c r="F1" t="s">
-        <v>342</v>
-      </c>
-      <c r="G1" t="s">
-        <v>343</v>
-      </c>
-      <c r="H1" t="s">
-        <v>344</v>
-      </c>
-      <c r="I1" t="s">
-        <v>345</v>
-      </c>
-      <c r="J1" t="s">
-        <v>346</v>
-      </c>
-      <c r="K1" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>348</v>
-      </c>
-      <c r="B2" t="s">
-        <v>349</v>
-      </c>
-      <c r="C2" t="s">
-        <v>350</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>351</v>
-      </c>
-      <c r="F2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" t="s">
-        <v>352</v>
-      </c>
-      <c r="H2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2">
-        <v>1.7106513699587575E-3</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>1.7775489958670895E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>348</v>
-      </c>
-      <c r="B3" t="s">
-        <v>349</v>
-      </c>
-      <c r="C3" t="s">
-        <v>350</v>
-      </c>
-      <c r="D3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" t="s">
-        <v>351</v>
-      </c>
-      <c r="F3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" t="s">
-        <v>352</v>
-      </c>
-      <c r="H3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I3">
-        <v>3.649024665057384E-3</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>2.0419058079983801E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>348</v>
-      </c>
-      <c r="B4" t="s">
-        <v>349</v>
-      </c>
-      <c r="C4" t="s">
-        <v>350</v>
-      </c>
-      <c r="D4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" t="s">
-        <v>351</v>
-      </c>
-      <c r="F4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G4" t="s">
-        <v>352</v>
-      </c>
-      <c r="H4" t="s">
-        <v>43</v>
-      </c>
-      <c r="I4">
-        <v>4.0064745893953089E-3</v>
-      </c>
-      <c r="J4">
-        <v>4.8790164169432049E-2</v>
-      </c>
-      <c r="K4">
-        <v>2.1775471671213478E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>348</v>
-      </c>
-      <c r="B5" t="s">
-        <v>349</v>
-      </c>
-      <c r="C5" t="s">
-        <v>350</v>
-      </c>
-      <c r="D5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" t="s">
-        <v>351</v>
-      </c>
-      <c r="F5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G5" t="s">
-        <v>352</v>
-      </c>
-      <c r="H5" t="s">
-        <v>51</v>
-      </c>
-      <c r="I5">
-        <v>3.0940714867255959E-3</v>
-      </c>
-      <c r="J5">
-        <v>1.980262729617973E-2</v>
-      </c>
-      <c r="K5">
-        <v>1.5010331638503445E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>348</v>
-      </c>
-      <c r="B6" t="s">
-        <v>349</v>
-      </c>
-      <c r="C6" t="s">
-        <v>350</v>
-      </c>
-      <c r="D6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" t="s">
-        <v>351</v>
-      </c>
-      <c r="F6" t="s">
-        <v>55</v>
-      </c>
-      <c r="G6" t="s">
-        <v>352</v>
-      </c>
-      <c r="H6" t="s">
-        <v>58</v>
-      </c>
-      <c r="I6">
-        <v>3.8703756544317736E-3</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>2.286024456369572E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>348</v>
-      </c>
-      <c r="B7" t="s">
-        <v>349</v>
-      </c>
-      <c r="C7" t="s">
-        <v>350</v>
-      </c>
-      <c r="D7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" t="s">
-        <v>351</v>
-      </c>
-      <c r="F7" t="s">
-        <v>62</v>
-      </c>
-      <c r="G7" t="s">
-        <v>352</v>
-      </c>
-      <c r="H7" t="s">
-        <v>65</v>
-      </c>
-      <c r="I7">
-        <v>4.017638968914862E-3</v>
-      </c>
-      <c r="J7">
-        <v>3.9220713153281329E-2</v>
-      </c>
-      <c r="K7">
-        <v>2.219677984429333E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>348</v>
-      </c>
-      <c r="B8" t="s">
-        <v>349</v>
-      </c>
-      <c r="C8" t="s">
-        <v>350</v>
-      </c>
-      <c r="D8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" t="s">
-        <v>351</v>
-      </c>
-      <c r="F8" t="s">
-        <v>69</v>
-      </c>
-      <c r="G8" t="s">
-        <v>352</v>
-      </c>
-      <c r="H8" t="s">
-        <v>72</v>
-      </c>
-      <c r="I8">
-        <v>3.7386530646937952E-3</v>
-      </c>
-      <c r="J8">
-        <v>2.9558802241544429E-2</v>
-      </c>
-      <c r="K8">
-        <v>2.219677984429333E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>348</v>
-      </c>
-      <c r="B9" t="s">
-        <v>349</v>
-      </c>
-      <c r="C9" t="s">
-        <v>350</v>
-      </c>
-      <c r="D9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9" t="s">
-        <v>351</v>
-      </c>
-      <c r="F9" t="s">
-        <v>74</v>
-      </c>
-      <c r="G9" t="s">
-        <v>352</v>
-      </c>
-      <c r="H9" t="s">
-        <v>77</v>
-      </c>
-      <c r="I9">
-        <v>3.1102284521522887E-3</v>
-      </c>
-      <c r="J9">
-        <v>-1.0050335853501451E-2</v>
-      </c>
-      <c r="K9">
-        <v>1.795428488821418E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>348</v>
-      </c>
-      <c r="B10" t="s">
-        <v>349</v>
-      </c>
-      <c r="C10" t="s">
-        <v>350</v>
-      </c>
-      <c r="D10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10" t="s">
-        <v>351</v>
-      </c>
-      <c r="F10" t="s">
-        <v>81</v>
-      </c>
-      <c r="G10" t="s">
-        <v>352</v>
-      </c>
-      <c r="H10" t="s">
-        <v>84</v>
-      </c>
-      <c r="I10">
-        <v>3.1802854664185814E-3</v>
-      </c>
-      <c r="J10">
-        <v>1.980262729617973E-2</v>
-      </c>
-      <c r="K10">
-        <v>2.0018269245279413E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>348</v>
-      </c>
-      <c r="B11" t="s">
-        <v>349</v>
-      </c>
-      <c r="C11" t="s">
-        <v>350</v>
-      </c>
-      <c r="D11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11" t="s">
-        <v>351</v>
-      </c>
-      <c r="F11" t="s">
-        <v>88</v>
-      </c>
-      <c r="G11" t="s">
-        <v>352</v>
-      </c>
-      <c r="H11" t="s">
-        <v>91</v>
-      </c>
-      <c r="I11">
-        <v>3.0830327170072495E-3</v>
-      </c>
-      <c r="J11">
-        <v>5.8268908123975824E-2</v>
-      </c>
-      <c r="K11">
-        <v>1.6932415547161402E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>348</v>
-      </c>
-      <c r="B12" t="s">
-        <v>349</v>
-      </c>
-      <c r="C12" t="s">
-        <v>350</v>
-      </c>
-      <c r="D12" t="s">
-        <v>3</v>
-      </c>
-      <c r="E12" t="s">
-        <v>351</v>
-      </c>
-      <c r="F12" t="s">
-        <v>95</v>
-      </c>
-      <c r="G12" t="s">
-        <v>352</v>
-      </c>
-      <c r="H12" t="s">
-        <v>91</v>
-      </c>
-      <c r="I12">
-        <v>3.1217885107430307E-3</v>
-      </c>
-      <c r="J12">
-        <v>9.950330853168092E-3</v>
-      </c>
-      <c r="K12">
-        <v>1.7775489958670895E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>348</v>
-      </c>
-      <c r="B13" t="s">
-        <v>349</v>
-      </c>
-      <c r="C13" t="s">
-        <v>350</v>
-      </c>
-      <c r="D13" t="s">
-        <v>3</v>
-      </c>
-      <c r="E13" t="s">
-        <v>351</v>
-      </c>
-      <c r="F13" t="s">
-        <v>99</v>
-      </c>
-      <c r="G13" t="s">
-        <v>352</v>
-      </c>
-      <c r="H13" t="s">
-        <v>65</v>
-      </c>
-      <c r="I13">
-        <v>4.6164610650375592E-3</v>
-      </c>
-      <c r="J13">
-        <v>1.980262729617973E-2</v>
-      </c>
-      <c r="K13">
-        <v>2.7403124648172694E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>348</v>
-      </c>
-      <c r="B14" t="s">
-        <v>349</v>
-      </c>
-      <c r="C14" t="s">
-        <v>350</v>
-      </c>
-      <c r="D14" t="s">
-        <v>3</v>
-      </c>
-      <c r="E14" t="s">
-        <v>351</v>
-      </c>
-      <c r="F14" t="s">
-        <v>103</v>
-      </c>
-      <c r="G14" t="s">
-        <v>352</v>
-      </c>
-      <c r="H14" t="s">
-        <v>51</v>
-      </c>
-      <c r="I14">
-        <v>4.5505201226154141E-3</v>
-      </c>
-      <c r="J14">
-        <v>5.8268908123975824E-2</v>
-      </c>
-      <c r="K14">
-        <v>2.8910378904847774E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>348</v>
-      </c>
-      <c r="B15" t="s">
-        <v>349</v>
-      </c>
-      <c r="C15" t="s">
-        <v>350</v>
-      </c>
-      <c r="D15" t="s">
-        <v>3</v>
-      </c>
-      <c r="E15" t="s">
-        <v>351</v>
-      </c>
-      <c r="F15" t="s">
-        <v>108</v>
-      </c>
-      <c r="G15" t="s">
-        <v>352</v>
-      </c>
-      <c r="H15" t="s">
-        <v>111</v>
-      </c>
-      <c r="I15">
-        <v>4.1554174164966174E-3</v>
-      </c>
-      <c r="J15">
-        <v>4.8790164169432049E-2</v>
-      </c>
-      <c r="K15">
-        <v>2.1984106183941941E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>348</v>
-      </c>
-      <c r="B16" t="s">
-        <v>349</v>
-      </c>
-      <c r="C16" t="s">
-        <v>350</v>
-      </c>
-      <c r="D16" t="s">
-        <v>3</v>
-      </c>
-      <c r="E16" t="s">
-        <v>351</v>
-      </c>
-      <c r="F16" t="s">
-        <v>113</v>
-      </c>
-      <c r="G16" t="s">
-        <v>352</v>
-      </c>
-      <c r="H16" t="s">
-        <v>91</v>
-      </c>
-      <c r="I16">
-        <v>3.6469588572924081E-3</v>
-      </c>
-      <c r="J16">
-        <v>-1.0050335853501451E-2</v>
-      </c>
-      <c r="K16">
-        <v>2.0625534854360972E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>348</v>
-      </c>
-      <c r="B17" t="s">
-        <v>349</v>
-      </c>
-      <c r="C17" t="s">
-        <v>350</v>
-      </c>
-      <c r="D17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E17" t="s">
-        <v>351</v>
-      </c>
-      <c r="F17" t="s">
-        <v>120</v>
-      </c>
-      <c r="G17" t="s">
-        <v>352</v>
-      </c>
-      <c r="H17" t="s">
-        <v>122</v>
-      </c>
-      <c r="I17">
-        <v>3.1016834013285568E-3</v>
-      </c>
-      <c r="J17">
-        <v>-3.0459207484708574E-2</v>
-      </c>
-      <c r="K17">
-        <v>1.832289147225909E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>348</v>
-      </c>
-      <c r="B18" t="s">
-        <v>349</v>
-      </c>
-      <c r="C18" t="s">
-        <v>350</v>
-      </c>
-      <c r="D18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E18" t="s">
-        <v>351</v>
-      </c>
-      <c r="F18" t="s">
-        <v>126</v>
-      </c>
-      <c r="G18" t="s">
-        <v>352</v>
-      </c>
-      <c r="H18" t="s">
-        <v>122</v>
-      </c>
-      <c r="I18">
-        <v>3.1093712759504904E-3</v>
-      </c>
-      <c r="J18">
-        <v>1.980262729617973E-2</v>
-      </c>
-      <c r="K18">
-        <v>1.7600222318099878E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>348</v>
-      </c>
-      <c r="B19" t="s">
-        <v>349</v>
-      </c>
-      <c r="C19" t="s">
-        <v>350</v>
-      </c>
-      <c r="D19" t="s">
-        <v>3</v>
-      </c>
-      <c r="E19" t="s">
-        <v>351</v>
-      </c>
-      <c r="F19" t="s">
-        <v>130</v>
-      </c>
-      <c r="G19" t="s">
-        <v>352</v>
-      </c>
-      <c r="H19" t="s">
-        <v>133</v>
-      </c>
-      <c r="I19">
-        <v>3.0459209921138621E-3</v>
-      </c>
-      <c r="J19">
-        <v>-1.0050335853501451E-2</v>
-      </c>
-      <c r="K19">
-        <v>1.795428488821418E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>348</v>
-      </c>
-      <c r="B20" t="s">
-        <v>349</v>
-      </c>
-      <c r="C20" t="s">
-        <v>350</v>
-      </c>
-      <c r="D20" t="s">
-        <v>3</v>
-      </c>
-      <c r="E20" t="s">
-        <v>351</v>
-      </c>
-      <c r="F20" t="s">
-        <v>136</v>
-      </c>
-      <c r="G20" t="s">
-        <v>352</v>
-      </c>
-      <c r="H20" t="s">
-        <v>139</v>
-      </c>
-      <c r="I20">
-        <v>3.5748833303499571E-3</v>
-      </c>
-      <c r="J20">
-        <v>-3.0459207484708574E-2</v>
-      </c>
-      <c r="K20">
-        <v>1.832289147225909E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>348</v>
-      </c>
-      <c r="B21" t="s">
-        <v>349</v>
-      </c>
-      <c r="C21" t="s">
-        <v>350</v>
-      </c>
-      <c r="D21" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" t="s">
-        <v>351</v>
-      </c>
-      <c r="F21" t="s">
-        <v>141</v>
-      </c>
-      <c r="G21" t="s">
-        <v>352</v>
-      </c>
-      <c r="H21" t="s">
-        <v>133</v>
-      </c>
-      <c r="I21">
-        <v>3.1102577503204702E-3</v>
-      </c>
-      <c r="J21">
-        <v>1.980262729617973E-2</v>
-      </c>
-      <c r="K21">
-        <v>1.7428378565682977E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>348</v>
-      </c>
-      <c r="B22" t="s">
-        <v>349</v>
-      </c>
-      <c r="C22" t="s">
-        <v>350</v>
-      </c>
-      <c r="D22" t="s">
-        <v>3</v>
-      </c>
-      <c r="E22" t="s">
-        <v>351</v>
-      </c>
-      <c r="F22" t="s">
-        <v>144</v>
-      </c>
-      <c r="G22" t="s">
-        <v>352</v>
-      </c>
-      <c r="H22" t="s">
-        <v>147</v>
-      </c>
-      <c r="I22">
-        <v>3.9103977687082164E-3</v>
-      </c>
-      <c r="J22">
-        <v>-1.0050335853501451E-2</v>
-      </c>
-      <c r="K22">
-        <v>2.3090308046130589E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>348</v>
-      </c>
-      <c r="B23" t="s">
-        <v>349</v>
-      </c>
-      <c r="C23" t="s">
-        <v>350</v>
-      </c>
-      <c r="D23" t="s">
-        <v>3</v>
-      </c>
-      <c r="E23" t="s">
-        <v>351</v>
-      </c>
-      <c r="F23" t="s">
-        <v>149</v>
-      </c>
-      <c r="G23" t="s">
-        <v>352</v>
-      </c>
-      <c r="H23" t="s">
-        <v>152</v>
-      </c>
-      <c r="I23">
-        <v>3.3351457186432043E-3</v>
-      </c>
-      <c r="J23">
-        <v>9.950330853168092E-3</v>
-      </c>
-      <c r="K23">
-        <v>2.021667644238281E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>348</v>
-      </c>
-      <c r="B24" t="s">
-        <v>349</v>
-      </c>
-      <c r="C24" t="s">
-        <v>350</v>
-      </c>
-      <c r="D24" t="s">
-        <v>3</v>
-      </c>
-      <c r="E24" t="s">
-        <v>351</v>
-      </c>
-      <c r="F24" t="s">
-        <v>154</v>
-      </c>
-      <c r="G24" t="s">
-        <v>352</v>
-      </c>
-      <c r="H24" t="s">
-        <v>77</v>
-      </c>
-      <c r="I24">
-        <v>4.6363533717789568E-3</v>
-      </c>
-      <c r="J24">
-        <v>9.950330853168092E-3</v>
-      </c>
-      <c r="K24">
-        <v>2.5278291490875252E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>348</v>
-      </c>
-      <c r="B25" t="s">
-        <v>349</v>
-      </c>
-      <c r="C25" t="s">
-        <v>350</v>
-      </c>
-      <c r="D25" t="s">
-        <v>3</v>
-      </c>
-      <c r="E25" t="s">
-        <v>351</v>
-      </c>
-      <c r="F25" t="s">
-        <v>157</v>
-      </c>
-      <c r="G25" t="s">
-        <v>352</v>
-      </c>
-      <c r="H25" t="s">
-        <v>160</v>
-      </c>
-      <c r="I25">
-        <v>3.1009539353891694E-3</v>
-      </c>
-      <c r="J25">
-        <v>-1.0050335853501451E-2</v>
-      </c>
-      <c r="K25">
-        <v>2.0625534854360972E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>348</v>
-      </c>
-      <c r="B26" t="s">
-        <v>349</v>
-      </c>
-      <c r="C26" t="s">
-        <v>350</v>
-      </c>
-      <c r="D26" t="s">
-        <v>3</v>
-      </c>
-      <c r="E26" t="s">
-        <v>351</v>
-      </c>
-      <c r="F26" t="s">
-        <v>163</v>
-      </c>
-      <c r="G26" t="s">
-        <v>352</v>
-      </c>
-      <c r="H26" t="s">
-        <v>160</v>
-      </c>
-      <c r="I26">
-        <v>3.1303571212109218E-3</v>
-      </c>
-      <c r="J26">
-        <v>9.950330853168092E-3</v>
-      </c>
-      <c r="K26">
-        <v>2.021667644238281E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>348</v>
-      </c>
-      <c r="B27" t="s">
-        <v>349</v>
-      </c>
-      <c r="C27" t="s">
-        <v>350</v>
-      </c>
-      <c r="D27" t="s">
-        <v>3</v>
-      </c>
-      <c r="E27" t="s">
-        <v>351</v>
-      </c>
-      <c r="F27" t="s">
-        <v>166</v>
-      </c>
-      <c r="G27" t="s">
-        <v>352</v>
-      </c>
-      <c r="H27" t="s">
-        <v>169</v>
-      </c>
-      <c r="I27">
-        <v>3.3858286475286349E-3</v>
-      </c>
-      <c r="J27">
-        <v>-2.0202707317519466E-2</v>
-      </c>
-      <c r="K27">
-        <v>1.8136714715237322E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>348</v>
-      </c>
-      <c r="B28" t="s">
-        <v>349</v>
-      </c>
-      <c r="C28" t="s">
-        <v>350</v>
-      </c>
-      <c r="D28" t="s">
-        <v>3</v>
-      </c>
-      <c r="E28" t="s">
-        <v>351</v>
-      </c>
-      <c r="F28" t="s">
-        <v>171</v>
-      </c>
-      <c r="G28" t="s">
-        <v>352</v>
-      </c>
-      <c r="H28" t="s">
-        <v>169</v>
-      </c>
-      <c r="I28">
-        <v>3.3858286475286349E-3</v>
-      </c>
-      <c r="J28">
-        <v>0</v>
-      </c>
-      <c r="K28">
-        <v>1.795428488821418E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>348</v>
-      </c>
-      <c r="B29" t="s">
-        <v>349</v>
-      </c>
-      <c r="C29" t="s">
-        <v>350</v>
-      </c>
-      <c r="D29" t="s">
-        <v>3</v>
-      </c>
-      <c r="E29" t="s">
-        <v>351</v>
-      </c>
-      <c r="F29" t="s">
-        <v>176</v>
-      </c>
-      <c r="G29" t="s">
-        <v>352</v>
-      </c>
-      <c r="H29" t="s">
-        <v>160</v>
-      </c>
-      <c r="I29">
-        <v>3.2840062847118239E-3</v>
-      </c>
-      <c r="J29">
-        <v>-1.0050335853501451E-2</v>
-      </c>
-      <c r="K29">
-        <v>2.0625534854360972E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>348</v>
-      </c>
-      <c r="B30" t="s">
-        <v>349</v>
-      </c>
-      <c r="C30" t="s">
-        <v>350</v>
-      </c>
-      <c r="D30" t="s">
-        <v>3</v>
-      </c>
-      <c r="E30" t="s">
-        <v>351</v>
-      </c>
-      <c r="F30" t="s">
-        <v>180</v>
-      </c>
-      <c r="G30" t="s">
-        <v>352</v>
-      </c>
-      <c r="H30" t="s">
-        <v>169</v>
-      </c>
-      <c r="I30">
-        <v>3.4401141223554918E-3</v>
-      </c>
-      <c r="J30">
-        <v>2.9558802241544429E-2</v>
-      </c>
-      <c r="K30">
-        <v>1.9823720491662328E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>348</v>
-      </c>
-      <c r="B31" t="s">
-        <v>349</v>
-      </c>
-      <c r="C31" t="s">
-        <v>350</v>
-      </c>
-      <c r="D31" t="s">
-        <v>3</v>
-      </c>
-      <c r="E31" t="s">
-        <v>351</v>
-      </c>
-      <c r="F31" t="s">
-        <v>185</v>
-      </c>
-      <c r="G31" t="s">
-        <v>352</v>
-      </c>
-      <c r="H31" t="s">
-        <v>188</v>
-      </c>
-      <c r="I31">
-        <v>3.1570426012529937E-3</v>
-      </c>
-      <c r="J31">
-        <v>-1.0050335853501451E-2</v>
-      </c>
-      <c r="K31">
-        <v>2.0625534854360972E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>348</v>
-      </c>
-      <c r="B32" t="s">
-        <v>349</v>
-      </c>
-      <c r="C32" t="s">
-        <v>350</v>
-      </c>
-      <c r="D32" t="s">
-        <v>3</v>
-      </c>
-      <c r="E32" t="s">
-        <v>351</v>
-      </c>
-      <c r="F32" t="s">
-        <v>190</v>
-      </c>
-      <c r="G32" t="s">
-        <v>352</v>
-      </c>
-      <c r="H32" t="s">
-        <v>152</v>
-      </c>
-      <c r="I32">
-        <v>3.8188506389133458E-3</v>
-      </c>
-      <c r="J32">
-        <v>9.950330853168092E-3</v>
-      </c>
-      <c r="K32">
-        <v>2.2634723369562348E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>348</v>
-      </c>
-      <c r="B33" t="s">
-        <v>349</v>
-      </c>
-      <c r="C33" t="s">
-        <v>350</v>
-      </c>
-      <c r="D33" t="s">
-        <v>3</v>
-      </c>
-      <c r="E33" t="s">
-        <v>351</v>
-      </c>
-      <c r="F33" t="s">
-        <v>193</v>
-      </c>
-      <c r="G33" t="s">
-        <v>352</v>
-      </c>
-      <c r="H33" t="s">
-        <v>188</v>
-      </c>
-      <c r="I33">
-        <v>3.2611000381207386E-3</v>
-      </c>
-      <c r="J33">
-        <v>9.950330853168092E-3</v>
-      </c>
-      <c r="K33">
-        <v>1.7775489958670895E-2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>348</v>
-      </c>
-      <c r="B34" t="s">
-        <v>349</v>
-      </c>
-      <c r="C34" t="s">
-        <v>350</v>
-      </c>
-      <c r="D34" t="s">
-        <v>3</v>
-      </c>
-      <c r="E34" t="s">
-        <v>351</v>
-      </c>
-      <c r="F34" t="s">
-        <v>196</v>
-      </c>
-      <c r="G34" t="s">
-        <v>352</v>
-      </c>
-      <c r="H34" t="s">
-        <v>160</v>
-      </c>
-      <c r="I34">
-        <v>3.4163905161264875E-3</v>
-      </c>
-      <c r="J34">
-        <v>1.980262729617973E-2</v>
-      </c>
-      <c r="K34">
-        <v>2.2413611171258761E-2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>348</v>
-      </c>
-      <c r="B35" t="s">
-        <v>349</v>
-      </c>
-      <c r="C35" t="s">
-        <v>350</v>
-      </c>
-      <c r="D35" t="s">
-        <v>3</v>
-      </c>
-      <c r="E35" t="s">
-        <v>351</v>
-      </c>
-      <c r="F35" t="s">
-        <v>199</v>
-      </c>
-      <c r="G35" t="s">
-        <v>352</v>
-      </c>
-      <c r="H35" t="s">
-        <v>201</v>
-      </c>
-      <c r="I35">
-        <v>3.1270864211269097E-3</v>
-      </c>
-      <c r="J35">
-        <v>-2.0202707317519466E-2</v>
-      </c>
-      <c r="K35">
-        <v>2.0836232401598792E-2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>348</v>
-      </c>
-      <c r="B36" t="s">
-        <v>349</v>
-      </c>
-      <c r="C36" t="s">
-        <v>350</v>
-      </c>
-      <c r="D36" t="s">
-        <v>3</v>
-      </c>
-      <c r="E36" t="s">
-        <v>351</v>
-      </c>
-      <c r="F36" t="s">
-        <v>203</v>
-      </c>
-      <c r="G36" t="s">
-        <v>352</v>
-      </c>
-      <c r="H36" t="s">
-        <v>160</v>
-      </c>
-      <c r="I36">
-        <v>3.4495150546990511E-3</v>
-      </c>
-      <c r="J36">
-        <v>9.950330853168092E-3</v>
-      </c>
-      <c r="K36">
-        <v>2.021667644238281E-2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>348</v>
-      </c>
-      <c r="B37" t="s">
-        <v>349</v>
-      </c>
-      <c r="C37" t="s">
-        <v>350</v>
-      </c>
-      <c r="D37" t="s">
-        <v>3</v>
-      </c>
-      <c r="E37" t="s">
-        <v>351</v>
-      </c>
-      <c r="F37" t="s">
-        <v>207</v>
-      </c>
-      <c r="G37" t="s">
-        <v>352</v>
-      </c>
-      <c r="H37" t="s">
-        <v>201</v>
-      </c>
-      <c r="I37">
-        <v>3.1359227769991375E-3</v>
-      </c>
-      <c r="J37">
-        <v>2.9558802241544429E-2</v>
-      </c>
-      <c r="K37">
-        <v>1.9823720491662328E-2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>348</v>
-      </c>
-      <c r="B38" t="s">
-        <v>349</v>
-      </c>
-      <c r="C38" t="s">
-        <v>350</v>
-      </c>
-      <c r="D38" t="s">
-        <v>3</v>
-      </c>
-      <c r="E38" t="s">
-        <v>351</v>
-      </c>
-      <c r="F38" t="s">
-        <v>211</v>
-      </c>
-      <c r="G38" t="s">
-        <v>352</v>
-      </c>
-      <c r="H38" t="s">
-        <v>188</v>
-      </c>
-      <c r="I38">
-        <v>3.2970040060210383E-3</v>
-      </c>
-      <c r="J38">
-        <v>9.950330853168092E-3</v>
-      </c>
-      <c r="K38">
-        <v>1.7600222318099878E-2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>348</v>
-      </c>
-      <c r="B39" t="s">
-        <v>349</v>
-      </c>
-      <c r="C39" t="s">
-        <v>350</v>
-      </c>
-      <c r="D39" t="s">
-        <v>3</v>
-      </c>
-      <c r="E39" t="s">
-        <v>351</v>
-      </c>
-      <c r="F39" t="s">
-        <v>215</v>
-      </c>
-      <c r="G39" t="s">
-        <v>352</v>
-      </c>
-      <c r="H39" t="s">
-        <v>147</v>
-      </c>
-      <c r="I39">
-        <v>4.731827345175914E-3</v>
-      </c>
-      <c r="J39">
-        <v>9.950330853168092E-3</v>
-      </c>
-      <c r="K39">
-        <v>2.2634723369562348E-2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>348</v>
-      </c>
-      <c r="B40" t="s">
-        <v>349</v>
-      </c>
-      <c r="C40" t="s">
-        <v>350</v>
-      </c>
-      <c r="D40" t="s">
-        <v>3</v>
-      </c>
-      <c r="E40" t="s">
-        <v>351</v>
-      </c>
-      <c r="F40" t="s">
-        <v>218</v>
-      </c>
-      <c r="G40" t="s">
-        <v>352</v>
-      </c>
-      <c r="H40" t="s">
-        <v>58</v>
-      </c>
-      <c r="I40">
-        <v>7.6547101529929129E-3</v>
-      </c>
-      <c r="J40">
-        <v>1.980262729617973E-2</v>
-      </c>
-      <c r="K40">
-        <v>3.5069130262398725E-2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>348</v>
-      </c>
-      <c r="B41" t="s">
-        <v>349</v>
-      </c>
-      <c r="C41" t="s">
-        <v>350</v>
-      </c>
-      <c r="D41" t="s">
-        <v>3</v>
-      </c>
-      <c r="E41" t="s">
-        <v>351</v>
-      </c>
-      <c r="F41" t="s">
-        <v>222</v>
-      </c>
-      <c r="G41" t="s">
-        <v>352</v>
-      </c>
-      <c r="H41" t="s">
-        <v>201</v>
-      </c>
-      <c r="I41">
-        <v>3.2347153051164972E-3</v>
-      </c>
-      <c r="J41">
-        <v>0</v>
-      </c>
-      <c r="K41">
-        <v>1.7775489958670895E-2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>348</v>
-      </c>
-      <c r="B42" t="s">
-        <v>349</v>
-      </c>
-      <c r="C42" t="s">
-        <v>350</v>
-      </c>
-      <c r="D42" t="s">
-        <v>3</v>
-      </c>
-      <c r="E42" t="s">
-        <v>351</v>
-      </c>
-      <c r="F42" t="s">
-        <v>226</v>
-      </c>
-      <c r="G42" t="s">
-        <v>352</v>
-      </c>
-      <c r="H42" t="s">
-        <v>169</v>
-      </c>
-      <c r="I42">
-        <v>3.7365871844980301E-3</v>
-      </c>
-      <c r="J42">
-        <v>2.9558802241544429E-2</v>
-      </c>
-      <c r="K42">
-        <v>1.9823720491662328E-2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
-        <v>348</v>
-      </c>
-      <c r="B43" t="s">
-        <v>349</v>
-      </c>
-      <c r="C43" t="s">
-        <v>350</v>
-      </c>
-      <c r="D43" t="s">
-        <v>3</v>
-      </c>
-      <c r="E43" t="s">
-        <v>351</v>
-      </c>
-      <c r="F43" t="s">
-        <v>228</v>
-      </c>
-      <c r="G43" t="s">
-        <v>352</v>
-      </c>
-      <c r="H43" t="s">
-        <v>230</v>
-      </c>
-      <c r="I43">
-        <v>3.0908838625917667E-3</v>
-      </c>
-      <c r="J43">
-        <v>1.980262729617973E-2</v>
-      </c>
-      <c r="K43">
-        <v>1.7428378565682977E-2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>348</v>
-      </c>
-      <c r="B44" t="s">
-        <v>349</v>
-      </c>
-      <c r="C44" t="s">
-        <v>350</v>
-      </c>
-      <c r="D44" t="s">
-        <v>3</v>
-      </c>
-      <c r="E44" t="s">
-        <v>351</v>
-      </c>
-      <c r="F44" t="s">
-        <v>232</v>
-      </c>
-      <c r="G44" t="s">
-        <v>352</v>
-      </c>
-      <c r="H44" t="s">
-        <v>230</v>
-      </c>
-      <c r="I44">
-        <v>3.0928807413129855E-3</v>
-      </c>
-      <c r="J44">
-        <v>1.980262729617973E-2</v>
-      </c>
-      <c r="K44">
-        <v>1.7600222318099878E-2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>348</v>
-      </c>
-      <c r="B45" t="s">
-        <v>349</v>
-      </c>
-      <c r="C45" t="s">
-        <v>350</v>
-      </c>
-      <c r="D45" t="s">
-        <v>3</v>
-      </c>
-      <c r="E45" t="s">
-        <v>351</v>
-      </c>
-      <c r="F45" t="s">
-        <v>235</v>
-      </c>
-      <c r="G45" t="s">
-        <v>352</v>
-      </c>
-      <c r="H45" t="s">
-        <v>188</v>
-      </c>
-      <c r="I45">
-        <v>3.4610202407590472E-3</v>
-      </c>
-      <c r="J45">
-        <v>1.980262729617973E-2</v>
-      </c>
-      <c r="K45">
-        <v>1.7428378565682977E-2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
-        <v>348</v>
-      </c>
-      <c r="B46" t="s">
-        <v>349</v>
-      </c>
-      <c r="C46" t="s">
-        <v>350</v>
-      </c>
-      <c r="D46" t="s">
-        <v>3</v>
-      </c>
-      <c r="E46" t="s">
-        <v>351</v>
-      </c>
-      <c r="F46" t="s">
-        <v>237</v>
-      </c>
-      <c r="G46" t="s">
-        <v>352</v>
-      </c>
-      <c r="H46" t="s">
-        <v>188</v>
-      </c>
-      <c r="I46">
-        <v>3.4963252656081026E-3</v>
-      </c>
-      <c r="J46">
-        <v>9.950330853168092E-3</v>
-      </c>
-      <c r="K46">
-        <v>1.7600222318099878E-2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
-        <v>348</v>
-      </c>
-      <c r="B47" t="s">
-        <v>349</v>
-      </c>
-      <c r="C47" t="s">
-        <v>350</v>
-      </c>
-      <c r="D47" t="s">
-        <v>3</v>
-      </c>
-      <c r="E47" t="s">
-        <v>351</v>
-      </c>
-      <c r="F47" t="s">
-        <v>240</v>
-      </c>
-      <c r="G47" t="s">
-        <v>352</v>
-      </c>
-      <c r="H47" t="s">
-        <v>230</v>
-      </c>
-      <c r="I47">
-        <v>3.187050371155891E-3</v>
-      </c>
-      <c r="J47">
-        <v>2.9558802241544429E-2</v>
-      </c>
-      <c r="K47">
-        <v>1.9823720491662328E-2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
-        <v>348</v>
-      </c>
-      <c r="B48" t="s">
-        <v>349</v>
-      </c>
-      <c r="C48" t="s">
-        <v>350</v>
-      </c>
-      <c r="D48" t="s">
-        <v>3</v>
-      </c>
-      <c r="E48" t="s">
-        <v>351</v>
-      </c>
-      <c r="F48" t="s">
-        <v>243</v>
-      </c>
-      <c r="G48" t="s">
-        <v>352</v>
-      </c>
-      <c r="H48" t="s">
-        <v>245</v>
-      </c>
-      <c r="I48">
-        <v>3.0193108779371599E-3</v>
-      </c>
-      <c r="J48">
-        <v>9.950330853168092E-3</v>
-      </c>
-      <c r="K48">
-        <v>2.021667644238281E-2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
-        <v>348</v>
-      </c>
-      <c r="B49" t="s">
-        <v>349</v>
-      </c>
-      <c r="C49" t="s">
-        <v>350</v>
-      </c>
-      <c r="D49" t="s">
-        <v>3</v>
-      </c>
-      <c r="E49" t="s">
-        <v>351</v>
-      </c>
-      <c r="F49" t="s">
-        <v>246</v>
-      </c>
-      <c r="G49" t="s">
-        <v>352</v>
-      </c>
-      <c r="H49" t="s">
-        <v>245</v>
-      </c>
-      <c r="I49">
-        <v>3.071047346779402E-3</v>
-      </c>
-      <c r="J49">
-        <v>0</v>
-      </c>
-      <c r="K49">
-        <v>2.0419058079983801E-2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
-        <v>348</v>
-      </c>
-      <c r="B50" t="s">
-        <v>349</v>
-      </c>
-      <c r="C50" t="s">
-        <v>350</v>
-      </c>
-      <c r="D50" t="s">
-        <v>3</v>
-      </c>
-      <c r="E50" t="s">
-        <v>351</v>
-      </c>
-      <c r="F50" t="s">
-        <v>248</v>
-      </c>
-      <c r="G50" t="s">
-        <v>352</v>
-      </c>
-      <c r="H50" t="s">
-        <v>139</v>
-      </c>
-      <c r="I50">
-        <v>4.8409172195352148E-3</v>
-      </c>
-      <c r="J50">
-        <v>9.950330853168092E-3</v>
-      </c>
-      <c r="K50">
-        <v>3.0344883383001391E-2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
-        <v>348</v>
-      </c>
-      <c r="B51" t="s">
-        <v>349</v>
-      </c>
-      <c r="C51" t="s">
-        <v>350</v>
-      </c>
-      <c r="D51" t="s">
-        <v>3</v>
-      </c>
-      <c r="E51" t="s">
-        <v>351</v>
-      </c>
-      <c r="F51" t="s">
-        <v>252</v>
-      </c>
-      <c r="G51" t="s">
-        <v>352</v>
-      </c>
-      <c r="H51" t="s">
-        <v>245</v>
-      </c>
-      <c r="I51">
-        <v>3.1132498103861412E-3</v>
-      </c>
-      <c r="J51">
-        <v>-3.0459207484708574E-2</v>
-      </c>
-      <c r="K51">
-        <v>1.5784541764818246E-2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
-        <v>348</v>
-      </c>
-      <c r="B52" t="s">
-        <v>349</v>
-      </c>
-      <c r="C52" t="s">
-        <v>350</v>
-      </c>
-      <c r="D52" t="s">
-        <v>3</v>
-      </c>
-      <c r="E52" t="s">
-        <v>351</v>
-      </c>
-      <c r="F52" t="s">
-        <v>255</v>
-      </c>
-      <c r="G52" t="s">
-        <v>352</v>
-      </c>
-      <c r="H52" t="s">
-        <v>91</v>
-      </c>
-      <c r="I52">
-        <v>5.3679176144036979E-3</v>
-      </c>
-      <c r="J52">
-        <v>3.9220713153281329E-2</v>
-      </c>
-      <c r="K52">
-        <v>2.1984106183941941E-2</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
-        <v>348</v>
-      </c>
-      <c r="B53" t="s">
-        <v>349</v>
-      </c>
-      <c r="C53" t="s">
-        <v>350</v>
-      </c>
-      <c r="D53" t="s">
-        <v>3</v>
-      </c>
-      <c r="E53" t="s">
-        <v>351</v>
-      </c>
-      <c r="F53" t="s">
-        <v>259</v>
-      </c>
-      <c r="G53" t="s">
-        <v>352</v>
-      </c>
-      <c r="H53" t="s">
-        <v>91</v>
-      </c>
-      <c r="I53">
-        <v>5.3834551170713757E-3</v>
-      </c>
-      <c r="J53">
-        <v>-2.0202707317519466E-2</v>
-      </c>
-      <c r="K53">
-        <v>2.851821581329508E-2</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
-        <v>348</v>
-      </c>
-      <c r="B54" t="s">
-        <v>349</v>
-      </c>
-      <c r="C54" t="s">
-        <v>350</v>
-      </c>
-      <c r="D54" t="s">
-        <v>3</v>
-      </c>
-      <c r="E54" t="s">
-        <v>351</v>
-      </c>
-      <c r="F54" t="s">
-        <v>262</v>
-      </c>
-      <c r="G54" t="s">
-        <v>352</v>
-      </c>
-      <c r="H54" t="s">
-        <v>245</v>
-      </c>
-      <c r="I54">
-        <v>3.157964334726288E-3</v>
-      </c>
-      <c r="J54">
-        <v>0</v>
-      </c>
-      <c r="K54">
-        <v>1.7775489958670895E-2</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
-        <v>348</v>
-      </c>
-      <c r="B55" t="s">
-        <v>349</v>
-      </c>
-      <c r="C55" t="s">
-        <v>350</v>
-      </c>
-      <c r="D55" t="s">
-        <v>3</v>
-      </c>
-      <c r="E55" t="s">
-        <v>351</v>
-      </c>
-      <c r="F55" t="s">
-        <v>265</v>
-      </c>
-      <c r="G55" t="s">
-        <v>352</v>
-      </c>
-      <c r="H55" t="s">
-        <v>122</v>
-      </c>
-      <c r="I55">
-        <v>4.5724640231131859E-3</v>
-      </c>
-      <c r="J55">
-        <v>2.9558802241544429E-2</v>
-      </c>
-      <c r="K55">
-        <v>2.4786670523889762E-2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
-        <v>348</v>
-      </c>
-      <c r="B56" t="s">
-        <v>349</v>
-      </c>
-      <c r="C56" t="s">
-        <v>350</v>
-      </c>
-      <c r="D56" t="s">
-        <v>3</v>
-      </c>
-      <c r="E56" t="s">
-        <v>351</v>
-      </c>
-      <c r="F56" t="s">
-        <v>268</v>
-      </c>
-      <c r="G56" t="s">
-        <v>352</v>
-      </c>
-      <c r="H56" t="s">
-        <v>230</v>
-      </c>
-      <c r="I56">
-        <v>3.3414160168904051E-3</v>
-      </c>
-      <c r="J56">
-        <v>9.950330853168092E-3</v>
-      </c>
-      <c r="K56">
-        <v>2.021667644238281E-2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
-        <v>348</v>
-      </c>
-      <c r="B57" t="s">
-        <v>349</v>
-      </c>
-      <c r="C57" t="s">
-        <v>350</v>
-      </c>
-      <c r="D57" t="s">
-        <v>3</v>
-      </c>
-      <c r="E57" t="s">
-        <v>351</v>
-      </c>
-      <c r="F57" t="s">
-        <v>270</v>
-      </c>
-      <c r="G57" t="s">
-        <v>352</v>
-      </c>
-      <c r="H57" t="s">
-        <v>245</v>
-      </c>
-      <c r="I57">
-        <v>3.1792521978924546E-3</v>
-      </c>
-      <c r="J57">
-        <v>9.950330853168092E-3</v>
-      </c>
-      <c r="K57">
-        <v>1.7600222318099878E-2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
-        <v>348</v>
-      </c>
-      <c r="B58" t="s">
-        <v>349</v>
-      </c>
-      <c r="C58" t="s">
-        <v>350</v>
-      </c>
-      <c r="D58" t="s">
-        <v>3</v>
-      </c>
-      <c r="E58" t="s">
-        <v>351</v>
-      </c>
-      <c r="F58" t="s">
-        <v>273</v>
-      </c>
-      <c r="G58" t="s">
-        <v>352</v>
-      </c>
-      <c r="H58" t="s">
-        <v>230</v>
-      </c>
-      <c r="I58">
-        <v>3.3624599660399333E-3</v>
-      </c>
-      <c r="J58">
-        <v>-3.0459207484708574E-2</v>
-      </c>
-      <c r="K58">
-        <v>2.1051281553062108E-2</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
-        <v>348</v>
-      </c>
-      <c r="B59" t="s">
-        <v>349</v>
-      </c>
-      <c r="C59" t="s">
-        <v>350</v>
-      </c>
-      <c r="D59" t="s">
-        <v>3</v>
-      </c>
-      <c r="E59" t="s">
-        <v>351</v>
-      </c>
-      <c r="F59" t="s">
-        <v>276</v>
-      </c>
-      <c r="G59" t="s">
-        <v>352</v>
-      </c>
-      <c r="H59" t="s">
-        <v>278</v>
-      </c>
-      <c r="I59">
-        <v>3.0193538814245456E-3</v>
-      </c>
-      <c r="J59">
-        <v>0</v>
-      </c>
-      <c r="K59">
-        <v>1.7775489958670895E-2</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
-        <v>348</v>
-      </c>
-      <c r="B60" t="s">
-        <v>349</v>
-      </c>
-      <c r="C60" t="s">
-        <v>350</v>
-      </c>
-      <c r="D60" t="s">
-        <v>3</v>
-      </c>
-      <c r="E60" t="s">
-        <v>351</v>
-      </c>
-      <c r="F60" t="s">
-        <v>279</v>
-      </c>
-      <c r="G60" t="s">
-        <v>352</v>
-      </c>
-      <c r="H60" t="s">
-        <v>278</v>
-      </c>
-      <c r="I60">
-        <v>3.0243671843956333E-3</v>
-      </c>
-      <c r="J60">
-        <v>1.980262729617973E-2</v>
-      </c>
-      <c r="K60">
-        <v>1.7428378565682977E-2</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A61" t="s">
-        <v>348</v>
-      </c>
-      <c r="B61" t="s">
-        <v>349</v>
-      </c>
-      <c r="C61" t="s">
-        <v>350</v>
-      </c>
-      <c r="D61" t="s">
-        <v>3</v>
-      </c>
-      <c r="E61" t="s">
-        <v>351</v>
-      </c>
-      <c r="F61" t="s">
-        <v>282</v>
-      </c>
-      <c r="G61" t="s">
-        <v>352</v>
-      </c>
-      <c r="H61" t="s">
-        <v>91</v>
-      </c>
-      <c r="I61">
-        <v>5.5237368363655111E-3</v>
-      </c>
-      <c r="J61">
-        <v>4.8790164169432049E-2</v>
-      </c>
-      <c r="K61">
-        <v>2.9186314075955181E-2</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A62" t="s">
-        <v>348</v>
-      </c>
-      <c r="B62" t="s">
-        <v>349</v>
-      </c>
-      <c r="C62" t="s">
-        <v>350</v>
-      </c>
-      <c r="D62" t="s">
-        <v>3</v>
-      </c>
-      <c r="E62" t="s">
-        <v>351</v>
-      </c>
-      <c r="F62" t="s">
-        <v>287</v>
-      </c>
-      <c r="G62" t="s">
-        <v>352</v>
-      </c>
-      <c r="H62" t="s">
-        <v>152</v>
-      </c>
-      <c r="I62">
-        <v>4.4739424041467394E-3</v>
-      </c>
-      <c r="J62">
-        <v>1.980262729617973E-2</v>
-      </c>
-      <c r="K62">
-        <v>3.0046692769485604E-2</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A63" t="s">
-        <v>348</v>
-      </c>
-      <c r="B63" t="s">
-        <v>349</v>
-      </c>
-      <c r="C63" t="s">
-        <v>350</v>
-      </c>
-      <c r="D63" t="s">
-        <v>3</v>
-      </c>
-      <c r="E63" t="s">
-        <v>351</v>
-      </c>
-      <c r="F63" t="s">
-        <v>291</v>
-      </c>
-      <c r="G63" t="s">
-        <v>352</v>
-      </c>
-      <c r="H63" t="s">
-        <v>245</v>
-      </c>
-      <c r="I63">
-        <v>3.2255089532494787E-3</v>
-      </c>
-      <c r="J63">
-        <v>0</v>
-      </c>
-      <c r="K63">
-        <v>1.7775489958670895E-2</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A64" t="s">
-        <v>348</v>
-      </c>
-      <c r="B64" t="s">
-        <v>349</v>
-      </c>
-      <c r="C64" t="s">
-        <v>350</v>
-      </c>
-      <c r="D64" t="s">
-        <v>3</v>
-      </c>
-      <c r="E64" t="s">
-        <v>351</v>
-      </c>
-      <c r="F64" t="s">
-        <v>293</v>
-      </c>
-      <c r="G64" t="s">
-        <v>352</v>
-      </c>
-      <c r="H64" t="s">
-        <v>230</v>
-      </c>
-      <c r="I64">
-        <v>3.413229426799249E-3</v>
-      </c>
-      <c r="J64">
-        <v>0</v>
-      </c>
-      <c r="K64">
-        <v>1.795428488821418E-2</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A65" t="s">
-        <v>348</v>
-      </c>
-      <c r="B65" t="s">
-        <v>349</v>
-      </c>
-      <c r="C65" t="s">
-        <v>350</v>
-      </c>
-      <c r="D65" t="s">
-        <v>3</v>
-      </c>
-      <c r="E65" t="s">
-        <v>351</v>
-      </c>
-      <c r="F65" t="s">
-        <v>296</v>
-      </c>
-      <c r="G65" t="s">
-        <v>352</v>
-      </c>
-      <c r="H65" t="s">
-        <v>278</v>
-      </c>
-      <c r="I65">
-        <v>3.0575583491919659E-3</v>
-      </c>
-      <c r="J65">
-        <v>1.980262729617973E-2</v>
-      </c>
-      <c r="K65">
-        <v>1.7600222318099878E-2</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A66" t="s">
-        <v>348</v>
-      </c>
-      <c r="B66" t="s">
-        <v>349</v>
-      </c>
-      <c r="C66" t="s">
-        <v>350</v>
-      </c>
-      <c r="D66" t="s">
-        <v>3</v>
-      </c>
-      <c r="E66" t="s">
-        <v>351</v>
-      </c>
-      <c r="F66" t="s">
-        <v>300</v>
-      </c>
-      <c r="G66" t="s">
-        <v>352</v>
-      </c>
-      <c r="H66" t="s">
-        <v>201</v>
-      </c>
-      <c r="I66">
-        <v>3.609083481225025E-3</v>
-      </c>
-      <c r="J66">
-        <v>2.9558802241544429E-2</v>
-      </c>
-      <c r="K66">
-        <v>1.9823720491662328E-2</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A67" t="s">
-        <v>348</v>
-      </c>
-      <c r="B67" t="s">
-        <v>349</v>
-      </c>
-      <c r="C67" t="s">
-        <v>350</v>
-      </c>
-      <c r="D67" t="s">
-        <v>3</v>
-      </c>
-      <c r="E67" t="s">
-        <v>351</v>
-      </c>
-      <c r="F67" t="s">
-        <v>303</v>
-      </c>
-      <c r="G67" t="s">
-        <v>352</v>
-      </c>
-      <c r="H67" t="s">
-        <v>51</v>
-      </c>
-      <c r="I67">
-        <v>7.21816696245005E-3</v>
-      </c>
-      <c r="J67">
-        <v>5.8268908123975824E-2</v>
-      </c>
-      <c r="K67">
-        <v>4.0807308595070944E-2</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A68" t="s">
-        <v>348</v>
-      </c>
-      <c r="B68" t="s">
-        <v>349</v>
-      </c>
-      <c r="C68" t="s">
-        <v>350</v>
-      </c>
-      <c r="D68" t="s">
-        <v>3</v>
-      </c>
-      <c r="E68" t="s">
-        <v>351</v>
-      </c>
-      <c r="F68" t="s">
-        <v>308</v>
-      </c>
-      <c r="G68" t="s">
-        <v>352</v>
-      </c>
-      <c r="H68" t="s">
-        <v>230</v>
-      </c>
-      <c r="I68">
-        <v>3.4422677991651496E-3</v>
-      </c>
-      <c r="J68">
-        <v>1.980262729617973E-2</v>
-      </c>
-      <c r="K68">
-        <v>2.0018269245279413E-2</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A69" t="s">
-        <v>348</v>
-      </c>
-      <c r="B69" t="s">
-        <v>349</v>
-      </c>
-      <c r="C69" t="s">
-        <v>350</v>
-      </c>
-      <c r="D69" t="s">
-        <v>3</v>
-      </c>
-      <c r="E69" t="s">
-        <v>351</v>
-      </c>
-      <c r="F69" t="s">
-        <v>312</v>
-      </c>
-      <c r="G69" t="s">
-        <v>352</v>
-      </c>
-      <c r="H69" t="s">
-        <v>160</v>
-      </c>
-      <c r="I69">
-        <v>4.0033087284456915E-3</v>
-      </c>
-      <c r="J69">
-        <v>-1.0050335853501451E-2</v>
-      </c>
-      <c r="K69">
-        <v>2.3090308046130589E-2</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A70" t="s">
-        <v>348</v>
-      </c>
-      <c r="B70" t="s">
-        <v>349</v>
-      </c>
-      <c r="C70" t="s">
-        <v>350</v>
-      </c>
-      <c r="D70" t="s">
-        <v>3</v>
-      </c>
-      <c r="E70" t="s">
-        <v>351</v>
-      </c>
-      <c r="F70" t="s">
-        <v>316</v>
-      </c>
-      <c r="G70" t="s">
-        <v>352</v>
-      </c>
-      <c r="H70" t="s">
-        <v>278</v>
-      </c>
-      <c r="I70">
-        <v>3.1008536966410077E-3</v>
-      </c>
-      <c r="J70">
-        <v>0</v>
-      </c>
-      <c r="K70">
-        <v>2.0419058079983801E-2</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A71" t="s">
-        <v>348</v>
-      </c>
-      <c r="B71" t="s">
-        <v>349</v>
-      </c>
-      <c r="C71" t="s">
-        <v>350</v>
-      </c>
-      <c r="D71" t="s">
-        <v>3</v>
-      </c>
-      <c r="E71" t="s">
-        <v>351</v>
-      </c>
-      <c r="F71" t="s">
-        <v>319</v>
-      </c>
-      <c r="G71" t="s">
-        <v>352</v>
-      </c>
-      <c r="H71" t="s">
-        <v>230</v>
-      </c>
-      <c r="I71">
-        <v>3.4830228110857933E-3</v>
-      </c>
-      <c r="J71">
-        <v>0</v>
-      </c>
-      <c r="K71">
-        <v>2.0419058079983801E-2</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Transferring Intro/Methods/Appendix to Bookdown
</commit_message>
<xml_diff>
--- a/MSc_Thesis/MSc_Thesis_Split/Data/Citations_Datasets/mokry_obesity_2016.xlsx
+++ b/MSc_Thesis/MSc_Thesis_Split/Data/Citations_Datasets/mokry_obesity_2016.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4f99f7067dc2a9a5/Documents/R/Working Directory/Data_Science_MSc/Dissertation_Bayes_MR/MSc_Thesis/MSc_Thesis_Split/Data/Citations_Datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{22C4E43D-6371-4515-9FCB-E71DF9F4DBB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4F584BA-4AD1-4B06-BBDC-BB0F4958DBBE}"/>
+  <xr:revisionPtr revIDLastSave="39" documentId="8_{22C4E43D-6371-4515-9FCB-E71DF9F4DBB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A93F10F-09D3-4F31-BA50-4CB9BFD7CF3F}"/>
   <bookViews>
-    <workbookView xWindow="12710" yWindow="0" windowWidth="12980" windowHeight="15370" xr2:uid="{8A3BB852-7168-48D5-AFAC-CE153936FD9B}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="12980" windowHeight="15370" activeTab="1" xr2:uid="{8A3BB852-7168-48D5-AFAC-CE153936FD9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Table004 (Page 7-8)" sheetId="2" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1309" uniqueCount="353">
   <si>
     <t>BMI-Associated</t>
   </si>
@@ -1056,13 +1056,67 @@
   </si>
   <si>
     <t>Upp_CI</t>
+  </si>
+  <si>
+    <t>SE_Lower_Only</t>
+  </si>
+  <si>
+    <t>SE_Both</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>Study_Ref</t>
+  </si>
+  <si>
+    <t>Study_DOI</t>
+  </si>
+  <si>
+    <t>Exposure</t>
+  </si>
+  <si>
+    <t>Outcome</t>
+  </si>
+  <si>
+    <t>Instrument</t>
+  </si>
+  <si>
+    <t>Reported_Measure</t>
+  </si>
+  <si>
+    <t>Coeff_G_X</t>
+  </si>
+  <si>
+    <t>Coeff_G_X_SE</t>
+  </si>
+  <si>
+    <t>Coeff_G_Y</t>
+  </si>
+  <si>
+    <t>Coeff_G_Y_SE</t>
+  </si>
+  <si>
+    <t>Mokry et al</t>
+  </si>
+  <si>
+    <t>[@mokry_obesity_2016]</t>
+  </si>
+  <si>
+    <t>10.1371/journal.pmed.1002053</t>
+  </si>
+  <si>
+    <t>Multiple Sclerosis</t>
+  </si>
+  <si>
+    <t>OR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1074,6 +1128,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1154,6 +1214,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1521,10 +1585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17ADCFF7-C1EB-4801-B550-02DC019036B8}">
-  <dimension ref="A1:AB72"/>
+  <dimension ref="A1:AD72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB3" sqref="AB3:AB72"/>
+    <sheetView topLeftCell="T2" workbookViewId="0">
+      <selection activeCell="AC72" sqref="AC3:AC72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1545,7 +1609,7 @@
     <col min="15" max="15" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1604,7 +1668,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -1657,10 +1721,13 @@
         <v>334</v>
       </c>
       <c r="AB2" s="1" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.35">
+        <v>335</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -1743,8 +1810,16 @@
         <f>(Y3-Z3)/1.96</f>
         <v>1.5540411981994171E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC3">
+        <f>(AA3-Z3)/2/1.96</f>
+        <v>1.7775489958670895E-2</v>
+      </c>
+      <c r="AD3">
+        <f>(AA3-Y3)/1.96</f>
+        <v>2.0010567935347619E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -1827,8 +1902,16 @@
         <f t="shared" ref="AB4:AB67" si="3">(Y4-Z4)/1.96</f>
         <v>2.0827548224619984E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC4">
+        <f t="shared" ref="AC4:AC67" si="4">(AA4-Z4)/2/1.96</f>
+        <v>2.0419058079983801E-2</v>
+      </c>
+      <c r="AD4">
+        <f t="shared" ref="AD4:AD67" si="5">(AA4-Y4)/1.96</f>
+        <v>2.0010567935347619E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -1911,8 +1994,16 @@
         <f t="shared" si="3"/>
         <v>1.9816241487889776E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC5">
+        <f t="shared" si="4"/>
+        <v>2.1775471671213478E-2</v>
+      </c>
+      <c r="AD5">
+        <f t="shared" si="5"/>
+        <v>2.3734701854537188E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>48</v>
       </c>
@@ -1995,8 +2086,16 @@
         <f t="shared" si="3"/>
         <v>1.5231103647796521E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC6">
+        <f t="shared" si="4"/>
+        <v>1.5010331638503445E-2</v>
+      </c>
+      <c r="AD6">
+        <f t="shared" si="5"/>
+        <v>1.4789559629210367E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>55</v>
       </c>
@@ -2079,8 +2178,16 @@
         <f t="shared" si="3"/>
         <v>2.0827548224619984E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC7">
+        <f t="shared" si="4"/>
+        <v>2.286024456369572E-2</v>
+      </c>
+      <c r="AD7">
+        <f t="shared" si="5"/>
+        <v>2.4892940902771454E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>62</v>
       </c>
@@ -2163,8 +2270,16 @@
         <f t="shared" si="3"/>
         <v>2.5138290309583051E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC8">
+        <f t="shared" si="4"/>
+        <v>2.219677984429333E-2</v>
+      </c>
+      <c r="AD8">
+        <f t="shared" si="5"/>
+        <v>1.9255269379003605E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>69</v>
       </c>
@@ -2247,8 +2362,16 @@
         <f t="shared" si="3"/>
         <v>2.0208743926043816E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC9">
+        <f t="shared" si="4"/>
+        <v>2.219677984429333E-2</v>
+      </c>
+      <c r="AD9">
+        <f t="shared" si="5"/>
+        <v>2.418481576254284E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>74</v>
       </c>
@@ -2331,8 +2454,16 @@
         <f t="shared" si="3"/>
         <v>1.5699825850384548E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC10">
+        <f t="shared" si="4"/>
+        <v>1.795428488821418E-2</v>
+      </c>
+      <c r="AD10">
+        <f t="shared" si="5"/>
+        <v>2.0208743926043816E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>81</v>
       </c>
@@ -2415,8 +2546,16 @@
         <f t="shared" si="3"/>
         <v>2.0410885006989385E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC11">
+        <f t="shared" si="4"/>
+        <v>2.0018269245279413E-2</v>
+      </c>
+      <c r="AD11">
+        <f t="shared" si="5"/>
+        <v>1.9625653483569438E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>88</v>
       </c>
@@ -2499,8 +2638,16 @@
         <f t="shared" si="3"/>
         <v>1.9625653483569438E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC12">
+        <f t="shared" si="4"/>
+        <v>1.6932415547161402E-2</v>
+      </c>
+      <c r="AD12">
+        <f t="shared" si="5"/>
+        <v>1.4239177610753362E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>95</v>
       </c>
@@ -2583,8 +2730,16 @@
         <f t="shared" si="3"/>
         <v>2.0617111396875849E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC13">
+        <f t="shared" si="4"/>
+        <v>1.7775489958670895E-2</v>
+      </c>
+      <c r="AD13">
+        <f t="shared" si="5"/>
+        <v>1.4933868520465937E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>99</v>
       </c>
@@ -2667,8 +2822,16 @@
         <f t="shared" si="3"/>
         <v>2.5643793255555259E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC14">
+        <f t="shared" si="4"/>
+        <v>2.7403124648172694E-2</v>
+      </c>
+      <c r="AD14">
+        <f t="shared" si="5"/>
+        <v>2.9162456040790135E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>103</v>
       </c>
@@ -2751,8 +2914,16 @@
         <f t="shared" si="3"/>
         <v>2.9729034757130523E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC15">
+        <f t="shared" si="4"/>
+        <v>2.8910378904847774E-2</v>
+      </c>
+      <c r="AD15">
+        <f t="shared" si="5"/>
+        <v>2.8091723052565024E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>108</v>
       </c>
@@ -2835,8 +3006,16 @@
         <f t="shared" si="3"/>
         <v>2.4892940902771454E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC16">
+        <f t="shared" si="4"/>
+        <v>2.1984106183941941E-2</v>
+      </c>
+      <c r="AD16">
+        <f t="shared" si="5"/>
+        <v>1.9075271465112429E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>113</v>
       </c>
@@ -2919,8 +3098,16 @@
         <f t="shared" si="3"/>
         <v>2.1042325782678128E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC17">
+        <f t="shared" si="4"/>
+        <v>2.0625534854360972E-2</v>
+      </c>
+      <c r="AD17">
+        <f t="shared" si="5"/>
+        <v>2.0208743926043816E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>120</v>
       </c>
@@ -3003,8 +3190,16 @@
         <f t="shared" si="3"/>
         <v>1.6028671547642325E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC18">
+        <f t="shared" si="4"/>
+        <v>1.832289147225909E-2</v>
+      </c>
+      <c r="AD18">
+        <f t="shared" si="5"/>
+        <v>2.0617111396875849E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>126</v>
       </c>
@@ -3087,8 +3282,16 @@
         <f t="shared" si="3"/>
         <v>2.0410885006989385E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC19">
+        <f t="shared" si="4"/>
+        <v>1.7600222318099878E-2</v>
+      </c>
+      <c r="AD19">
+        <f t="shared" si="5"/>
+        <v>1.4789559629210367E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>130</v>
       </c>
@@ -3171,8 +3374,16 @@
         <f t="shared" si="3"/>
         <v>1.5699825850384548E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC20">
+        <f t="shared" si="4"/>
+        <v>1.795428488821418E-2</v>
+      </c>
+      <c r="AD20">
+        <f t="shared" si="5"/>
+        <v>2.0208743926043816E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>136</v>
       </c>
@@ -3255,8 +3466,16 @@
         <f t="shared" si="3"/>
         <v>1.6028671547642325E-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC21">
+        <f t="shared" si="4"/>
+        <v>1.832289147225909E-2</v>
+      </c>
+      <c r="AD21">
+        <f t="shared" si="5"/>
+        <v>2.0617111396875849E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>141</v>
       </c>
@@ -3339,8 +3558,16 @@
         <f t="shared" si="3"/>
         <v>1.5231103647796521E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC22">
+        <f t="shared" si="4"/>
+        <v>1.7428378565682977E-2</v>
+      </c>
+      <c r="AD22">
+        <f t="shared" si="5"/>
+        <v>1.9625653483569438E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>144</v>
       </c>
@@ -3423,8 +3650,16 @@
         <f t="shared" si="3"/>
         <v>2.1042325782678128E-2</v>
       </c>
-    </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC23">
+        <f t="shared" si="4"/>
+        <v>2.3090308046130589E-2</v>
+      </c>
+      <c r="AD23">
+        <f t="shared" si="5"/>
+        <v>2.5138290309583051E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>149</v>
       </c>
@@ -3507,8 +3742,16 @@
         <f t="shared" si="3"/>
         <v>2.0617111396875849E-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC24">
+        <f t="shared" si="4"/>
+        <v>2.021667644238281E-2</v>
+      </c>
+      <c r="AD24">
+        <f t="shared" si="5"/>
+        <v>1.9816241487889776E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>154</v>
       </c>
@@ -3591,8 +3834,16 @@
         <f t="shared" si="3"/>
         <v>2.5904247639501662E-2</v>
       </c>
-    </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC25">
+        <f t="shared" si="4"/>
+        <v>2.5278291490875252E-2</v>
+      </c>
+      <c r="AD25">
+        <f t="shared" si="5"/>
+        <v>2.4652335342248845E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>157</v>
       </c>
@@ -3675,8 +3926,16 @@
         <f t="shared" si="3"/>
         <v>2.1042325782678128E-2</v>
       </c>
-    </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC26">
+        <f t="shared" si="4"/>
+        <v>2.0625534854360972E-2</v>
+      </c>
+      <c r="AD26">
+        <f t="shared" si="5"/>
+        <v>2.0208743926043816E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>163</v>
       </c>
@@ -3759,8 +4018,16 @@
         <f t="shared" si="3"/>
         <v>2.0617111396875849E-2</v>
       </c>
-    </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC27">
+        <f t="shared" si="4"/>
+        <v>2.021667644238281E-2</v>
+      </c>
+      <c r="AD27">
+        <f t="shared" si="5"/>
+        <v>1.9816241487889776E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>166</v>
       </c>
@@ -3843,8 +4110,16 @@
         <f t="shared" si="3"/>
         <v>1.586254442348526E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC28">
+        <f t="shared" si="4"/>
+        <v>1.8136714715237322E-2</v>
+      </c>
+      <c r="AD28">
+        <f t="shared" si="5"/>
+        <v>2.0410885006989385E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>171</v>
       </c>
@@ -3927,8 +4202,16 @@
         <f t="shared" si="3"/>
         <v>2.0827548224619984E-2</v>
       </c>
-    </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC29">
+        <f t="shared" si="4"/>
+        <v>1.795428488821418E-2</v>
+      </c>
+      <c r="AD29">
+        <f t="shared" si="5"/>
+        <v>1.5081021551808382E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>176</v>
       </c>
@@ -4011,8 +4294,16 @@
         <f t="shared" si="3"/>
         <v>2.1042325782678128E-2</v>
       </c>
-    </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC30">
+        <f t="shared" si="4"/>
+        <v>2.0625534854360972E-2</v>
+      </c>
+      <c r="AD30">
+        <f t="shared" si="5"/>
+        <v>2.0208743926043816E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>180</v>
       </c>
@@ -4095,8 +4386,16 @@
         <f t="shared" si="3"/>
         <v>2.0208743926043816E-2</v>
       </c>
-    </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC31">
+        <f t="shared" si="4"/>
+        <v>1.9823720491662328E-2</v>
+      </c>
+      <c r="AD31">
+        <f t="shared" si="5"/>
+        <v>1.9438697057280834E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>185</v>
       </c>
@@ -4179,8 +4478,16 @@
         <f t="shared" si="3"/>
         <v>2.1042325782678128E-2</v>
       </c>
-    </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC32">
+        <f t="shared" si="4"/>
+        <v>2.0625534854360972E-2</v>
+      </c>
+      <c r="AD32">
+        <f t="shared" si="5"/>
+        <v>2.0208743926043816E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>190</v>
       </c>
@@ -4263,8 +4570,16 @@
         <f t="shared" si="3"/>
         <v>2.0617111396875849E-2</v>
       </c>
-    </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC33">
+        <f t="shared" si="4"/>
+        <v>2.2634723369562348E-2</v>
+      </c>
+      <c r="AD33">
+        <f t="shared" si="5"/>
+        <v>2.4652335342248845E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>193</v>
       </c>
@@ -4347,8 +4662,16 @@
         <f t="shared" si="3"/>
         <v>2.0617111396875849E-2</v>
       </c>
-    </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC34">
+        <f t="shared" si="4"/>
+        <v>1.7775489958670895E-2</v>
+      </c>
+      <c r="AD34">
+        <f t="shared" si="5"/>
+        <v>1.4933868520465937E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>196</v>
       </c>
@@ -4431,8 +4754,16 @@
         <f t="shared" si="3"/>
         <v>2.0410885006989385E-2</v>
       </c>
-    </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC35">
+        <f t="shared" si="4"/>
+        <v>2.2413611171258761E-2</v>
+      </c>
+      <c r="AD35">
+        <f t="shared" si="5"/>
+        <v>2.4416337335528129E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>199</v>
       </c>
@@ -4515,8 +4846,16 @@
         <f t="shared" si="3"/>
         <v>2.1261579796208196E-2</v>
       </c>
-    </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC36">
+        <f t="shared" si="4"/>
+        <v>2.0836232401598792E-2</v>
+      </c>
+      <c r="AD36">
+        <f t="shared" si="5"/>
+        <v>2.0410885006989385E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>203</v>
       </c>
@@ -4599,8 +4938,16 @@
         <f t="shared" si="3"/>
         <v>2.0617111396875849E-2</v>
       </c>
-    </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC37">
+        <f t="shared" si="4"/>
+        <v>2.021667644238281E-2</v>
+      </c>
+      <c r="AD37">
+        <f t="shared" si="5"/>
+        <v>1.9816241487889776E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>207</v>
       </c>
@@ -4683,8 +5030,16 @@
         <f t="shared" si="3"/>
         <v>2.0208743926043816E-2</v>
       </c>
-    </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC38">
+        <f t="shared" si="4"/>
+        <v>1.9823720491662328E-2</v>
+      </c>
+      <c r="AD38">
+        <f t="shared" si="5"/>
+        <v>1.9438697057280834E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>211</v>
       </c>
@@ -4767,8 +5122,16 @@
         <f t="shared" si="3"/>
         <v>1.5384203148309978E-2</v>
       </c>
-    </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC39">
+        <f t="shared" si="4"/>
+        <v>1.7600222318099878E-2</v>
+      </c>
+      <c r="AD39">
+        <f t="shared" si="5"/>
+        <v>1.9816241487889776E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>215</v>
       </c>
@@ -4851,8 +5214,16 @@
         <f t="shared" si="3"/>
         <v>2.0617111396875849E-2</v>
       </c>
-    </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC40">
+        <f t="shared" si="4"/>
+        <v>2.2634723369562348E-2</v>
+      </c>
+      <c r="AD40">
+        <f t="shared" si="5"/>
+        <v>2.4652335342248845E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>218</v>
       </c>
@@ -4935,8 +5306,16 @@
         <f t="shared" si="3"/>
         <v>3.6273429430474645E-2</v>
       </c>
-    </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC41">
+        <f t="shared" si="4"/>
+        <v>3.5069130262398725E-2</v>
+      </c>
+      <c r="AD41">
+        <f t="shared" si="5"/>
+        <v>3.3864831094322805E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>222</v>
       </c>
@@ -5019,8 +5398,16 @@
         <f t="shared" si="3"/>
         <v>1.5540411981994171E-2</v>
       </c>
-    </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC42">
+        <f t="shared" si="4"/>
+        <v>1.7775489958670895E-2</v>
+      </c>
+      <c r="AD42">
+        <f t="shared" si="5"/>
+        <v>2.0010567935347619E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>226</v>
       </c>
@@ -5103,8 +5490,16 @@
         <f t="shared" si="3"/>
         <v>2.0208743926043816E-2</v>
       </c>
-    </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC43">
+        <f t="shared" si="4"/>
+        <v>1.9823720491662328E-2</v>
+      </c>
+      <c r="AD43">
+        <f t="shared" si="5"/>
+        <v>1.9438697057280834E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>228</v>
       </c>
@@ -5187,8 +5582,16 @@
         <f t="shared" si="3"/>
         <v>1.5231103647796521E-2</v>
       </c>
-    </row>
-    <row r="45" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC44">
+        <f t="shared" si="4"/>
+        <v>1.7428378565682977E-2</v>
+      </c>
+      <c r="AD44">
+        <f t="shared" si="5"/>
+        <v>1.9625653483569438E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>232</v>
       </c>
@@ -5271,8 +5674,16 @@
         <f t="shared" si="3"/>
         <v>2.0410885006989385E-2</v>
       </c>
-    </row>
-    <row r="46" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC45">
+        <f t="shared" si="4"/>
+        <v>1.7600222318099878E-2</v>
+      </c>
+      <c r="AD45">
+        <f t="shared" si="5"/>
+        <v>1.4789559629210367E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>235</v>
       </c>
@@ -5355,8 +5766,16 @@
         <f t="shared" si="3"/>
         <v>1.5231103647796521E-2</v>
       </c>
-    </row>
-    <row r="47" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC46">
+        <f t="shared" si="4"/>
+        <v>1.7428378565682977E-2</v>
+      </c>
+      <c r="AD46">
+        <f t="shared" si="5"/>
+        <v>1.9625653483569438E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>237</v>
       </c>
@@ -5439,8 +5858,16 @@
         <f t="shared" si="3"/>
         <v>1.5384203148309978E-2</v>
       </c>
-    </row>
-    <row r="48" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC47">
+        <f t="shared" si="4"/>
+        <v>1.7600222318099878E-2</v>
+      </c>
+      <c r="AD47">
+        <f t="shared" si="5"/>
+        <v>1.9816241487889776E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>240</v>
       </c>
@@ -5523,8 +5950,16 @@
         <f t="shared" si="3"/>
         <v>2.0208743926043816E-2</v>
       </c>
-    </row>
-    <row r="49" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC48">
+        <f t="shared" si="4"/>
+        <v>1.9823720491662328E-2</v>
+      </c>
+      <c r="AD48">
+        <f t="shared" si="5"/>
+        <v>1.9438697057280834E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>243</v>
       </c>
@@ -5607,8 +6042,16 @@
         <f t="shared" si="3"/>
         <v>2.0617111396875849E-2</v>
       </c>
-    </row>
-    <row r="50" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC49">
+        <f t="shared" si="4"/>
+        <v>2.021667644238281E-2</v>
+      </c>
+      <c r="AD49">
+        <f t="shared" si="5"/>
+        <v>1.9816241487889776E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>246</v>
       </c>
@@ -5691,8 +6134,16 @@
         <f t="shared" si="3"/>
         <v>2.0827548224619984E-2</v>
       </c>
-    </row>
-    <row r="51" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC50">
+        <f t="shared" si="4"/>
+        <v>2.0419058079983801E-2</v>
+      </c>
+      <c r="AD50">
+        <f t="shared" si="5"/>
+        <v>2.0010567935347619E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>248</v>
       </c>
@@ -5775,8 +6226,16 @@
         <f t="shared" si="3"/>
         <v>3.1246747571795241E-2</v>
       </c>
-    </row>
-    <row r="52" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC51">
+        <f t="shared" si="4"/>
+        <v>3.0344883383001391E-2</v>
+      </c>
+      <c r="AD51">
+        <f t="shared" si="5"/>
+        <v>2.9443019194207536E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>252</v>
       </c>
@@ -5859,8 +6318,16 @@
         <f t="shared" si="3"/>
         <v>1.6028671547642325E-2</v>
       </c>
-    </row>
-    <row r="53" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC52">
+        <f t="shared" si="4"/>
+        <v>1.5784541764818246E-2</v>
+      </c>
+      <c r="AD52">
+        <f t="shared" si="5"/>
+        <v>1.5540411981994171E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>255</v>
       </c>
@@ -5943,8 +6410,16 @@
         <f t="shared" si="3"/>
         <v>2.0010567935347619E-2</v>
       </c>
-    </row>
-    <row r="54" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC53">
+        <f t="shared" si="4"/>
+        <v>2.1984106183941941E-2</v>
+      </c>
+      <c r="AD53">
+        <f t="shared" si="5"/>
+        <v>2.3957644432536267E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>259</v>
       </c>
@@ -6027,8 +6502,16 @@
         <f t="shared" si="3"/>
         <v>2.6718359957814238E-2</v>
       </c>
-    </row>
-    <row r="55" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC54">
+        <f t="shared" si="4"/>
+        <v>2.851821581329508E-2</v>
+      </c>
+      <c r="AD54">
+        <f t="shared" si="5"/>
+        <v>3.0318071668775915E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>262</v>
       </c>
@@ -6111,8 +6594,16 @@
         <f t="shared" si="3"/>
         <v>1.5540411981994171E-2</v>
       </c>
-    </row>
-    <row r="56" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC55">
+        <f t="shared" si="4"/>
+        <v>1.7775489958670895E-2</v>
+      </c>
+      <c r="AD55">
+        <f t="shared" si="5"/>
+        <v>2.0010567935347619E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>265</v>
       </c>
@@ -6195,8 +6686,16 @@
         <f t="shared" si="3"/>
         <v>2.538852528523668E-2</v>
       </c>
-    </row>
-    <row r="57" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC56">
+        <f t="shared" si="4"/>
+        <v>2.4786670523889762E-2</v>
+      </c>
+      <c r="AD56">
+        <f t="shared" si="5"/>
+        <v>2.418481576254284E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>268</v>
       </c>
@@ -6279,8 +6778,16 @@
         <f t="shared" si="3"/>
         <v>2.0617111396875849E-2</v>
       </c>
-    </row>
-    <row r="58" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC57">
+        <f t="shared" si="4"/>
+        <v>2.021667644238281E-2</v>
+      </c>
+      <c r="AD57">
+        <f t="shared" si="5"/>
+        <v>1.9816241487889776E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>270</v>
       </c>
@@ -6363,8 +6870,16 @@
         <f t="shared" si="3"/>
         <v>1.5384203148309978E-2</v>
       </c>
-    </row>
-    <row r="59" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC58">
+        <f t="shared" si="4"/>
+        <v>1.7600222318099878E-2</v>
+      </c>
+      <c r="AD58">
+        <f t="shared" si="5"/>
+        <v>1.9816241487889776E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>273</v>
       </c>
@@ -6447,8 +6962,16 @@
         <f t="shared" si="3"/>
         <v>2.1485451709248368E-2</v>
       </c>
-    </row>
-    <row r="60" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC59">
+        <f t="shared" si="4"/>
+        <v>2.1051281553062108E-2</v>
+      </c>
+      <c r="AD59">
+        <f t="shared" si="5"/>
+        <v>2.0617111396875849E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>276</v>
       </c>
@@ -6531,8 +7054,16 @@
         <f t="shared" si="3"/>
         <v>1.5540411981994171E-2</v>
       </c>
-    </row>
-    <row r="61" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC60">
+        <f t="shared" si="4"/>
+        <v>1.7775489958670895E-2</v>
+      </c>
+      <c r="AD60">
+        <f t="shared" si="5"/>
+        <v>2.0010567935347619E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>279</v>
       </c>
@@ -6615,8 +7146,16 @@
         <f t="shared" si="3"/>
         <v>1.5231103647796521E-2</v>
       </c>
-    </row>
-    <row r="62" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC61">
+        <f t="shared" si="4"/>
+        <v>1.7428378565682977E-2</v>
+      </c>
+      <c r="AD61">
+        <f t="shared" si="5"/>
+        <v>1.9625653483569438E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>282</v>
       </c>
@@ -6699,8 +7238,16 @@
         <f t="shared" si="3"/>
         <v>3.0020663277006889E-2</v>
       </c>
-    </row>
-    <row r="63" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC62">
+        <f t="shared" si="4"/>
+        <v>2.9186314075955181E-2</v>
+      </c>
+      <c r="AD62">
+        <f t="shared" si="5"/>
+        <v>2.8351964874903473E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>287</v>
       </c>
@@ -6783,8 +7330,16 @@
         <f t="shared" si="3"/>
         <v>3.0930929498181069E-2</v>
       </c>
-    </row>
-    <row r="64" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC63">
+        <f t="shared" si="4"/>
+        <v>3.0046692769485604E-2</v>
+      </c>
+      <c r="AD63">
+        <f t="shared" si="5"/>
+        <v>2.9162456040790135E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>291</v>
       </c>
@@ -6867,8 +7422,16 @@
         <f t="shared" si="3"/>
         <v>1.5540411981994171E-2</v>
       </c>
-    </row>
-    <row r="65" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC64">
+        <f t="shared" si="4"/>
+        <v>1.7775489958670895E-2</v>
+      </c>
+      <c r="AD64">
+        <f t="shared" si="5"/>
+        <v>2.0010567935347619E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>293</v>
       </c>
@@ -6951,8 +7514,16 @@
         <f t="shared" si="3"/>
         <v>2.0827548224619984E-2</v>
       </c>
-    </row>
-    <row r="66" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC65">
+        <f t="shared" si="4"/>
+        <v>1.795428488821418E-2</v>
+      </c>
+      <c r="AD65">
+        <f t="shared" si="5"/>
+        <v>1.5081021551808382E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>296</v>
       </c>
@@ -7035,8 +7606,16 @@
         <f t="shared" si="3"/>
         <v>2.0410885006989385E-2</v>
       </c>
-    </row>
-    <row r="67" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC66">
+        <f t="shared" si="4"/>
+        <v>1.7600222318099878E-2</v>
+      </c>
+      <c r="AD66">
+        <f t="shared" si="5"/>
+        <v>1.4789559629210367E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>300</v>
       </c>
@@ -7119,8 +7698,16 @@
         <f t="shared" si="3"/>
         <v>2.0208743926043816E-2</v>
       </c>
-    </row>
-    <row r="68" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC67">
+        <f t="shared" si="4"/>
+        <v>1.9823720491662328E-2</v>
+      </c>
+      <c r="AD67">
+        <f t="shared" si="5"/>
+        <v>1.9438697057280834E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>303</v>
       </c>
@@ -7172,11 +7759,11 @@
         <v>322035</v>
       </c>
       <c r="S68">
-        <f t="shared" ref="S68:S72" si="4">_xlfn.T.INV.2T(Q68,R68)</f>
+        <f t="shared" ref="S68:S72" si="6">_xlfn.T.INV.2T(Q68,R68)</f>
         <v>5.5415731179516623</v>
       </c>
       <c r="T68">
-        <f t="shared" ref="T68:T72" si="5">ABS(S68)</f>
+        <f t="shared" ref="T68:T72" si="7">ABS(S68)</f>
         <v>5.5415731179516623</v>
       </c>
       <c r="U68" t="str">
@@ -7184,7 +7771,7 @@
         <v>0.040</v>
       </c>
       <c r="V68">
-        <f t="shared" ref="V68:V72" si="6">U68/T68</f>
+        <f t="shared" ref="V68:V72" si="8">U68/T68</f>
         <v>7.21816696245005E-3</v>
       </c>
       <c r="Y68">
@@ -7200,11 +7787,19 @@
         <v>0.13976194237515863</v>
       </c>
       <c r="AB68">
-        <f t="shared" ref="AB68:AB72" si="7">(Y68-Z68)/1.96</f>
+        <f t="shared" ref="AB68:AB72" si="9">(Y68-Z68)/1.96</f>
         <v>4.0036538490558826E-2</v>
       </c>
-    </row>
-    <row r="69" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC68">
+        <f t="shared" ref="AC68:AC72" si="10">(AA68-Z68)/2/1.96</f>
+        <v>4.0807308595070944E-2</v>
+      </c>
+      <c r="AD68">
+        <f t="shared" ref="AD68:AD72" si="11">(AA68-Y68)/1.96</f>
+        <v>4.1578078699583063E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>308</v>
       </c>
@@ -7256,11 +7851,11 @@
         <v>322035</v>
       </c>
       <c r="S69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>5.5196170398503144</v>
       </c>
       <c r="T69">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5.5196170398503144</v>
       </c>
       <c r="U69" t="str">
@@ -7268,7 +7863,7 @@
         <v>0.019</v>
       </c>
       <c r="V69">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>3.4422677991651496E-3</v>
       </c>
       <c r="Y69">
@@ -7284,11 +7879,19 @@
         <v>5.8268908123975824E-2</v>
       </c>
       <c r="AB69">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2.0410885006989385E-2</v>
       </c>
-    </row>
-    <row r="70" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC69">
+        <f t="shared" si="10"/>
+        <v>2.0018269245279413E-2</v>
+      </c>
+      <c r="AD69">
+        <f t="shared" si="11"/>
+        <v>1.9625653483569438E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>312</v>
       </c>
@@ -7340,11 +7943,11 @@
         <v>322035</v>
       </c>
       <c r="S70">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>5.49545425854319</v>
       </c>
       <c r="T70">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5.49545425854319</v>
       </c>
       <c r="U70" t="str">
@@ -7352,7 +7955,7 @@
         <v>0.022</v>
       </c>
       <c r="V70">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>4.0033087284456915E-3</v>
       </c>
       <c r="Y70">
@@ -7368,11 +7971,19 @@
         <v>3.9220713153281329E-2</v>
       </c>
       <c r="AB70">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2.1042325782678128E-2</v>
       </c>
-    </row>
-    <row r="71" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC70">
+        <f t="shared" si="10"/>
+        <v>2.3090308046130589E-2</v>
+      </c>
+      <c r="AD70">
+        <f t="shared" si="11"/>
+        <v>2.5138290309583051E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>316</v>
       </c>
@@ -7424,11 +8035,11 @@
         <v>322035</v>
       </c>
       <c r="S71">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>5.4823612021473993</v>
       </c>
       <c r="T71">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5.4823612021473993</v>
       </c>
       <c r="U71" t="str">
@@ -7436,7 +8047,7 @@
         <v>0.017</v>
       </c>
       <c r="V71">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>3.1008536966410077E-3</v>
       </c>
       <c r="Y71">
@@ -7452,11 +8063,19 @@
         <v>3.9220713153281329E-2</v>
       </c>
       <c r="AB71">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2.0827548224619984E-2</v>
       </c>
-    </row>
-    <row r="72" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC71">
+        <f t="shared" si="10"/>
+        <v>2.0419058079983801E-2</v>
+      </c>
+      <c r="AD71">
+        <f t="shared" si="11"/>
+        <v>2.0010567935347619E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>319</v>
       </c>
@@ -7508,11 +8127,11 @@
         <v>322035</v>
       </c>
       <c r="S72">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>5.4550317441294514</v>
       </c>
       <c r="T72">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5.4550317441294514</v>
       </c>
       <c r="U72" t="str">
@@ -7520,7 +8139,7 @@
         <v>0.019</v>
       </c>
       <c r="V72">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>3.4830228110857933E-3</v>
       </c>
       <c r="Y72">
@@ -7536,8 +8155,16 @@
         <v>3.9220713153281329E-2</v>
       </c>
       <c r="AB72">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2.0827548224619984E-2</v>
+      </c>
+      <c r="AC72">
+        <f t="shared" si="10"/>
+        <v>2.0419058079983801E-2</v>
+      </c>
+      <c r="AD72">
+        <f t="shared" si="11"/>
+        <v>2.0010567935347619E-2</v>
       </c>
     </row>
   </sheetData>
@@ -7550,12 +8177,2501 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE890338-A9EB-449D-8D4F-895A2109274B}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K71"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G71"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>337</v>
+      </c>
+      <c r="B1" t="s">
+        <v>338</v>
+      </c>
+      <c r="C1" t="s">
+        <v>339</v>
+      </c>
+      <c r="D1" t="s">
+        <v>340</v>
+      </c>
+      <c r="E1" t="s">
+        <v>341</v>
+      </c>
+      <c r="F1" t="s">
+        <v>342</v>
+      </c>
+      <c r="G1" t="s">
+        <v>343</v>
+      </c>
+      <c r="H1" t="s">
+        <v>344</v>
+      </c>
+      <c r="I1" t="s">
+        <v>345</v>
+      </c>
+      <c r="J1" t="s">
+        <v>346</v>
+      </c>
+      <c r="K1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>348</v>
+      </c>
+      <c r="B2" t="s">
+        <v>349</v>
+      </c>
+      <c r="C2" t="s">
+        <v>350</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>351</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" t="s">
+        <v>352</v>
+      </c>
+      <c r="H2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2">
+        <v>1.7106513699587575E-3</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>1.7775489958670895E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>348</v>
+      </c>
+      <c r="B3" t="s">
+        <v>349</v>
+      </c>
+      <c r="C3" t="s">
+        <v>350</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>351</v>
+      </c>
+      <c r="F3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" t="s">
+        <v>352</v>
+      </c>
+      <c r="H3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I3">
+        <v>3.649024665057384E-3</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>2.0419058079983801E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>348</v>
+      </c>
+      <c r="B4" t="s">
+        <v>349</v>
+      </c>
+      <c r="C4" t="s">
+        <v>350</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>351</v>
+      </c>
+      <c r="F4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" t="s">
+        <v>352</v>
+      </c>
+      <c r="H4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I4">
+        <v>4.0064745893953089E-3</v>
+      </c>
+      <c r="J4">
+        <v>4.8790164169432049E-2</v>
+      </c>
+      <c r="K4">
+        <v>2.1775471671213478E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>348</v>
+      </c>
+      <c r="B5" t="s">
+        <v>349</v>
+      </c>
+      <c r="C5" t="s">
+        <v>350</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>351</v>
+      </c>
+      <c r="F5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" t="s">
+        <v>352</v>
+      </c>
+      <c r="H5" t="s">
+        <v>51</v>
+      </c>
+      <c r="I5">
+        <v>3.0940714867255959E-3</v>
+      </c>
+      <c r="J5">
+        <v>1.980262729617973E-2</v>
+      </c>
+      <c r="K5">
+        <v>1.5010331638503445E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>348</v>
+      </c>
+      <c r="B6" t="s">
+        <v>349</v>
+      </c>
+      <c r="C6" t="s">
+        <v>350</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>351</v>
+      </c>
+      <c r="F6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G6" t="s">
+        <v>352</v>
+      </c>
+      <c r="H6" t="s">
+        <v>58</v>
+      </c>
+      <c r="I6">
+        <v>3.8703756544317736E-3</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>2.286024456369572E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>348</v>
+      </c>
+      <c r="B7" t="s">
+        <v>349</v>
+      </c>
+      <c r="C7" t="s">
+        <v>350</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" t="s">
+        <v>351</v>
+      </c>
+      <c r="F7" t="s">
+        <v>62</v>
+      </c>
+      <c r="G7" t="s">
+        <v>352</v>
+      </c>
+      <c r="H7" t="s">
+        <v>65</v>
+      </c>
+      <c r="I7">
+        <v>4.017638968914862E-3</v>
+      </c>
+      <c r="J7">
+        <v>3.9220713153281329E-2</v>
+      </c>
+      <c r="K7">
+        <v>2.219677984429333E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>348</v>
+      </c>
+      <c r="B8" t="s">
+        <v>349</v>
+      </c>
+      <c r="C8" t="s">
+        <v>350</v>
+      </c>
+      <c r="D8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" t="s">
+        <v>351</v>
+      </c>
+      <c r="F8" t="s">
+        <v>69</v>
+      </c>
+      <c r="G8" t="s">
+        <v>352</v>
+      </c>
+      <c r="H8" t="s">
+        <v>72</v>
+      </c>
+      <c r="I8">
+        <v>3.7386530646937952E-3</v>
+      </c>
+      <c r="J8">
+        <v>2.9558802241544429E-2</v>
+      </c>
+      <c r="K8">
+        <v>2.219677984429333E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>348</v>
+      </c>
+      <c r="B9" t="s">
+        <v>349</v>
+      </c>
+      <c r="C9" t="s">
+        <v>350</v>
+      </c>
+      <c r="D9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" t="s">
+        <v>351</v>
+      </c>
+      <c r="F9" t="s">
+        <v>74</v>
+      </c>
+      <c r="G9" t="s">
+        <v>352</v>
+      </c>
+      <c r="H9" t="s">
+        <v>77</v>
+      </c>
+      <c r="I9">
+        <v>3.1102284521522887E-3</v>
+      </c>
+      <c r="J9">
+        <v>-1.0050335853501451E-2</v>
+      </c>
+      <c r="K9">
+        <v>1.795428488821418E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>348</v>
+      </c>
+      <c r="B10" t="s">
+        <v>349</v>
+      </c>
+      <c r="C10" t="s">
+        <v>350</v>
+      </c>
+      <c r="D10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" t="s">
+        <v>351</v>
+      </c>
+      <c r="F10" t="s">
+        <v>81</v>
+      </c>
+      <c r="G10" t="s">
+        <v>352</v>
+      </c>
+      <c r="H10" t="s">
+        <v>84</v>
+      </c>
+      <c r="I10">
+        <v>3.1802854664185814E-3</v>
+      </c>
+      <c r="J10">
+        <v>1.980262729617973E-2</v>
+      </c>
+      <c r="K10">
+        <v>2.0018269245279413E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>348</v>
+      </c>
+      <c r="B11" t="s">
+        <v>349</v>
+      </c>
+      <c r="C11" t="s">
+        <v>350</v>
+      </c>
+      <c r="D11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" t="s">
+        <v>351</v>
+      </c>
+      <c r="F11" t="s">
+        <v>88</v>
+      </c>
+      <c r="G11" t="s">
+        <v>352</v>
+      </c>
+      <c r="H11" t="s">
+        <v>91</v>
+      </c>
+      <c r="I11">
+        <v>3.0830327170072495E-3</v>
+      </c>
+      <c r="J11">
+        <v>5.8268908123975824E-2</v>
+      </c>
+      <c r="K11">
+        <v>1.6932415547161402E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>348</v>
+      </c>
+      <c r="B12" t="s">
+        <v>349</v>
+      </c>
+      <c r="C12" t="s">
+        <v>350</v>
+      </c>
+      <c r="D12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" t="s">
+        <v>351</v>
+      </c>
+      <c r="F12" t="s">
+        <v>95</v>
+      </c>
+      <c r="G12" t="s">
+        <v>352</v>
+      </c>
+      <c r="H12" t="s">
+        <v>91</v>
+      </c>
+      <c r="I12">
+        <v>3.1217885107430307E-3</v>
+      </c>
+      <c r="J12">
+        <v>9.950330853168092E-3</v>
+      </c>
+      <c r="K12">
+        <v>1.7775489958670895E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>348</v>
+      </c>
+      <c r="B13" t="s">
+        <v>349</v>
+      </c>
+      <c r="C13" t="s">
+        <v>350</v>
+      </c>
+      <c r="D13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" t="s">
+        <v>351</v>
+      </c>
+      <c r="F13" t="s">
+        <v>99</v>
+      </c>
+      <c r="G13" t="s">
+        <v>352</v>
+      </c>
+      <c r="H13" t="s">
+        <v>65</v>
+      </c>
+      <c r="I13">
+        <v>4.6164610650375592E-3</v>
+      </c>
+      <c r="J13">
+        <v>1.980262729617973E-2</v>
+      </c>
+      <c r="K13">
+        <v>2.7403124648172694E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>348</v>
+      </c>
+      <c r="B14" t="s">
+        <v>349</v>
+      </c>
+      <c r="C14" t="s">
+        <v>350</v>
+      </c>
+      <c r="D14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" t="s">
+        <v>351</v>
+      </c>
+      <c r="F14" t="s">
+        <v>103</v>
+      </c>
+      <c r="G14" t="s">
+        <v>352</v>
+      </c>
+      <c r="H14" t="s">
+        <v>51</v>
+      </c>
+      <c r="I14">
+        <v>4.5505201226154141E-3</v>
+      </c>
+      <c r="J14">
+        <v>5.8268908123975824E-2</v>
+      </c>
+      <c r="K14">
+        <v>2.8910378904847774E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>348</v>
+      </c>
+      <c r="B15" t="s">
+        <v>349</v>
+      </c>
+      <c r="C15" t="s">
+        <v>350</v>
+      </c>
+      <c r="D15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" t="s">
+        <v>351</v>
+      </c>
+      <c r="F15" t="s">
+        <v>108</v>
+      </c>
+      <c r="G15" t="s">
+        <v>352</v>
+      </c>
+      <c r="H15" t="s">
+        <v>111</v>
+      </c>
+      <c r="I15">
+        <v>4.1554174164966174E-3</v>
+      </c>
+      <c r="J15">
+        <v>4.8790164169432049E-2</v>
+      </c>
+      <c r="K15">
+        <v>2.1984106183941941E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>348</v>
+      </c>
+      <c r="B16" t="s">
+        <v>349</v>
+      </c>
+      <c r="C16" t="s">
+        <v>350</v>
+      </c>
+      <c r="D16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" t="s">
+        <v>351</v>
+      </c>
+      <c r="F16" t="s">
+        <v>113</v>
+      </c>
+      <c r="G16" t="s">
+        <v>352</v>
+      </c>
+      <c r="H16" t="s">
+        <v>91</v>
+      </c>
+      <c r="I16">
+        <v>3.6469588572924081E-3</v>
+      </c>
+      <c r="J16">
+        <v>-1.0050335853501451E-2</v>
+      </c>
+      <c r="K16">
+        <v>2.0625534854360972E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>348</v>
+      </c>
+      <c r="B17" t="s">
+        <v>349</v>
+      </c>
+      <c r="C17" t="s">
+        <v>350</v>
+      </c>
+      <c r="D17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" t="s">
+        <v>351</v>
+      </c>
+      <c r="F17" t="s">
+        <v>120</v>
+      </c>
+      <c r="G17" t="s">
+        <v>352</v>
+      </c>
+      <c r="H17" t="s">
+        <v>122</v>
+      </c>
+      <c r="I17">
+        <v>3.1016834013285568E-3</v>
+      </c>
+      <c r="J17">
+        <v>-3.0459207484708574E-2</v>
+      </c>
+      <c r="K17">
+        <v>1.832289147225909E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>348</v>
+      </c>
+      <c r="B18" t="s">
+        <v>349</v>
+      </c>
+      <c r="C18" t="s">
+        <v>350</v>
+      </c>
+      <c r="D18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" t="s">
+        <v>351</v>
+      </c>
+      <c r="F18" t="s">
+        <v>126</v>
+      </c>
+      <c r="G18" t="s">
+        <v>352</v>
+      </c>
+      <c r="H18" t="s">
+        <v>122</v>
+      </c>
+      <c r="I18">
+        <v>3.1093712759504904E-3</v>
+      </c>
+      <c r="J18">
+        <v>1.980262729617973E-2</v>
+      </c>
+      <c r="K18">
+        <v>1.7600222318099878E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>348</v>
+      </c>
+      <c r="B19" t="s">
+        <v>349</v>
+      </c>
+      <c r="C19" t="s">
+        <v>350</v>
+      </c>
+      <c r="D19" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" t="s">
+        <v>351</v>
+      </c>
+      <c r="F19" t="s">
+        <v>130</v>
+      </c>
+      <c r="G19" t="s">
+        <v>352</v>
+      </c>
+      <c r="H19" t="s">
+        <v>133</v>
+      </c>
+      <c r="I19">
+        <v>3.0459209921138621E-3</v>
+      </c>
+      <c r="J19">
+        <v>-1.0050335853501451E-2</v>
+      </c>
+      <c r="K19">
+        <v>1.795428488821418E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>348</v>
+      </c>
+      <c r="B20" t="s">
+        <v>349</v>
+      </c>
+      <c r="C20" t="s">
+        <v>350</v>
+      </c>
+      <c r="D20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" t="s">
+        <v>351</v>
+      </c>
+      <c r="F20" t="s">
+        <v>136</v>
+      </c>
+      <c r="G20" t="s">
+        <v>352</v>
+      </c>
+      <c r="H20" t="s">
+        <v>139</v>
+      </c>
+      <c r="I20">
+        <v>3.5748833303499571E-3</v>
+      </c>
+      <c r="J20">
+        <v>-3.0459207484708574E-2</v>
+      </c>
+      <c r="K20">
+        <v>1.832289147225909E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>348</v>
+      </c>
+      <c r="B21" t="s">
+        <v>349</v>
+      </c>
+      <c r="C21" t="s">
+        <v>350</v>
+      </c>
+      <c r="D21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" t="s">
+        <v>351</v>
+      </c>
+      <c r="F21" t="s">
+        <v>141</v>
+      </c>
+      <c r="G21" t="s">
+        <v>352</v>
+      </c>
+      <c r="H21" t="s">
+        <v>133</v>
+      </c>
+      <c r="I21">
+        <v>3.1102577503204702E-3</v>
+      </c>
+      <c r="J21">
+        <v>1.980262729617973E-2</v>
+      </c>
+      <c r="K21">
+        <v>1.7428378565682977E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>348</v>
+      </c>
+      <c r="B22" t="s">
+        <v>349</v>
+      </c>
+      <c r="C22" t="s">
+        <v>350</v>
+      </c>
+      <c r="D22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" t="s">
+        <v>351</v>
+      </c>
+      <c r="F22" t="s">
+        <v>144</v>
+      </c>
+      <c r="G22" t="s">
+        <v>352</v>
+      </c>
+      <c r="H22" t="s">
+        <v>147</v>
+      </c>
+      <c r="I22">
+        <v>3.9103977687082164E-3</v>
+      </c>
+      <c r="J22">
+        <v>-1.0050335853501451E-2</v>
+      </c>
+      <c r="K22">
+        <v>2.3090308046130589E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>348</v>
+      </c>
+      <c r="B23" t="s">
+        <v>349</v>
+      </c>
+      <c r="C23" t="s">
+        <v>350</v>
+      </c>
+      <c r="D23" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" t="s">
+        <v>351</v>
+      </c>
+      <c r="F23" t="s">
+        <v>149</v>
+      </c>
+      <c r="G23" t="s">
+        <v>352</v>
+      </c>
+      <c r="H23" t="s">
+        <v>152</v>
+      </c>
+      <c r="I23">
+        <v>3.3351457186432043E-3</v>
+      </c>
+      <c r="J23">
+        <v>9.950330853168092E-3</v>
+      </c>
+      <c r="K23">
+        <v>2.021667644238281E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>348</v>
+      </c>
+      <c r="B24" t="s">
+        <v>349</v>
+      </c>
+      <c r="C24" t="s">
+        <v>350</v>
+      </c>
+      <c r="D24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" t="s">
+        <v>351</v>
+      </c>
+      <c r="F24" t="s">
+        <v>154</v>
+      </c>
+      <c r="G24" t="s">
+        <v>352</v>
+      </c>
+      <c r="H24" t="s">
+        <v>77</v>
+      </c>
+      <c r="I24">
+        <v>4.6363533717789568E-3</v>
+      </c>
+      <c r="J24">
+        <v>9.950330853168092E-3</v>
+      </c>
+      <c r="K24">
+        <v>2.5278291490875252E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>348</v>
+      </c>
+      <c r="B25" t="s">
+        <v>349</v>
+      </c>
+      <c r="C25" t="s">
+        <v>350</v>
+      </c>
+      <c r="D25" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" t="s">
+        <v>351</v>
+      </c>
+      <c r="F25" t="s">
+        <v>157</v>
+      </c>
+      <c r="G25" t="s">
+        <v>352</v>
+      </c>
+      <c r="H25" t="s">
+        <v>160</v>
+      </c>
+      <c r="I25">
+        <v>3.1009539353891694E-3</v>
+      </c>
+      <c r="J25">
+        <v>-1.0050335853501451E-2</v>
+      </c>
+      <c r="K25">
+        <v>2.0625534854360972E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>348</v>
+      </c>
+      <c r="B26" t="s">
+        <v>349</v>
+      </c>
+      <c r="C26" t="s">
+        <v>350</v>
+      </c>
+      <c r="D26" t="s">
+        <v>3</v>
+      </c>
+      <c r="E26" t="s">
+        <v>351</v>
+      </c>
+      <c r="F26" t="s">
+        <v>163</v>
+      </c>
+      <c r="G26" t="s">
+        <v>352</v>
+      </c>
+      <c r="H26" t="s">
+        <v>160</v>
+      </c>
+      <c r="I26">
+        <v>3.1303571212109218E-3</v>
+      </c>
+      <c r="J26">
+        <v>9.950330853168092E-3</v>
+      </c>
+      <c r="K26">
+        <v>2.021667644238281E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>348</v>
+      </c>
+      <c r="B27" t="s">
+        <v>349</v>
+      </c>
+      <c r="C27" t="s">
+        <v>350</v>
+      </c>
+      <c r="D27" t="s">
+        <v>3</v>
+      </c>
+      <c r="E27" t="s">
+        <v>351</v>
+      </c>
+      <c r="F27" t="s">
+        <v>166</v>
+      </c>
+      <c r="G27" t="s">
+        <v>352</v>
+      </c>
+      <c r="H27" t="s">
+        <v>169</v>
+      </c>
+      <c r="I27">
+        <v>3.3858286475286349E-3</v>
+      </c>
+      <c r="J27">
+        <v>-2.0202707317519466E-2</v>
+      </c>
+      <c r="K27">
+        <v>1.8136714715237322E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>348</v>
+      </c>
+      <c r="B28" t="s">
+        <v>349</v>
+      </c>
+      <c r="C28" t="s">
+        <v>350</v>
+      </c>
+      <c r="D28" t="s">
+        <v>3</v>
+      </c>
+      <c r="E28" t="s">
+        <v>351</v>
+      </c>
+      <c r="F28" t="s">
+        <v>171</v>
+      </c>
+      <c r="G28" t="s">
+        <v>352</v>
+      </c>
+      <c r="H28" t="s">
+        <v>169</v>
+      </c>
+      <c r="I28">
+        <v>3.3858286475286349E-3</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <v>1.795428488821418E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>348</v>
+      </c>
+      <c r="B29" t="s">
+        <v>349</v>
+      </c>
+      <c r="C29" t="s">
+        <v>350</v>
+      </c>
+      <c r="D29" t="s">
+        <v>3</v>
+      </c>
+      <c r="E29" t="s">
+        <v>351</v>
+      </c>
+      <c r="F29" t="s">
+        <v>176</v>
+      </c>
+      <c r="G29" t="s">
+        <v>352</v>
+      </c>
+      <c r="H29" t="s">
+        <v>160</v>
+      </c>
+      <c r="I29">
+        <v>3.2840062847118239E-3</v>
+      </c>
+      <c r="J29">
+        <v>-1.0050335853501451E-2</v>
+      </c>
+      <c r="K29">
+        <v>2.0625534854360972E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>348</v>
+      </c>
+      <c r="B30" t="s">
+        <v>349</v>
+      </c>
+      <c r="C30" t="s">
+        <v>350</v>
+      </c>
+      <c r="D30" t="s">
+        <v>3</v>
+      </c>
+      <c r="E30" t="s">
+        <v>351</v>
+      </c>
+      <c r="F30" t="s">
+        <v>180</v>
+      </c>
+      <c r="G30" t="s">
+        <v>352</v>
+      </c>
+      <c r="H30" t="s">
+        <v>169</v>
+      </c>
+      <c r="I30">
+        <v>3.4401141223554918E-3</v>
+      </c>
+      <c r="J30">
+        <v>2.9558802241544429E-2</v>
+      </c>
+      <c r="K30">
+        <v>1.9823720491662328E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>348</v>
+      </c>
+      <c r="B31" t="s">
+        <v>349</v>
+      </c>
+      <c r="C31" t="s">
+        <v>350</v>
+      </c>
+      <c r="D31" t="s">
+        <v>3</v>
+      </c>
+      <c r="E31" t="s">
+        <v>351</v>
+      </c>
+      <c r="F31" t="s">
+        <v>185</v>
+      </c>
+      <c r="G31" t="s">
+        <v>352</v>
+      </c>
+      <c r="H31" t="s">
+        <v>188</v>
+      </c>
+      <c r="I31">
+        <v>3.1570426012529937E-3</v>
+      </c>
+      <c r="J31">
+        <v>-1.0050335853501451E-2</v>
+      </c>
+      <c r="K31">
+        <v>2.0625534854360972E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>348</v>
+      </c>
+      <c r="B32" t="s">
+        <v>349</v>
+      </c>
+      <c r="C32" t="s">
+        <v>350</v>
+      </c>
+      <c r="D32" t="s">
+        <v>3</v>
+      </c>
+      <c r="E32" t="s">
+        <v>351</v>
+      </c>
+      <c r="F32" t="s">
+        <v>190</v>
+      </c>
+      <c r="G32" t="s">
+        <v>352</v>
+      </c>
+      <c r="H32" t="s">
+        <v>152</v>
+      </c>
+      <c r="I32">
+        <v>3.8188506389133458E-3</v>
+      </c>
+      <c r="J32">
+        <v>9.950330853168092E-3</v>
+      </c>
+      <c r="K32">
+        <v>2.2634723369562348E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>348</v>
+      </c>
+      <c r="B33" t="s">
+        <v>349</v>
+      </c>
+      <c r="C33" t="s">
+        <v>350</v>
+      </c>
+      <c r="D33" t="s">
+        <v>3</v>
+      </c>
+      <c r="E33" t="s">
+        <v>351</v>
+      </c>
+      <c r="F33" t="s">
+        <v>193</v>
+      </c>
+      <c r="G33" t="s">
+        <v>352</v>
+      </c>
+      <c r="H33" t="s">
+        <v>188</v>
+      </c>
+      <c r="I33">
+        <v>3.2611000381207386E-3</v>
+      </c>
+      <c r="J33">
+        <v>9.950330853168092E-3</v>
+      </c>
+      <c r="K33">
+        <v>1.7775489958670895E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>348</v>
+      </c>
+      <c r="B34" t="s">
+        <v>349</v>
+      </c>
+      <c r="C34" t="s">
+        <v>350</v>
+      </c>
+      <c r="D34" t="s">
+        <v>3</v>
+      </c>
+      <c r="E34" t="s">
+        <v>351</v>
+      </c>
+      <c r="F34" t="s">
+        <v>196</v>
+      </c>
+      <c r="G34" t="s">
+        <v>352</v>
+      </c>
+      <c r="H34" t="s">
+        <v>160</v>
+      </c>
+      <c r="I34">
+        <v>3.4163905161264875E-3</v>
+      </c>
+      <c r="J34">
+        <v>1.980262729617973E-2</v>
+      </c>
+      <c r="K34">
+        <v>2.2413611171258761E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>348</v>
+      </c>
+      <c r="B35" t="s">
+        <v>349</v>
+      </c>
+      <c r="C35" t="s">
+        <v>350</v>
+      </c>
+      <c r="D35" t="s">
+        <v>3</v>
+      </c>
+      <c r="E35" t="s">
+        <v>351</v>
+      </c>
+      <c r="F35" t="s">
+        <v>199</v>
+      </c>
+      <c r="G35" t="s">
+        <v>352</v>
+      </c>
+      <c r="H35" t="s">
+        <v>201</v>
+      </c>
+      <c r="I35">
+        <v>3.1270864211269097E-3</v>
+      </c>
+      <c r="J35">
+        <v>-2.0202707317519466E-2</v>
+      </c>
+      <c r="K35">
+        <v>2.0836232401598792E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>348</v>
+      </c>
+      <c r="B36" t="s">
+        <v>349</v>
+      </c>
+      <c r="C36" t="s">
+        <v>350</v>
+      </c>
+      <c r="D36" t="s">
+        <v>3</v>
+      </c>
+      <c r="E36" t="s">
+        <v>351</v>
+      </c>
+      <c r="F36" t="s">
+        <v>203</v>
+      </c>
+      <c r="G36" t="s">
+        <v>352</v>
+      </c>
+      <c r="H36" t="s">
+        <v>160</v>
+      </c>
+      <c r="I36">
+        <v>3.4495150546990511E-3</v>
+      </c>
+      <c r="J36">
+        <v>9.950330853168092E-3</v>
+      </c>
+      <c r="K36">
+        <v>2.021667644238281E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>348</v>
+      </c>
+      <c r="B37" t="s">
+        <v>349</v>
+      </c>
+      <c r="C37" t="s">
+        <v>350</v>
+      </c>
+      <c r="D37" t="s">
+        <v>3</v>
+      </c>
+      <c r="E37" t="s">
+        <v>351</v>
+      </c>
+      <c r="F37" t="s">
+        <v>207</v>
+      </c>
+      <c r="G37" t="s">
+        <v>352</v>
+      </c>
+      <c r="H37" t="s">
+        <v>201</v>
+      </c>
+      <c r="I37">
+        <v>3.1359227769991375E-3</v>
+      </c>
+      <c r="J37">
+        <v>2.9558802241544429E-2</v>
+      </c>
+      <c r="K37">
+        <v>1.9823720491662328E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>348</v>
+      </c>
+      <c r="B38" t="s">
+        <v>349</v>
+      </c>
+      <c r="C38" t="s">
+        <v>350</v>
+      </c>
+      <c r="D38" t="s">
+        <v>3</v>
+      </c>
+      <c r="E38" t="s">
+        <v>351</v>
+      </c>
+      <c r="F38" t="s">
+        <v>211</v>
+      </c>
+      <c r="G38" t="s">
+        <v>352</v>
+      </c>
+      <c r="H38" t="s">
+        <v>188</v>
+      </c>
+      <c r="I38">
+        <v>3.2970040060210383E-3</v>
+      </c>
+      <c r="J38">
+        <v>9.950330853168092E-3</v>
+      </c>
+      <c r="K38">
+        <v>1.7600222318099878E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>348</v>
+      </c>
+      <c r="B39" t="s">
+        <v>349</v>
+      </c>
+      <c r="C39" t="s">
+        <v>350</v>
+      </c>
+      <c r="D39" t="s">
+        <v>3</v>
+      </c>
+      <c r="E39" t="s">
+        <v>351</v>
+      </c>
+      <c r="F39" t="s">
+        <v>215</v>
+      </c>
+      <c r="G39" t="s">
+        <v>352</v>
+      </c>
+      <c r="H39" t="s">
+        <v>147</v>
+      </c>
+      <c r="I39">
+        <v>4.731827345175914E-3</v>
+      </c>
+      <c r="J39">
+        <v>9.950330853168092E-3</v>
+      </c>
+      <c r="K39">
+        <v>2.2634723369562348E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>348</v>
+      </c>
+      <c r="B40" t="s">
+        <v>349</v>
+      </c>
+      <c r="C40" t="s">
+        <v>350</v>
+      </c>
+      <c r="D40" t="s">
+        <v>3</v>
+      </c>
+      <c r="E40" t="s">
+        <v>351</v>
+      </c>
+      <c r="F40" t="s">
+        <v>218</v>
+      </c>
+      <c r="G40" t="s">
+        <v>352</v>
+      </c>
+      <c r="H40" t="s">
+        <v>58</v>
+      </c>
+      <c r="I40">
+        <v>7.6547101529929129E-3</v>
+      </c>
+      <c r="J40">
+        <v>1.980262729617973E-2</v>
+      </c>
+      <c r="K40">
+        <v>3.5069130262398725E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>348</v>
+      </c>
+      <c r="B41" t="s">
+        <v>349</v>
+      </c>
+      <c r="C41" t="s">
+        <v>350</v>
+      </c>
+      <c r="D41" t="s">
+        <v>3</v>
+      </c>
+      <c r="E41" t="s">
+        <v>351</v>
+      </c>
+      <c r="F41" t="s">
+        <v>222</v>
+      </c>
+      <c r="G41" t="s">
+        <v>352</v>
+      </c>
+      <c r="H41" t="s">
+        <v>201</v>
+      </c>
+      <c r="I41">
+        <v>3.2347153051164972E-3</v>
+      </c>
+      <c r="J41">
+        <v>0</v>
+      </c>
+      <c r="K41">
+        <v>1.7775489958670895E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>348</v>
+      </c>
+      <c r="B42" t="s">
+        <v>349</v>
+      </c>
+      <c r="C42" t="s">
+        <v>350</v>
+      </c>
+      <c r="D42" t="s">
+        <v>3</v>
+      </c>
+      <c r="E42" t="s">
+        <v>351</v>
+      </c>
+      <c r="F42" t="s">
+        <v>226</v>
+      </c>
+      <c r="G42" t="s">
+        <v>352</v>
+      </c>
+      <c r="H42" t="s">
+        <v>169</v>
+      </c>
+      <c r="I42">
+        <v>3.7365871844980301E-3</v>
+      </c>
+      <c r="J42">
+        <v>2.9558802241544429E-2</v>
+      </c>
+      <c r="K42">
+        <v>1.9823720491662328E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>348</v>
+      </c>
+      <c r="B43" t="s">
+        <v>349</v>
+      </c>
+      <c r="C43" t="s">
+        <v>350</v>
+      </c>
+      <c r="D43" t="s">
+        <v>3</v>
+      </c>
+      <c r="E43" t="s">
+        <v>351</v>
+      </c>
+      <c r="F43" t="s">
+        <v>228</v>
+      </c>
+      <c r="G43" t="s">
+        <v>352</v>
+      </c>
+      <c r="H43" t="s">
+        <v>230</v>
+      </c>
+      <c r="I43">
+        <v>3.0908838625917667E-3</v>
+      </c>
+      <c r="J43">
+        <v>1.980262729617973E-2</v>
+      </c>
+      <c r="K43">
+        <v>1.7428378565682977E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>348</v>
+      </c>
+      <c r="B44" t="s">
+        <v>349</v>
+      </c>
+      <c r="C44" t="s">
+        <v>350</v>
+      </c>
+      <c r="D44" t="s">
+        <v>3</v>
+      </c>
+      <c r="E44" t="s">
+        <v>351</v>
+      </c>
+      <c r="F44" t="s">
+        <v>232</v>
+      </c>
+      <c r="G44" t="s">
+        <v>352</v>
+      </c>
+      <c r="H44" t="s">
+        <v>230</v>
+      </c>
+      <c r="I44">
+        <v>3.0928807413129855E-3</v>
+      </c>
+      <c r="J44">
+        <v>1.980262729617973E-2</v>
+      </c>
+      <c r="K44">
+        <v>1.7600222318099878E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>348</v>
+      </c>
+      <c r="B45" t="s">
+        <v>349</v>
+      </c>
+      <c r="C45" t="s">
+        <v>350</v>
+      </c>
+      <c r="D45" t="s">
+        <v>3</v>
+      </c>
+      <c r="E45" t="s">
+        <v>351</v>
+      </c>
+      <c r="F45" t="s">
+        <v>235</v>
+      </c>
+      <c r="G45" t="s">
+        <v>352</v>
+      </c>
+      <c r="H45" t="s">
+        <v>188</v>
+      </c>
+      <c r="I45">
+        <v>3.4610202407590472E-3</v>
+      </c>
+      <c r="J45">
+        <v>1.980262729617973E-2</v>
+      </c>
+      <c r="K45">
+        <v>1.7428378565682977E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>348</v>
+      </c>
+      <c r="B46" t="s">
+        <v>349</v>
+      </c>
+      <c r="C46" t="s">
+        <v>350</v>
+      </c>
+      <c r="D46" t="s">
+        <v>3</v>
+      </c>
+      <c r="E46" t="s">
+        <v>351</v>
+      </c>
+      <c r="F46" t="s">
+        <v>237</v>
+      </c>
+      <c r="G46" t="s">
+        <v>352</v>
+      </c>
+      <c r="H46" t="s">
+        <v>188</v>
+      </c>
+      <c r="I46">
+        <v>3.4963252656081026E-3</v>
+      </c>
+      <c r="J46">
+        <v>9.950330853168092E-3</v>
+      </c>
+      <c r="K46">
+        <v>1.7600222318099878E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>348</v>
+      </c>
+      <c r="B47" t="s">
+        <v>349</v>
+      </c>
+      <c r="C47" t="s">
+        <v>350</v>
+      </c>
+      <c r="D47" t="s">
+        <v>3</v>
+      </c>
+      <c r="E47" t="s">
+        <v>351</v>
+      </c>
+      <c r="F47" t="s">
+        <v>240</v>
+      </c>
+      <c r="G47" t="s">
+        <v>352</v>
+      </c>
+      <c r="H47" t="s">
+        <v>230</v>
+      </c>
+      <c r="I47">
+        <v>3.187050371155891E-3</v>
+      </c>
+      <c r="J47">
+        <v>2.9558802241544429E-2</v>
+      </c>
+      <c r="K47">
+        <v>1.9823720491662328E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>348</v>
+      </c>
+      <c r="B48" t="s">
+        <v>349</v>
+      </c>
+      <c r="C48" t="s">
+        <v>350</v>
+      </c>
+      <c r="D48" t="s">
+        <v>3</v>
+      </c>
+      <c r="E48" t="s">
+        <v>351</v>
+      </c>
+      <c r="F48" t="s">
+        <v>243</v>
+      </c>
+      <c r="G48" t="s">
+        <v>352</v>
+      </c>
+      <c r="H48" t="s">
+        <v>245</v>
+      </c>
+      <c r="I48">
+        <v>3.0193108779371599E-3</v>
+      </c>
+      <c r="J48">
+        <v>9.950330853168092E-3</v>
+      </c>
+      <c r="K48">
+        <v>2.021667644238281E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>348</v>
+      </c>
+      <c r="B49" t="s">
+        <v>349</v>
+      </c>
+      <c r="C49" t="s">
+        <v>350</v>
+      </c>
+      <c r="D49" t="s">
+        <v>3</v>
+      </c>
+      <c r="E49" t="s">
+        <v>351</v>
+      </c>
+      <c r="F49" t="s">
+        <v>246</v>
+      </c>
+      <c r="G49" t="s">
+        <v>352</v>
+      </c>
+      <c r="H49" t="s">
+        <v>245</v>
+      </c>
+      <c r="I49">
+        <v>3.071047346779402E-3</v>
+      </c>
+      <c r="J49">
+        <v>0</v>
+      </c>
+      <c r="K49">
+        <v>2.0419058079983801E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>348</v>
+      </c>
+      <c r="B50" t="s">
+        <v>349</v>
+      </c>
+      <c r="C50" t="s">
+        <v>350</v>
+      </c>
+      <c r="D50" t="s">
+        <v>3</v>
+      </c>
+      <c r="E50" t="s">
+        <v>351</v>
+      </c>
+      <c r="F50" t="s">
+        <v>248</v>
+      </c>
+      <c r="G50" t="s">
+        <v>352</v>
+      </c>
+      <c r="H50" t="s">
+        <v>139</v>
+      </c>
+      <c r="I50">
+        <v>4.8409172195352148E-3</v>
+      </c>
+      <c r="J50">
+        <v>9.950330853168092E-3</v>
+      </c>
+      <c r="K50">
+        <v>3.0344883383001391E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>348</v>
+      </c>
+      <c r="B51" t="s">
+        <v>349</v>
+      </c>
+      <c r="C51" t="s">
+        <v>350</v>
+      </c>
+      <c r="D51" t="s">
+        <v>3</v>
+      </c>
+      <c r="E51" t="s">
+        <v>351</v>
+      </c>
+      <c r="F51" t="s">
+        <v>252</v>
+      </c>
+      <c r="G51" t="s">
+        <v>352</v>
+      </c>
+      <c r="H51" t="s">
+        <v>245</v>
+      </c>
+      <c r="I51">
+        <v>3.1132498103861412E-3</v>
+      </c>
+      <c r="J51">
+        <v>-3.0459207484708574E-2</v>
+      </c>
+      <c r="K51">
+        <v>1.5784541764818246E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>348</v>
+      </c>
+      <c r="B52" t="s">
+        <v>349</v>
+      </c>
+      <c r="C52" t="s">
+        <v>350</v>
+      </c>
+      <c r="D52" t="s">
+        <v>3</v>
+      </c>
+      <c r="E52" t="s">
+        <v>351</v>
+      </c>
+      <c r="F52" t="s">
+        <v>255</v>
+      </c>
+      <c r="G52" t="s">
+        <v>352</v>
+      </c>
+      <c r="H52" t="s">
+        <v>91</v>
+      </c>
+      <c r="I52">
+        <v>5.3679176144036979E-3</v>
+      </c>
+      <c r="J52">
+        <v>3.9220713153281329E-2</v>
+      </c>
+      <c r="K52">
+        <v>2.1984106183941941E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>348</v>
+      </c>
+      <c r="B53" t="s">
+        <v>349</v>
+      </c>
+      <c r="C53" t="s">
+        <v>350</v>
+      </c>
+      <c r="D53" t="s">
+        <v>3</v>
+      </c>
+      <c r="E53" t="s">
+        <v>351</v>
+      </c>
+      <c r="F53" t="s">
+        <v>259</v>
+      </c>
+      <c r="G53" t="s">
+        <v>352</v>
+      </c>
+      <c r="H53" t="s">
+        <v>91</v>
+      </c>
+      <c r="I53">
+        <v>5.3834551170713757E-3</v>
+      </c>
+      <c r="J53">
+        <v>-2.0202707317519466E-2</v>
+      </c>
+      <c r="K53">
+        <v>2.851821581329508E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>348</v>
+      </c>
+      <c r="B54" t="s">
+        <v>349</v>
+      </c>
+      <c r="C54" t="s">
+        <v>350</v>
+      </c>
+      <c r="D54" t="s">
+        <v>3</v>
+      </c>
+      <c r="E54" t="s">
+        <v>351</v>
+      </c>
+      <c r="F54" t="s">
+        <v>262</v>
+      </c>
+      <c r="G54" t="s">
+        <v>352</v>
+      </c>
+      <c r="H54" t="s">
+        <v>245</v>
+      </c>
+      <c r="I54">
+        <v>3.157964334726288E-3</v>
+      </c>
+      <c r="J54">
+        <v>0</v>
+      </c>
+      <c r="K54">
+        <v>1.7775489958670895E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>348</v>
+      </c>
+      <c r="B55" t="s">
+        <v>349</v>
+      </c>
+      <c r="C55" t="s">
+        <v>350</v>
+      </c>
+      <c r="D55" t="s">
+        <v>3</v>
+      </c>
+      <c r="E55" t="s">
+        <v>351</v>
+      </c>
+      <c r="F55" t="s">
+        <v>265</v>
+      </c>
+      <c r="G55" t="s">
+        <v>352</v>
+      </c>
+      <c r="H55" t="s">
+        <v>122</v>
+      </c>
+      <c r="I55">
+        <v>4.5724640231131859E-3</v>
+      </c>
+      <c r="J55">
+        <v>2.9558802241544429E-2</v>
+      </c>
+      <c r="K55">
+        <v>2.4786670523889762E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>348</v>
+      </c>
+      <c r="B56" t="s">
+        <v>349</v>
+      </c>
+      <c r="C56" t="s">
+        <v>350</v>
+      </c>
+      <c r="D56" t="s">
+        <v>3</v>
+      </c>
+      <c r="E56" t="s">
+        <v>351</v>
+      </c>
+      <c r="F56" t="s">
+        <v>268</v>
+      </c>
+      <c r="G56" t="s">
+        <v>352</v>
+      </c>
+      <c r="H56" t="s">
+        <v>230</v>
+      </c>
+      <c r="I56">
+        <v>3.3414160168904051E-3</v>
+      </c>
+      <c r="J56">
+        <v>9.950330853168092E-3</v>
+      </c>
+      <c r="K56">
+        <v>2.021667644238281E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>348</v>
+      </c>
+      <c r="B57" t="s">
+        <v>349</v>
+      </c>
+      <c r="C57" t="s">
+        <v>350</v>
+      </c>
+      <c r="D57" t="s">
+        <v>3</v>
+      </c>
+      <c r="E57" t="s">
+        <v>351</v>
+      </c>
+      <c r="F57" t="s">
+        <v>270</v>
+      </c>
+      <c r="G57" t="s">
+        <v>352</v>
+      </c>
+      <c r="H57" t="s">
+        <v>245</v>
+      </c>
+      <c r="I57">
+        <v>3.1792521978924546E-3</v>
+      </c>
+      <c r="J57">
+        <v>9.950330853168092E-3</v>
+      </c>
+      <c r="K57">
+        <v>1.7600222318099878E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>348</v>
+      </c>
+      <c r="B58" t="s">
+        <v>349</v>
+      </c>
+      <c r="C58" t="s">
+        <v>350</v>
+      </c>
+      <c r="D58" t="s">
+        <v>3</v>
+      </c>
+      <c r="E58" t="s">
+        <v>351</v>
+      </c>
+      <c r="F58" t="s">
+        <v>273</v>
+      </c>
+      <c r="G58" t="s">
+        <v>352</v>
+      </c>
+      <c r="H58" t="s">
+        <v>230</v>
+      </c>
+      <c r="I58">
+        <v>3.3624599660399333E-3</v>
+      </c>
+      <c r="J58">
+        <v>-3.0459207484708574E-2</v>
+      </c>
+      <c r="K58">
+        <v>2.1051281553062108E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>348</v>
+      </c>
+      <c r="B59" t="s">
+        <v>349</v>
+      </c>
+      <c r="C59" t="s">
+        <v>350</v>
+      </c>
+      <c r="D59" t="s">
+        <v>3</v>
+      </c>
+      <c r="E59" t="s">
+        <v>351</v>
+      </c>
+      <c r="F59" t="s">
+        <v>276</v>
+      </c>
+      <c r="G59" t="s">
+        <v>352</v>
+      </c>
+      <c r="H59" t="s">
+        <v>278</v>
+      </c>
+      <c r="I59">
+        <v>3.0193538814245456E-3</v>
+      </c>
+      <c r="J59">
+        <v>0</v>
+      </c>
+      <c r="K59">
+        <v>1.7775489958670895E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>348</v>
+      </c>
+      <c r="B60" t="s">
+        <v>349</v>
+      </c>
+      <c r="C60" t="s">
+        <v>350</v>
+      </c>
+      <c r="D60" t="s">
+        <v>3</v>
+      </c>
+      <c r="E60" t="s">
+        <v>351</v>
+      </c>
+      <c r="F60" t="s">
+        <v>279</v>
+      </c>
+      <c r="G60" t="s">
+        <v>352</v>
+      </c>
+      <c r="H60" t="s">
+        <v>278</v>
+      </c>
+      <c r="I60">
+        <v>3.0243671843956333E-3</v>
+      </c>
+      <c r="J60">
+        <v>1.980262729617973E-2</v>
+      </c>
+      <c r="K60">
+        <v>1.7428378565682977E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>348</v>
+      </c>
+      <c r="B61" t="s">
+        <v>349</v>
+      </c>
+      <c r="C61" t="s">
+        <v>350</v>
+      </c>
+      <c r="D61" t="s">
+        <v>3</v>
+      </c>
+      <c r="E61" t="s">
+        <v>351</v>
+      </c>
+      <c r="F61" t="s">
+        <v>282</v>
+      </c>
+      <c r="G61" t="s">
+        <v>352</v>
+      </c>
+      <c r="H61" t="s">
+        <v>91</v>
+      </c>
+      <c r="I61">
+        <v>5.5237368363655111E-3</v>
+      </c>
+      <c r="J61">
+        <v>4.8790164169432049E-2</v>
+      </c>
+      <c r="K61">
+        <v>2.9186314075955181E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>348</v>
+      </c>
+      <c r="B62" t="s">
+        <v>349</v>
+      </c>
+      <c r="C62" t="s">
+        <v>350</v>
+      </c>
+      <c r="D62" t="s">
+        <v>3</v>
+      </c>
+      <c r="E62" t="s">
+        <v>351</v>
+      </c>
+      <c r="F62" t="s">
+        <v>287</v>
+      </c>
+      <c r="G62" t="s">
+        <v>352</v>
+      </c>
+      <c r="H62" t="s">
+        <v>152</v>
+      </c>
+      <c r="I62">
+        <v>4.4739424041467394E-3</v>
+      </c>
+      <c r="J62">
+        <v>1.980262729617973E-2</v>
+      </c>
+      <c r="K62">
+        <v>3.0046692769485604E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>348</v>
+      </c>
+      <c r="B63" t="s">
+        <v>349</v>
+      </c>
+      <c r="C63" t="s">
+        <v>350</v>
+      </c>
+      <c r="D63" t="s">
+        <v>3</v>
+      </c>
+      <c r="E63" t="s">
+        <v>351</v>
+      </c>
+      <c r="F63" t="s">
+        <v>291</v>
+      </c>
+      <c r="G63" t="s">
+        <v>352</v>
+      </c>
+      <c r="H63" t="s">
+        <v>245</v>
+      </c>
+      <c r="I63">
+        <v>3.2255089532494787E-3</v>
+      </c>
+      <c r="J63">
+        <v>0</v>
+      </c>
+      <c r="K63">
+        <v>1.7775489958670895E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>348</v>
+      </c>
+      <c r="B64" t="s">
+        <v>349</v>
+      </c>
+      <c r="C64" t="s">
+        <v>350</v>
+      </c>
+      <c r="D64" t="s">
+        <v>3</v>
+      </c>
+      <c r="E64" t="s">
+        <v>351</v>
+      </c>
+      <c r="F64" t="s">
+        <v>293</v>
+      </c>
+      <c r="G64" t="s">
+        <v>352</v>
+      </c>
+      <c r="H64" t="s">
+        <v>230</v>
+      </c>
+      <c r="I64">
+        <v>3.413229426799249E-3</v>
+      </c>
+      <c r="J64">
+        <v>0</v>
+      </c>
+      <c r="K64">
+        <v>1.795428488821418E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>348</v>
+      </c>
+      <c r="B65" t="s">
+        <v>349</v>
+      </c>
+      <c r="C65" t="s">
+        <v>350</v>
+      </c>
+      <c r="D65" t="s">
+        <v>3</v>
+      </c>
+      <c r="E65" t="s">
+        <v>351</v>
+      </c>
+      <c r="F65" t="s">
+        <v>296</v>
+      </c>
+      <c r="G65" t="s">
+        <v>352</v>
+      </c>
+      <c r="H65" t="s">
+        <v>278</v>
+      </c>
+      <c r="I65">
+        <v>3.0575583491919659E-3</v>
+      </c>
+      <c r="J65">
+        <v>1.980262729617973E-2</v>
+      </c>
+      <c r="K65">
+        <v>1.7600222318099878E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>348</v>
+      </c>
+      <c r="B66" t="s">
+        <v>349</v>
+      </c>
+      <c r="C66" t="s">
+        <v>350</v>
+      </c>
+      <c r="D66" t="s">
+        <v>3</v>
+      </c>
+      <c r="E66" t="s">
+        <v>351</v>
+      </c>
+      <c r="F66" t="s">
+        <v>300</v>
+      </c>
+      <c r="G66" t="s">
+        <v>352</v>
+      </c>
+      <c r="H66" t="s">
+        <v>201</v>
+      </c>
+      <c r="I66">
+        <v>3.609083481225025E-3</v>
+      </c>
+      <c r="J66">
+        <v>2.9558802241544429E-2</v>
+      </c>
+      <c r="K66">
+        <v>1.9823720491662328E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>348</v>
+      </c>
+      <c r="B67" t="s">
+        <v>349</v>
+      </c>
+      <c r="C67" t="s">
+        <v>350</v>
+      </c>
+      <c r="D67" t="s">
+        <v>3</v>
+      </c>
+      <c r="E67" t="s">
+        <v>351</v>
+      </c>
+      <c r="F67" t="s">
+        <v>303</v>
+      </c>
+      <c r="G67" t="s">
+        <v>352</v>
+      </c>
+      <c r="H67" t="s">
+        <v>51</v>
+      </c>
+      <c r="I67">
+        <v>7.21816696245005E-3</v>
+      </c>
+      <c r="J67">
+        <v>5.8268908123975824E-2</v>
+      </c>
+      <c r="K67">
+        <v>4.0807308595070944E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>348</v>
+      </c>
+      <c r="B68" t="s">
+        <v>349</v>
+      </c>
+      <c r="C68" t="s">
+        <v>350</v>
+      </c>
+      <c r="D68" t="s">
+        <v>3</v>
+      </c>
+      <c r="E68" t="s">
+        <v>351</v>
+      </c>
+      <c r="F68" t="s">
+        <v>308</v>
+      </c>
+      <c r="G68" t="s">
+        <v>352</v>
+      </c>
+      <c r="H68" t="s">
+        <v>230</v>
+      </c>
+      <c r="I68">
+        <v>3.4422677991651496E-3</v>
+      </c>
+      <c r="J68">
+        <v>1.980262729617973E-2</v>
+      </c>
+      <c r="K68">
+        <v>2.0018269245279413E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>348</v>
+      </c>
+      <c r="B69" t="s">
+        <v>349</v>
+      </c>
+      <c r="C69" t="s">
+        <v>350</v>
+      </c>
+      <c r="D69" t="s">
+        <v>3</v>
+      </c>
+      <c r="E69" t="s">
+        <v>351</v>
+      </c>
+      <c r="F69" t="s">
+        <v>312</v>
+      </c>
+      <c r="G69" t="s">
+        <v>352</v>
+      </c>
+      <c r="H69" t="s">
+        <v>160</v>
+      </c>
+      <c r="I69">
+        <v>4.0033087284456915E-3</v>
+      </c>
+      <c r="J69">
+        <v>-1.0050335853501451E-2</v>
+      </c>
+      <c r="K69">
+        <v>2.3090308046130589E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>348</v>
+      </c>
+      <c r="B70" t="s">
+        <v>349</v>
+      </c>
+      <c r="C70" t="s">
+        <v>350</v>
+      </c>
+      <c r="D70" t="s">
+        <v>3</v>
+      </c>
+      <c r="E70" t="s">
+        <v>351</v>
+      </c>
+      <c r="F70" t="s">
+        <v>316</v>
+      </c>
+      <c r="G70" t="s">
+        <v>352</v>
+      </c>
+      <c r="H70" t="s">
+        <v>278</v>
+      </c>
+      <c r="I70">
+        <v>3.1008536966410077E-3</v>
+      </c>
+      <c r="J70">
+        <v>0</v>
+      </c>
+      <c r="K70">
+        <v>2.0419058079983801E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>348</v>
+      </c>
+      <c r="B71" t="s">
+        <v>349</v>
+      </c>
+      <c r="C71" t="s">
+        <v>350</v>
+      </c>
+      <c r="D71" t="s">
+        <v>3</v>
+      </c>
+      <c r="E71" t="s">
+        <v>351</v>
+      </c>
+      <c r="F71" t="s">
+        <v>319</v>
+      </c>
+      <c r="G71" t="s">
+        <v>352</v>
+      </c>
+      <c r="H71" t="s">
+        <v>230</v>
+      </c>
+      <c r="I71">
+        <v>3.4830228110857933E-3</v>
+      </c>
+      <c r="J71">
+        <v>0</v>
+      </c>
+      <c r="K71">
+        <v>2.0419058079983801E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>